<commit_message>
Creating SQL insertion spreadsheet and adding .mp3 files
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C414C550-643A-4172-B068-A5212BD75639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A26099-AE72-46EC-832C-378AEB25C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -37,12 +37,72 @@
   </si>
   <si>
     <t>Death Note OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Song Name</t>
+  </si>
+  <si>
+    <t>The World</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Anime</t>
+  </si>
+  <si>
+    <t>Death Note OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Angel Beats OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Angel Beats OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Attack On Titan OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Attack On Titan OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Berserk OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Berserk OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Chainsaw Man OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Chainsaw Man OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Code Geass OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Code Geass OP1 - Hard</t>
+  </si>
+  <si>
+    <t>My Soul, Your Beats!</t>
+  </si>
+  <si>
+    <t>Guren no Yumiya</t>
+  </si>
+  <si>
+    <t>Tell Me Why</t>
+  </si>
+  <si>
+    <t>Kick Back</t>
+  </si>
+  <si>
+    <t>COLORS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,8 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,37 +450,264 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E2" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="2" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="103.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D11" si="0">"./"&amp;LOWER(C2)&amp;"/"&amp;A2&amp;".mp3"</f>
+        <v>./anime/Angel Beats OP1 - Easy.mp3</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f t="shared" ref="E2:E11" si="1">"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;");"</f>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Angel Beats OP1 - Easy', 'My Soul, Your Beats!', 'Anime', './anime/Angel Beats OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Angel Beats OP1 - Hard.mp3</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Angel Beats OP1 - Hard', 'My Soul, Your Beats!', 'Anime', './anime/Angel Beats OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Attack On Titan OP1 - Easy.mp3</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Guren no Yumiya', 'Anime', './anime/Attack On Titan OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Attack On Titan OP1 - Hard.mp3</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Guren no Yumiya', 'Anime', './anime/Attack On Titan OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Berserk OP1 - Easy.mp3</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Berserk OP1 - Easy', 'Tell Me Why', 'Anime', './anime/Berserk OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Berserk OP1 - Hard.mp3</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Berserk OP1 - Hard', 'Tell Me Why', 'Anime', './anime/Berserk OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Chainsaw Man OP1 - Easy.mp3</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Kick Back', 'Anime', './anime/Chainsaw Man OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Chainsaw Man OP1 - Hard.mp3</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Kick Back', 'Anime', './anime/Chainsaw Man OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Code Geass OP1 - Easy.mp3</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Code Geass OP1 - Easy', 'COLORS', 'Anime', './anime/Code Geass OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>./anime/Code Geass OP1 - Hard.mp3</v>
+      </c>
+      <c r="E11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Code Geass OP1 - Hard', 'COLORS', 'Anime', './anime/Code Geass OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="str">
-        <f>"./"&amp;A2&amp;".mp3"</f>
-        <v>./Death Note OP1 - Easy.mp3</v>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="str">
+        <f>"./"&amp;LOWER(C12)&amp;"/"&amp;A12&amp;".mp3"</f>
+        <v>./anime/Death Note OP1 - Easy.mp3</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A12&amp;"'"&amp;", "&amp;"'"&amp;B12&amp;"'"&amp;", "&amp;"'"&amp;C12&amp;"'"&amp;", "&amp;"'"&amp;D12&amp;"'"&amp;");"</f>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Note OP1 - Easy', 'The World', 'Anime', './anime/Death Note OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="str">
+        <f>"./"&amp;LOWER(C13)&amp;"/"&amp;A13&amp;".mp3"</f>
+        <v>./anime/Death Note OP1 - Hard.mp3</v>
+      </c>
+      <c r="E13" s="1" t="str">
+        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A13&amp;"'"&amp;", "&amp;"'"&amp;B13&amp;"'"&amp;", "&amp;"'"&amp;C13&amp;"'"&amp;", "&amp;"'"&amp;D13&amp;"'"&amp;");"</f>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Note OP1 - Hard', 'The World', 'Anime', './anime/Death Note OP1 - Hard.mp3');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding song tracks and updating spreadsheet
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A26099-AE72-46EC-832C-378AEB25C53E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B1532E-6DB7-4F2B-B8A6-DCEFD0FA8418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Anime" sheetId="1" r:id="rId1"/>
+    <sheet name="TV" sheetId="2" r:id="rId2"/>
+    <sheet name="Video Games" sheetId="3" r:id="rId3"/>
+    <sheet name="Indie" sheetId="4" r:id="rId4"/>
+    <sheet name="Top40" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -97,6 +109,147 @@
   </si>
   <si>
     <t>COLORS</t>
+  </si>
+  <si>
+    <t>Death Parade OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Death Parade OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Dragon Ball Z OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Dragon Ball Z OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Ergo Proxy OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Ergo Proxy OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Evangelion OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Evangelion OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Fate Stay Night UBW OP2 - Easy</t>
+  </si>
+  <si>
+    <t>Fate Stay Night UBW OP2 - Hard</t>
+  </si>
+  <si>
+    <t>Guilty Crown OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Guilty Crown OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Jojo OP2 - Easy</t>
+  </si>
+  <si>
+    <t>Jojo OP2 - Hard</t>
+  </si>
+  <si>
+    <t>Jujutsu Kaisen OP2 - Easy</t>
+  </si>
+  <si>
+    <t>Jujutsu Kaisen OP2 - Hard</t>
+  </si>
+  <si>
+    <t>One Punch Man OP1 - Easy</t>
+  </si>
+  <si>
+    <t>One Punch Man OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Flyers</t>
+  </si>
+  <si>
+    <t>Cha-La Head-Cha-La</t>
+  </si>
+  <si>
+    <t>Kiri</t>
+  </si>
+  <si>
+    <t>Brave Shine</t>
+  </si>
+  <si>
+    <t>My Dearest</t>
+  </si>
+  <si>
+    <t>Bloody Stream</t>
+  </si>
+  <si>
+    <t>Vivid Vice</t>
+  </si>
+  <si>
+    <t>The Hero!! ~Ikareru Ken ni Honō o Tsukeru~</t>
+  </si>
+  <si>
+    <t>A Cruel Angel''s Thesis</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Angel Beats</t>
+  </si>
+  <si>
+    <t>Chainsaw Man</t>
+  </si>
+  <si>
+    <t>Code Geass</t>
+  </si>
+  <si>
+    <t>Death Note</t>
+  </si>
+  <si>
+    <t>Death Parade</t>
+  </si>
+  <si>
+    <t>Attack on Titan</t>
+  </si>
+  <si>
+    <t>Berserk</t>
+  </si>
+  <si>
+    <t>Dragon Ball Z</t>
+  </si>
+  <si>
+    <t>Ergo Proxy</t>
+  </si>
+  <si>
+    <t>Guilty Crown</t>
+  </si>
+  <si>
+    <t>Jujutsu Kaisen</t>
+  </si>
+  <si>
+    <t>Neon Genesis Evangelion</t>
+  </si>
+  <si>
+    <t>Fate Stay Night - Unlimited Blade Works</t>
+  </si>
+  <si>
+    <t>Jojo's Bizarre Adventure</t>
+  </si>
+  <si>
+    <t>One Punch Man</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Song</t>
   </si>
 </sst>
 </file>
@@ -451,266 +604,853 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="103.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="97.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="str">
-        <f t="shared" ref="D2:D11" si="0">"./"&amp;LOWER(C2)&amp;"/"&amp;A2&amp;".mp3"</f>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F11" si="0">"./"&amp;LOWER(E2)&amp;"/"&amp;A2&amp;".mp3"</f>
         <v>./anime/Angel Beats OP1 - Easy.mp3</v>
       </c>
-      <c r="E2" s="1" t="str">
-        <f t="shared" ref="E2:E11" si="1">"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;");"</f>
+      <c r="G2" s="1" t="str">
+        <f t="shared" ref="G2:G11" si="1">"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;");"</f>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Angel Beats OP1 - Easy', 'My Soul, Your Beats!', 'Anime', './anime/Angel Beats OP1 - Easy.mp3');</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="str">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Angel Beats OP1 - Hard.mp3</v>
       </c>
-      <c r="E3" s="1" t="str">
+      <c r="G3" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Angel Beats OP1 - Hard', 'My Soul, Your Beats!', 'Anime', './anime/Angel Beats OP1 - Hard.mp3');</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="str">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Attack On Titan OP1 - Easy.mp3</v>
       </c>
-      <c r="E4" s="1" t="str">
+      <c r="G4" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Guren no Yumiya', 'Anime', './anime/Attack On Titan OP1 - Easy.mp3');</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="str">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Attack On Titan OP1 - Hard.mp3</v>
       </c>
-      <c r="E5" s="1" t="str">
+      <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Guren no Yumiya', 'Anime', './anime/Attack On Titan OP1 - Hard.mp3');</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="str">
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Berserk OP1 - Easy.mp3</v>
       </c>
-      <c r="E6" s="1" t="str">
+      <c r="G6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Berserk OP1 - Easy', 'Tell Me Why', 'Anime', './anime/Berserk OP1 - Easy.mp3');</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="str">
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Berserk OP1 - Hard.mp3</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="G7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Berserk OP1 - Hard', 'Tell Me Why', 'Anime', './anime/Berserk OP1 - Hard.mp3');</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="str">
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Chainsaw Man OP1 - Easy.mp3</v>
       </c>
-      <c r="E8" s="1" t="str">
+      <c r="G8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Kick Back', 'Anime', './anime/Chainsaw Man OP1 - Easy.mp3');</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="str">
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Chainsaw Man OP1 - Hard.mp3</v>
       </c>
-      <c r="E9" s="1" t="str">
+      <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Kick Back', 'Anime', './anime/Chainsaw Man OP1 - Hard.mp3');</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="str">
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Code Geass OP1 - Easy.mp3</v>
       </c>
-      <c r="E10" s="1" t="str">
+      <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Code Geass OP1 - Easy', 'COLORS', 'Anime', './anime/Code Geass OP1 - Easy.mp3');</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="str">
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Code Geass OP1 - Hard.mp3</v>
       </c>
-      <c r="E11" s="1" t="str">
+      <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Code Geass OP1 - Hard', 'COLORS', 'Anime', './anime/Code Geass OP1 - Hard.mp3');</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="str">
-        <f>"./"&amp;LOWER(C12)&amp;"/"&amp;A12&amp;".mp3"</f>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="str">
+        <f>"./"&amp;LOWER(E12)&amp;"/"&amp;A12&amp;".mp3"</f>
         <v>./anime/Death Note OP1 - Easy.mp3</v>
       </c>
-      <c r="E12" s="1" t="str">
-        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A12&amp;"'"&amp;", "&amp;"'"&amp;B12&amp;"'"&amp;", "&amp;"'"&amp;C12&amp;"'"&amp;", "&amp;"'"&amp;D12&amp;"'"&amp;");"</f>
+      <c r="G12" s="1" t="str">
+        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A12&amp;"'"&amp;", "&amp;"'"&amp;D12&amp;"'"&amp;", "&amp;"'"&amp;E12&amp;"'"&amp;", "&amp;"'"&amp;F12&amp;"'"&amp;");"</f>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Note OP1 - Easy', 'The World', 'Anime', './anime/Death Note OP1 - Easy.mp3');</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="str">
-        <f>"./"&amp;LOWER(C13)&amp;"/"&amp;A13&amp;".mp3"</f>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="str">
+        <f>"./"&amp;LOWER(E13)&amp;"/"&amp;A13&amp;".mp3"</f>
         <v>./anime/Death Note OP1 - Hard.mp3</v>
       </c>
-      <c r="E13" s="1" t="str">
-        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A13&amp;"'"&amp;", "&amp;"'"&amp;B13&amp;"'"&amp;", "&amp;"'"&amp;C13&amp;"'"&amp;", "&amp;"'"&amp;D13&amp;"'"&amp;");"</f>
+      <c r="G13" s="1" t="str">
+        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A13&amp;"'"&amp;", "&amp;"'"&amp;D13&amp;"'"&amp;", "&amp;"'"&amp;E13&amp;"'"&amp;", "&amp;"'"&amp;F13&amp;"'"&amp;");"</f>
         <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Note OP1 - Hard', 'The World', 'Anime', './anime/Death Note OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" ref="F14:F31" si="2">"./"&amp;LOWER(E14)&amp;"/"&amp;A14&amp;".mp3"</f>
+        <v>./anime/Death Parade OP1 - Easy.mp3</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f t="shared" ref="G14:G31" si="3">"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A14&amp;"'"&amp;", "&amp;"'"&amp;D14&amp;"'"&amp;", "&amp;"'"&amp;E14&amp;"'"&amp;", "&amp;"'"&amp;F14&amp;"'"&amp;");"</f>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Parade OP1 - Easy', 'Flyers', 'Anime', './anime/Death Parade OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Death Parade OP1 - Hard.mp3</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Parade OP1 - Hard', 'Flyers', 'Anime', './anime/Death Parade OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Dragon Ball Z OP1 - Easy.mp3</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Dragon Ball Z OP1 - Easy', 'Cha-La Head-Cha-La', 'Anime', './anime/Dragon Ball Z OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Dragon Ball Z OP1 - Hard.mp3</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Dragon Ball Z OP1 - Hard', 'Cha-La Head-Cha-La', 'Anime', './anime/Dragon Ball Z OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Ergo Proxy OP1 - Easy.mp3</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Ergo Proxy OP1 - Easy', 'Kiri', 'Anime', './anime/Ergo Proxy OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Ergo Proxy OP1 - Hard.mp3</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Ergo Proxy OP1 - Hard', 'Kiri', 'Anime', './anime/Ergo Proxy OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Evangelion OP1 - Easy.mp3</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Evangelion OP1 - Easy', 'A Cruel Angel''s Thesis', 'Anime', './anime/Evangelion OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Evangelion OP1 - Hard.mp3</v>
+      </c>
+      <c r="G21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Evangelion OP1 - Hard', 'A Cruel Angel''s Thesis', 'Anime', './anime/Evangelion OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Fate Stay Night UBW OP2 - Easy.mp3</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Brave Shine', 'Anime', './anime/Fate Stay Night UBW OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Fate Stay Night UBW OP2 - Hard.mp3</v>
+      </c>
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Brave Shine', 'Anime', './anime/Fate Stay Night UBW OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Guilty Crown OP1 - Easy.mp3</v>
+      </c>
+      <c r="G24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Guilty Crown OP1 - Easy', 'My Dearest', 'Anime', './anime/Guilty Crown OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Guilty Crown OP1 - Hard.mp3</v>
+      </c>
+      <c r="G25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Guilty Crown OP1 - Hard', 'My Dearest', 'Anime', './anime/Guilty Crown OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Jojo OP2 - Easy.mp3</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jojo OP2 - Easy', 'Bloody Stream', 'Anime', './anime/Jojo OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Jojo OP2 - Hard.mp3</v>
+      </c>
+      <c r="G27" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jojo OP2 - Hard', 'Bloody Stream', 'Anime', './anime/Jojo OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Jujutsu Kaisen OP2 - Easy.mp3</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Vivid Vice', 'Anime', './anime/Jujutsu Kaisen OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Jujutsu Kaisen OP2 - Hard.mp3</v>
+      </c>
+      <c r="G29" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Vivid Vice', 'Anime', './anime/Jujutsu Kaisen OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/One Punch Man OP1 - Easy.mp3</v>
+      </c>
+      <c r="G30" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('One Punch Man OP1 - Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'Anime', './anime/One Punch Man OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/One Punch Man OP1 - Hard.mp3</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('One Punch Man OP1 - Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'Anime', './anime/One Punch Man OP1 - Hard.mp3');</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4588B35-0419-4A99-A836-6C071068D931}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4660A0F-0001-4A59-8D0F-2E53EB11BF5C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CA925E-03FE-40D3-AABA-1A74A02935DE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FAF1CE-36A1-4CA5-ABB7-09355FB87B89}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding SQL calls, preparing frontend to include info from database
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B1532E-6DB7-4F2B-B8A6-DCEFD0FA8418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD1D16D-79DA-4DEF-8ED6-0C467852D707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="112">
   <si>
     <t>Name</t>
   </si>
@@ -234,9 +226,6 @@
     <t>Fate Stay Night - Unlimited Blade Works</t>
   </si>
   <si>
-    <t>Jojo's Bizarre Adventure</t>
-  </si>
-  <si>
     <t>One Punch Man</t>
   </si>
   <si>
@@ -250,6 +239,132 @@
   </si>
   <si>
     <t>Song</t>
+  </si>
+  <si>
+    <t>Psycho Pass OP2 - Easy</t>
+  </si>
+  <si>
+    <t>Psycho Pass OP2 - Hard</t>
+  </si>
+  <si>
+    <t>Ranking of Kings OP2 - Easy</t>
+  </si>
+  <si>
+    <t>Ranking of Kings OP2 - Hard</t>
+  </si>
+  <si>
+    <t>Soul Eater OP2 - Easy</t>
+  </si>
+  <si>
+    <t>Soul Eater OP2 - Hard</t>
+  </si>
+  <si>
+    <t>Tokyo Ghoul OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Tokyo Ghoul OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Vinland Saga OP1 - Easy</t>
+  </si>
+  <si>
+    <t>Vinland Saga OP1 - Hard</t>
+  </si>
+  <si>
+    <t>Psycho Pass</t>
+  </si>
+  <si>
+    <t>Soul Eater</t>
+  </si>
+  <si>
+    <t>Tokyo Ghoul</t>
+  </si>
+  <si>
+    <t>Vinland Saga</t>
+  </si>
+  <si>
+    <t>Ranking of Kings</t>
+  </si>
+  <si>
+    <t>Out of Control</t>
+  </si>
+  <si>
+    <t>Naked Hero</t>
+  </si>
+  <si>
+    <t>Black Paper Moon</t>
+  </si>
+  <si>
+    <t>Unravel</t>
+  </si>
+  <si>
+    <t>Mukanjyo</t>
+  </si>
+  <si>
+    <t>Artist</t>
+  </si>
+  <si>
+    <t>Lia</t>
+  </si>
+  <si>
+    <t>Linked Horizon</t>
+  </si>
+  <si>
+    <t>PENPALS</t>
+  </si>
+  <si>
+    <t>Kenshi Yonezu</t>
+  </si>
+  <si>
+    <t>FLOW</t>
+  </si>
+  <si>
+    <t>Nightmare</t>
+  </si>
+  <si>
+    <t>BRADIO</t>
+  </si>
+  <si>
+    <t>Hironobu Kageyama</t>
+  </si>
+  <si>
+    <t>Monoral</t>
+  </si>
+  <si>
+    <t>Yoko Takahashi</t>
+  </si>
+  <si>
+    <t>Aimer</t>
+  </si>
+  <si>
+    <t>Koeda</t>
+  </si>
+  <si>
+    <t>Coda</t>
+  </si>
+  <si>
+    <t>Who-Ya Extended</t>
+  </si>
+  <si>
+    <t>JAM Project</t>
+  </si>
+  <si>
+    <t>Vaundy</t>
+  </si>
+  <si>
+    <t>Tomoko Kawase</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>Survive Said The Prophet</t>
+  </si>
+  <si>
+    <t>Jojo''s Bizarre Adventure</t>
+  </si>
+  <si>
+    <t>Nothing''s Carved in Stone</t>
   </si>
 </sst>
 </file>
@@ -604,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,12 +731,13 @@
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="97.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="97.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -629,22 +745,25 @@
         <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -652,24 +771,27 @@
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F11" si="0">"./"&amp;LOWER(E2)&amp;"/"&amp;A2&amp;".mp3"</f>
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G11" si="0">"./"&amp;LOWER(F2)&amp;"/"&amp;A2&amp;".mp3"</f>
         <v>./anime/Angel Beats OP1 - Easy.mp3</v>
       </c>
-      <c r="G2" s="1" t="str">
-        <f t="shared" ref="G2:G11" si="1">"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;");"</f>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Angel Beats OP1 - Easy', 'My Soul, Your Beats!', 'Anime', './anime/Angel Beats OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="str">
+        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', './anime/Angel Beats OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -677,24 +799,27 @@
         <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="str">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Angel Beats OP1 - Hard.mp3</v>
       </c>
-      <c r="G3" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Angel Beats OP1 - Hard', 'My Soul, Your Beats!', 'Anime', './anime/Angel Beats OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H3:H41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', './anime/Angel Beats OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -702,24 +827,27 @@
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="str">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Attack On Titan OP1 - Easy.mp3</v>
       </c>
-      <c r="G4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Guren no Yumiya', 'Anime', './anime/Attack On Titan OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', './anime/Attack On Titan OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -727,24 +855,27 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="str">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Attack On Titan OP1 - Hard.mp3</v>
       </c>
-      <c r="G5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Guren no Yumiya', 'Anime', './anime/Attack On Titan OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', './anime/Attack On Titan OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -752,24 +883,27 @@
         <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="str">
+        <v>93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Berserk OP1 - Easy.mp3</v>
       </c>
-      <c r="G6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Berserk OP1 - Easy', 'Tell Me Why', 'Anime', './anime/Berserk OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', './anime/Berserk OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -777,24 +911,27 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="str">
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Berserk OP1 - Hard.mp3</v>
       </c>
-      <c r="G7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Berserk OP1 - Hard', 'Tell Me Why', 'Anime', './anime/Berserk OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', './anime/Berserk OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -802,24 +939,27 @@
         <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" t="str">
+        <v>94</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Chainsaw Man OP1 - Easy.mp3</v>
       </c>
-      <c r="G8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Kick Back', 'Anime', './anime/Chainsaw Man OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', './anime/Chainsaw Man OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -827,24 +967,27 @@
         <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
         <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="str">
+        <v>94</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Chainsaw Man OP1 - Hard.mp3</v>
       </c>
-      <c r="G9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Kick Back', 'Anime', './anime/Chainsaw Man OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', './anime/Chainsaw Man OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -852,24 +995,27 @@
         <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="str">
+        <v>95</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Code Geass OP1 - Easy.mp3</v>
       </c>
-      <c r="G10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Code Geass OP1 - Easy', 'COLORS', 'Anime', './anime/Code Geass OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', './anime/Code Geass OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -877,24 +1023,27 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" t="str">
+        <v>95</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>./anime/Code Geass OP1 - Hard.mp3</v>
       </c>
-      <c r="G11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Code Geass OP1 - Hard', 'COLORS', 'Anime', './anime/Code Geass OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', './anime/Code Geass OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -902,24 +1051,27 @@
         <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" t="str">
-        <f>"./"&amp;LOWER(E12)&amp;"/"&amp;A12&amp;".mp3"</f>
+        <v>96</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="str">
+        <f>"./"&amp;LOWER(F12)&amp;"/"&amp;A12&amp;".mp3"</f>
         <v>./anime/Death Note OP1 - Easy.mp3</v>
       </c>
-      <c r="G12" s="1" t="str">
-        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A12&amp;"'"&amp;", "&amp;"'"&amp;D12&amp;"'"&amp;", "&amp;"'"&amp;E12&amp;"'"&amp;", "&amp;"'"&amp;F12&amp;"'"&amp;");"</f>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Note OP1 - Easy', 'The World', 'Anime', './anime/Death Note OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', './anime/Death Note OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -927,24 +1079,27 @@
         <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" t="str">
-        <f>"./"&amp;LOWER(E13)&amp;"/"&amp;A13&amp;".mp3"</f>
+        <v>96</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="str">
+        <f>"./"&amp;LOWER(F13)&amp;"/"&amp;A13&amp;".mp3"</f>
         <v>./anime/Death Note OP1 - Hard.mp3</v>
       </c>
-      <c r="G13" s="1" t="str">
-        <f>"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A13&amp;"'"&amp;", "&amp;"'"&amp;D13&amp;"'"&amp;", "&amp;"'"&amp;E13&amp;"'"&amp;", "&amp;"'"&amp;F13&amp;"'"&amp;");"</f>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Note OP1 - Hard', 'The World', 'Anime', './anime/Death Note OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', './anime/Death Note OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -952,24 +1107,27 @@
         <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
         <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" ref="F14:F31" si="2">"./"&amp;LOWER(E14)&amp;"/"&amp;A14&amp;".mp3"</f>
+        <v>97</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" ref="G14:G41" si="2">"./"&amp;LOWER(F14)&amp;"/"&amp;A14&amp;".mp3"</f>
         <v>./anime/Death Parade OP1 - Easy.mp3</v>
       </c>
-      <c r="G14" s="1" t="str">
-        <f t="shared" ref="G14:G31" si="3">"INSERT INTO songs (name, song_name, category, location) VALUES ('"&amp;A14&amp;"'"&amp;", "&amp;"'"&amp;D14&amp;"'"&amp;", "&amp;"'"&amp;E14&amp;"'"&amp;", "&amp;"'"&amp;F14&amp;"'"&amp;");"</f>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Parade OP1 - Easy', 'Flyers', 'Anime', './anime/Death Parade OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', './anime/Death Parade OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -977,24 +1135,27 @@
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
         <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" t="str">
+        <v>97</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Death Parade OP1 - Hard.mp3</v>
       </c>
-      <c r="G15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Death Parade OP1 - Hard', 'Flyers', 'Anime', './anime/Death Parade OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', './anime/Death Parade OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1002,24 +1163,27 @@
         <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" t="str">
+        <v>98</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Dragon Ball Z OP1 - Easy.mp3</v>
       </c>
-      <c r="G16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Dragon Ball Z OP1 - Easy', 'Cha-La Head-Cha-La', 'Anime', './anime/Dragon Ball Z OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', './anime/Dragon Ball Z OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1027,24 +1191,27 @@
         <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" t="str">
+        <v>98</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Dragon Ball Z OP1 - Hard.mp3</v>
       </c>
-      <c r="G17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Dragon Ball Z OP1 - Hard', 'Cha-La Head-Cha-La', 'Anime', './anime/Dragon Ball Z OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', './anime/Dragon Ball Z OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1052,24 +1219,27 @@
         <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="str">
+        <v>99</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Ergo Proxy OP1 - Easy.mp3</v>
       </c>
-      <c r="G18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Ergo Proxy OP1 - Easy', 'Kiri', 'Anime', './anime/Ergo Proxy OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', './anime/Ergo Proxy OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1077,24 +1247,27 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
         <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" t="str">
+        <v>99</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Ergo Proxy OP1 - Hard.mp3</v>
       </c>
-      <c r="G19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Ergo Proxy OP1 - Hard', 'Kiri', 'Anime', './anime/Ergo Proxy OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', './anime/Ergo Proxy OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1102,24 +1275,27 @@
         <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" t="str">
+        <v>100</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Evangelion OP1 - Easy.mp3</v>
       </c>
-      <c r="G20" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Evangelion OP1 - Easy', 'A Cruel Angel''s Thesis', 'Anime', './anime/Evangelion OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', './anime/Evangelion OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1127,24 +1303,27 @@
         <v>63</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" t="str">
+        <v>100</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Evangelion OP1 - Hard.mp3</v>
       </c>
-      <c r="G21" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Evangelion OP1 - Hard', 'A Cruel Angel''s Thesis', 'Anime', './anime/Evangelion OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', './anime/Evangelion OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1152,24 +1331,27 @@
         <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
         <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" t="str">
+        <v>101</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Fate Stay Night UBW OP2 - Easy.mp3</v>
       </c>
-      <c r="G22" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Brave Shine', 'Anime', './anime/Fate Stay Night UBW OP2 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', './anime/Fate Stay Night UBW OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1177,24 +1359,27 @@
         <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
         <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" t="str">
+        <v>101</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Fate Stay Night UBW OP2 - Hard.mp3</v>
       </c>
-      <c r="G23" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Brave Shine', 'Anime', './anime/Fate Stay Night UBW OP2 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', './anime/Fate Stay Night UBW OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1202,24 +1387,27 @@
         <v>61</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" t="str">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Guilty Crown OP1 - Easy.mp3</v>
       </c>
-      <c r="G24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Guilty Crown OP1 - Easy', 'My Dearest', 'Anime', './anime/Guilty Crown OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', './anime/Guilty Crown OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1227,74 +1415,83 @@
         <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" t="str">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Guilty Crown OP1 - Hard.mp3</v>
       </c>
-      <c r="G25" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Guilty Crown OP1 - Hard', 'My Dearest', 'Anime', './anime/Guilty Crown OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', './anime/Guilty Crown OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
         <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="str">
+        <v>103</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Jojo OP2 - Easy.mp3</v>
       </c>
-      <c r="G26" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jojo OP2 - Easy', 'Bloody Stream', 'Anime', './anime/Jojo OP2 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', './anime/Jojo OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
         <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" t="str">
+        <v>103</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Jojo OP2 - Hard.mp3</v>
       </c>
-      <c r="G27" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jojo OP2 - Hard', 'Bloody Stream', 'Anime', './anime/Jojo OP2 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', './anime/Jojo OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1302,24 +1499,27 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
         <v>48</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="str">
+        <v>104</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Jujutsu Kaisen OP2 - Easy.mp3</v>
       </c>
-      <c r="G28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Vivid Vice', 'Anime', './anime/Jujutsu Kaisen OP2 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', './anime/Jujutsu Kaisen OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1327,71 +1527,360 @@
         <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" t="str">
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" t="str">
         <f t="shared" si="2"/>
         <v>./anime/Jujutsu Kaisen OP2 - Hard.mp3</v>
       </c>
-      <c r="G29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Vivid Vice', 'Anime', './anime/Jujutsu Kaisen OP2 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', './anime/Jujutsu Kaisen OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
         <v>49</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" t="str">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="str">
         <f t="shared" si="2"/>
         <v>./anime/One Punch Man OP1 - Easy.mp3</v>
       </c>
-      <c r="G30" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('One Punch Man OP1 - Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'Anime', './anime/One Punch Man OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', './anime/One Punch Man OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
         <v>49</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="str">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="str">
         <f t="shared" si="2"/>
         <v>./anime/One Punch Man OP1 - Hard.mp3</v>
       </c>
-      <c r="G31" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, song_name, category, location) VALUES ('One Punch Man OP1 - Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'Anime', './anime/One Punch Man OP1 - Hard.mp3');</v>
+      <c r="H31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', './anime/One Punch Man OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Psycho Pass OP2 - Easy.mp3</v>
+      </c>
+      <c r="H32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', './anime/Psycho Pass OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Psycho Pass OP2 - Hard.mp3</v>
+      </c>
+      <c r="H33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', './anime/Psycho Pass OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Ranking of Kings OP2 - Easy.mp3</v>
+      </c>
+      <c r="H34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', './anime/Ranking of Kings OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Ranking of Kings OP2 - Hard.mp3</v>
+      </c>
+      <c r="H35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', './anime/Ranking of Kings OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Soul Eater OP2 - Easy.mp3</v>
+      </c>
+      <c r="H36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', './anime/Soul Eater OP2 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Soul Eater OP2 - Hard.mp3</v>
+      </c>
+      <c r="H37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', './anime/Soul Eater OP2 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Tokyo Ghoul OP1 - Easy.mp3</v>
+      </c>
+      <c r="H38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', './anime/Tokyo Ghoul OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>88</v>
+      </c>
+      <c r="E39" t="s">
+        <v>108</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Tokyo Ghoul OP1 - Hard.mp3</v>
+      </c>
+      <c r="H39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', './anime/Tokyo Ghoul OP1 - Hard.mp3');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Vinland Saga OP1 - Easy.mp3</v>
+      </c>
+      <c r="H40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', './anime/Vinland Saga OP1 - Easy.mp3');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="2"/>
+        <v>./anime/Vinland Saga OP1 - Hard.mp3</v>
+      </c>
+      <c r="H41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', './anime/Vinland Saga OP1 - Hard.mp3');</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +1922,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added random music track playback
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD1D16D-79DA-4DEF-8ED6-0C467852D707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B696C98F-CC20-4811-8F6B-2C7441B78774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -721,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,12 +791,12 @@
         <v>7</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G11" si="0">"./"&amp;LOWER(F2)&amp;"/"&amp;A2&amp;".mp3"</f>
-        <v>./anime/Angel Beats OP1 - Easy.mp3</v>
+        <f>"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
+        <v>music/anime/Angel Beats OP1 - Easy</v>
       </c>
       <c r="H2" s="1" t="str">
         <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', './anime/Angel Beats OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Easy');</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -811,12 +819,12 @@
         <v>7</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>./anime/Angel Beats OP1 - Hard.mp3</v>
+        <f t="shared" ref="G3:G41" si="0">"music/"&amp;LOWER(F3)&amp;"/"&amp;A3</f>
+        <v>music/anime/Angel Beats OP1 - Hard</v>
       </c>
       <c r="H3" s="1" t="str">
         <f t="shared" ref="H3:H41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', './anime/Angel Beats OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Hard');</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -840,11 +848,11 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Attack On Titan OP1 - Easy.mp3</v>
+        <v>music/anime/Attack On Titan OP1 - Easy</v>
       </c>
       <c r="H4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', './anime/Attack On Titan OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Easy');</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -868,14 +876,14 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Attack On Titan OP1 - Hard.mp3</v>
+        <v>music/anime/Attack On Titan OP1 - Hard</v>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', './anime/Attack On Titan OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Hard');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -896,14 +904,14 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Berserk OP1 - Easy.mp3</v>
+        <v>music/anime/Berserk OP1 - Easy</v>
       </c>
       <c r="H6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', './anime/Berserk OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Easy');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -924,11 +932,11 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Berserk OP1 - Hard.mp3</v>
+        <v>music/anime/Berserk OP1 - Hard</v>
       </c>
       <c r="H7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', './anime/Berserk OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Hard');</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -952,11 +960,11 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Chainsaw Man OP1 - Easy.mp3</v>
+        <v>music/anime/Chainsaw Man OP1 - Easy</v>
       </c>
       <c r="H8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', './anime/Chainsaw Man OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Easy');</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -980,14 +988,14 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Chainsaw Man OP1 - Hard.mp3</v>
+        <v>music/anime/Chainsaw Man OP1 - Hard</v>
       </c>
       <c r="H9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', './anime/Chainsaw Man OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Hard');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1008,14 +1016,14 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Code Geass OP1 - Easy.mp3</v>
+        <v>music/anime/Code Geass OP1 - Easy</v>
       </c>
       <c r="H10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', './anime/Code Geass OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Easy');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1036,14 +1044,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>./anime/Code Geass OP1 - Hard.mp3</v>
+        <v>music/anime/Code Geass OP1 - Hard</v>
       </c>
       <c r="H11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', './anime/Code Geass OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Hard');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1063,15 +1071,15 @@
         <v>7</v>
       </c>
       <c r="G12" t="str">
-        <f>"./"&amp;LOWER(F12)&amp;"/"&amp;A12&amp;".mp3"</f>
-        <v>./anime/Death Note OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Death Note OP1 - Easy</v>
       </c>
       <c r="H12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', './anime/Death Note OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Easy');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1091,12 +1099,12 @@
         <v>7</v>
       </c>
       <c r="G13" t="str">
-        <f>"./"&amp;LOWER(F13)&amp;"/"&amp;A13&amp;".mp3"</f>
-        <v>./anime/Death Note OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Death Note OP1 - Hard</v>
       </c>
       <c r="H13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', './anime/Death Note OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Hard');</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1119,12 +1127,12 @@
         <v>7</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" ref="G14:G41" si="2">"./"&amp;LOWER(F14)&amp;"/"&amp;A14&amp;".mp3"</f>
-        <v>./anime/Death Parade OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Death Parade OP1 - Easy</v>
       </c>
       <c r="H14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', './anime/Death Parade OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Easy');</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1147,12 +1155,12 @@
         <v>7</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Death Parade OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Death Parade OP1 - Hard</v>
       </c>
       <c r="H15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', './anime/Death Parade OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Hard');</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1175,12 +1183,12 @@
         <v>7</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Dragon Ball Z OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Dragon Ball Z OP1 - Easy</v>
       </c>
       <c r="H16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', './anime/Dragon Ball Z OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Easy');</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1203,15 +1211,15 @@
         <v>7</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Dragon Ball Z OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Dragon Ball Z OP1 - Hard</v>
       </c>
       <c r="H17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', './anime/Dragon Ball Z OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Hard');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1231,15 +1239,15 @@
         <v>7</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Ergo Proxy OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Ergo Proxy OP1 - Easy</v>
       </c>
       <c r="H18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', './anime/Ergo Proxy OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Easy');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1259,12 +1267,12 @@
         <v>7</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Ergo Proxy OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Ergo Proxy OP1 - Hard</v>
       </c>
       <c r="H19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', './anime/Ergo Proxy OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Hard');</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1287,12 +1295,12 @@
         <v>7</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Evangelion OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Evangelion OP1 - Easy</v>
       </c>
       <c r="H20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', './anime/Evangelion OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Easy');</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1315,12 +1323,12 @@
         <v>7</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Evangelion OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Evangelion OP1 - Hard</v>
       </c>
       <c r="H21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', './anime/Evangelion OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Hard');</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1343,12 +1351,12 @@
         <v>7</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Fate Stay Night UBW OP2 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Fate Stay Night UBW OP2 - Easy</v>
       </c>
       <c r="H22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', './anime/Fate Stay Night UBW OP2 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Easy');</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1371,12 +1379,12 @@
         <v>7</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Fate Stay Night UBW OP2 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Fate Stay Night UBW OP2 - Hard</v>
       </c>
       <c r="H23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', './anime/Fate Stay Night UBW OP2 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Hard');</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1399,12 +1407,12 @@
         <v>7</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Guilty Crown OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Guilty Crown OP1 - Easy</v>
       </c>
       <c r="H24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', './anime/Guilty Crown OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Easy');</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1427,15 +1435,15 @@
         <v>7</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Guilty Crown OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Guilty Crown OP1 - Hard</v>
       </c>
       <c r="H25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', './anime/Guilty Crown OP1 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Hard');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1455,15 +1463,15 @@
         <v>7</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Jojo OP2 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Jojo OP2 - Easy</v>
       </c>
       <c r="H26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', './anime/Jojo OP2 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Easy');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1483,12 +1491,12 @@
         <v>7</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Jojo OP2 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Jojo OP2 - Hard</v>
       </c>
       <c r="H27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', './anime/Jojo OP2 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Hard');</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1511,12 +1519,12 @@
         <v>7</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Jujutsu Kaisen OP2 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Jujutsu Kaisen OP2 - Easy</v>
       </c>
       <c r="H28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', './anime/Jujutsu Kaisen OP2 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Easy');</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1539,12 +1547,12 @@
         <v>7</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Jujutsu Kaisen OP2 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Jujutsu Kaisen OP2 - Hard</v>
       </c>
       <c r="H29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', './anime/Jujutsu Kaisen OP2 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Hard');</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1567,12 +1575,12 @@
         <v>7</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/One Punch Man OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/One Punch Man OP1 - Easy</v>
       </c>
       <c r="H30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', './anime/One Punch Man OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Easy');</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1595,12 +1603,12 @@
         <v>7</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/One Punch Man OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/One Punch Man OP1 - Hard</v>
       </c>
       <c r="H31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', './anime/One Punch Man OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Hard');</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1623,12 +1631,12 @@
         <v>7</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Psycho Pass OP2 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Psycho Pass OP2 - Easy</v>
       </c>
       <c r="H32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', './anime/Psycho Pass OP2 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Easy');</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1651,12 +1659,12 @@
         <v>7</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Psycho Pass OP2 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Psycho Pass OP2 - Hard</v>
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', './anime/Psycho Pass OP2 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Hard');</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1679,12 +1687,12 @@
         <v>7</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Ranking of Kings OP2 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Ranking of Kings OP2 - Easy</v>
       </c>
       <c r="H34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', './anime/Ranking of Kings OP2 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Easy');</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1707,12 +1715,12 @@
         <v>7</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Ranking of Kings OP2 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Ranking of Kings OP2 - Hard</v>
       </c>
       <c r="H35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', './anime/Ranking of Kings OP2 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Hard');</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1735,12 +1743,12 @@
         <v>7</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Soul Eater OP2 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Soul Eater OP2 - Easy</v>
       </c>
       <c r="H36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', './anime/Soul Eater OP2 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Easy');</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1763,15 +1771,15 @@
         <v>7</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Soul Eater OP2 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Soul Eater OP2 - Hard</v>
       </c>
       <c r="H37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', './anime/Soul Eater OP2 - Hard.mp3');</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Hard');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1791,15 +1799,15 @@
         <v>7</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Tokyo Ghoul OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Tokyo Ghoul OP1 - Easy</v>
       </c>
       <c r="H38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', './anime/Tokyo Ghoul OP1 - Easy.mp3');</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Easy');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1819,12 +1827,12 @@
         <v>7</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Tokyo Ghoul OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Tokyo Ghoul OP1 - Hard</v>
       </c>
       <c r="H39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', './anime/Tokyo Ghoul OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Hard');</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1847,12 +1855,12 @@
         <v>7</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Vinland Saga OP1 - Easy.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Vinland Saga OP1 - Easy</v>
       </c>
       <c r="H40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', './anime/Vinland Saga OP1 - Easy.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Easy');</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1875,12 +1883,12 @@
         <v>7</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="2"/>
-        <v>./anime/Vinland Saga OP1 - Hard.mp3</v>
+        <f t="shared" si="0"/>
+        <v>music/anime/Vinland Saga OP1 - Hard</v>
       </c>
       <c r="H41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', './anime/Vinland Saga OP1 - Hard.mp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Hard');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally finished question answer logic, started working on video URL links
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B696C98F-CC20-4811-8F6B-2C7441B78774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C39F3D-E5BF-46EE-AD41-1D6A00EC5301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,20 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -373,6 +365,12 @@
   </si>
   <si>
     <t>Nothing''s Carved in Stone</t>
+  </si>
+  <si>
+    <t>Video Link</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/kNyR46eHDxE</t>
   </si>
 </sst>
 </file>
@@ -408,11 +406,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,10 +741,11 @@
     <col min="5" max="5" width="40.28515625" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="97.140625" customWidth="1"/>
+    <col min="8" max="8" width="42.140625" customWidth="1"/>
+    <col min="9" max="9" width="107.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -768,10 +768,13 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -794,12 +797,12 @@
         <f>"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
         <v>music/anime/Angel Beats OP1 - Easy</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="str">
+        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;", "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -822,12 +825,12 @@
         <f t="shared" ref="G3:G41" si="0">"music/"&amp;LOWER(F3)&amp;"/"&amp;A3</f>
         <v>music/anime/Angel Beats OP1 - Hard</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;", "&amp;"'"&amp;H3&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -850,12 +853,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Attack On Titan OP1 - Easy</v>
       </c>
-      <c r="H4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -878,12 +881,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Attack On Titan OP1 - Hard</v>
       </c>
-      <c r="H5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -906,12 +909,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Berserk OP1 - Easy</v>
       </c>
-      <c r="H6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -934,12 +937,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Berserk OP1 - Hard</v>
       </c>
-      <c r="H7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -962,12 +965,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Chainsaw Man OP1 - Easy</v>
       </c>
-      <c r="H8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -990,12 +993,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Chainsaw Man OP1 - Hard</v>
       </c>
-      <c r="H9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1018,12 +1021,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Code Geass OP1 - Easy</v>
       </c>
-      <c r="H10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1046,12 +1049,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Code Geass OP1 - Hard</v>
       </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1074,12 +1077,15 @@
         <f t="shared" si="0"/>
         <v>music/anime/Death Note OP1 - Easy</v>
       </c>
-      <c r="H12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Easy, 'https://www.youtube.com/embed/kNyR46eHDxE');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1102,12 +1108,15 @@
         <f t="shared" si="0"/>
         <v>music/anime/Death Note OP1 - Hard</v>
       </c>
-      <c r="H13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Hard, 'https://www.youtube.com/embed/kNyR46eHDxE');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1130,12 +1139,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Death Parade OP1 - Easy</v>
       </c>
-      <c r="H14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1158,12 +1167,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Death Parade OP1 - Hard</v>
       </c>
-      <c r="H15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1186,12 +1195,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Dragon Ball Z OP1 - Easy</v>
       </c>
-      <c r="H16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1214,12 +1223,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Dragon Ball Z OP1 - Hard</v>
       </c>
-      <c r="H17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1242,12 +1251,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Ergo Proxy OP1 - Easy</v>
       </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1270,12 +1279,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Ergo Proxy OP1 - Hard</v>
       </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1298,12 +1307,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Evangelion OP1 - Easy</v>
       </c>
-      <c r="H20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1326,12 +1335,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Evangelion OP1 - Hard</v>
       </c>
-      <c r="H21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1354,12 +1363,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Fate Stay Night UBW OP2 - Easy</v>
       </c>
-      <c r="H22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Easy');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1382,12 +1391,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Fate Stay Night UBW OP2 - Hard</v>
       </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Hard');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1410,12 +1419,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Guilty Crown OP1 - Easy</v>
       </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1438,12 +1447,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Guilty Crown OP1 - Hard</v>
       </c>
-      <c r="H25" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1466,12 +1475,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Jojo OP2 - Easy</v>
       </c>
-      <c r="H26" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Easy');</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1494,12 +1503,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Jojo OP2 - Hard</v>
       </c>
-      <c r="H27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Hard');</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1522,12 +1531,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Jujutsu Kaisen OP2 - Easy</v>
       </c>
-      <c r="H28" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Easy');</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1550,12 +1559,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Jujutsu Kaisen OP2 - Hard</v>
       </c>
-      <c r="H29" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Hard');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1578,12 +1587,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/One Punch Man OP1 - Easy</v>
       </c>
-      <c r="H30" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1606,12 +1615,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/One Punch Man OP1 - Hard</v>
       </c>
-      <c r="H31" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1634,12 +1643,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Psycho Pass OP2 - Easy</v>
       </c>
-      <c r="H32" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Easy');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1662,12 +1671,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Psycho Pass OP2 - Hard</v>
       </c>
-      <c r="H33" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Hard');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
@@ -1690,12 +1699,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Ranking of Kings OP2 - Easy</v>
       </c>
-      <c r="H34" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Easy');</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1718,12 +1727,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Ranking of Kings OP2 - Hard</v>
       </c>
-      <c r="H35" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Hard');</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1746,12 +1755,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Soul Eater OP2 - Easy</v>
       </c>
-      <c r="H36" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Easy');</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1774,12 +1783,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Soul Eater OP2 - Hard</v>
       </c>
-      <c r="H37" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Hard');</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1802,12 +1811,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Tokyo Ghoul OP1 - Easy</v>
       </c>
-      <c r="H38" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1830,12 +1839,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Tokyo Ghoul OP1 - Hard</v>
       </c>
-      <c r="H39" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Hard');</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Hard, '');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1858,12 +1867,12 @@
         <f t="shared" si="0"/>
         <v>music/anime/Vinland Saga OP1 - Easy</v>
       </c>
-      <c r="H40" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Easy');</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Easy, '');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -1886,9 +1895,9 @@
         <f t="shared" si="0"/>
         <v>music/anime/Vinland Saga OP1 - Hard</v>
       </c>
-      <c r="H41" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Hard');</v>
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Hard, '');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementing material ui design
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4F71EC-6057-40D0-9A0E-CCC5BA70465D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDE4300-2823-4E74-A3D9-5FAEF8F5EB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anime" sheetId="1" r:id="rId1"/>
     <sheet name="Indie" sheetId="6" r:id="rId2"/>
-    <sheet name="TV" sheetId="2" r:id="rId3"/>
-    <sheet name="Video Games" sheetId="3" r:id="rId4"/>
+    <sheet name="Games" sheetId="7" r:id="rId3"/>
+    <sheet name="TV" sheetId="2" r:id="rId4"/>
     <sheet name="Top40" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="281">
   <si>
     <t>Name</t>
   </si>
@@ -740,6 +740,138 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN</t>
+  </si>
+  <si>
+    <t>Persona 5 - Easy</t>
+  </si>
+  <si>
+    <t>Persona 5 - Hard</t>
+  </si>
+  <si>
+    <t>Persona 5</t>
+  </si>
+  <si>
+    <t>Last Surprise</t>
+  </si>
+  <si>
+    <t>Video Games</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH</t>
+  </si>
+  <si>
+    <t>Shoji Meguro</t>
+  </si>
+  <si>
+    <t>The Only Thing I Know For Real</t>
+  </si>
+  <si>
+    <t>Metal Gear Rising: Revengeance</t>
+  </si>
+  <si>
+    <t>Edge Of Dawn</t>
+  </si>
+  <si>
+    <t>Fire Emblem: Three Houses</t>
+  </si>
+  <si>
+    <t>Forced Battle</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei III: Nocturne</t>
+  </si>
+  <si>
+    <t>Persona 4</t>
+  </si>
+  <si>
+    <t>Persona 3</t>
+  </si>
+  <si>
+    <t>Code Vein</t>
+  </si>
+  <si>
+    <t>Requiem</t>
+  </si>
+  <si>
+    <t>Ornstein &amp; Smough</t>
+  </si>
+  <si>
+    <t>Dark Souls</t>
+  </si>
+  <si>
+    <t>The Place I'll Return To Someday</t>
+  </si>
+  <si>
+    <t>Outer Wilds</t>
+  </si>
+  <si>
+    <t>14.3 Billion Years</t>
+  </si>
+  <si>
+    <t>Mass Destruction</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei V</t>
+  </si>
+  <si>
+    <t>Spring (The Valley Comes Alive)</t>
+  </si>
+  <si>
+    <t>Stardew Valley</t>
+  </si>
+  <si>
+    <t>Subnautica</t>
+  </si>
+  <si>
+    <t>Abandon Ship</t>
+  </si>
+  <si>
+    <t>Theme Of Laura</t>
+  </si>
+  <si>
+    <t>Silent Hill 2</t>
+  </si>
+  <si>
+    <t>Prologue</t>
+  </si>
+  <si>
+    <t>Shadow Of The Colossus</t>
+  </si>
+  <si>
+    <t>Baba Yetu</t>
+  </si>
+  <si>
+    <t>Civilisation 4</t>
+  </si>
+  <si>
+    <t>Dragonborn (Theme)</t>
+  </si>
+  <si>
+    <t>The Elder Scrolls V: Skyrim</t>
+  </si>
+  <si>
+    <t>Dearly Beloved</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts</t>
+  </si>
+  <si>
+    <t>Final Fantasy X</t>
+  </si>
+  <si>
+    <t>Final Fantasy IX</t>
+  </si>
+  <si>
+    <t>To Zanarkand</t>
+  </si>
+  <si>
+    <t>Final Fantasy VII</t>
+  </si>
+  <si>
+    <t>One Winged Angel</t>
   </si>
 </sst>
 </file>
@@ -2402,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7033B7E-9E28-44F0-AF22-AF8799EBF584}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -3711,7 +3843,7 @@
         <f t="shared" ref="G42:G43" si="2">"music/"&amp;LOWER(F42)&amp;"/"&amp;A42</f>
         <v>music/indie/Iron And Wine - Easy</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" t="s">
         <v>236</v>
       </c>
       <c r="I42" s="1" t="str">
@@ -3742,7 +3874,7 @@
         <f t="shared" si="2"/>
         <v>music/indie/Iron And Wine - Hard</v>
       </c>
-      <c r="H43" s="4" t="s">
+      <c r="H43" t="s">
         <v>236</v>
       </c>
       <c r="I43" s="1" t="str">
@@ -3758,19 +3890,274 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4588B35-0419-4A99-A836-6C071068D931}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F96BC2-62DB-49FB-AD78-FA2CCE8FE0BD}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="107.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" t="s">
+        <v>241</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G3" si="0">"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
+        <v>music/video games/Persona 5 - Easy</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f t="shared" ref="I2:I3" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Easy', 'Persona 5', 'Easy', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Easy', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 5 - Hard</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Hard', 'Persona 5', 'Hard', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Hard', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="D6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>277</v>
+      </c>
+      <c r="D9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>255</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" t="s">
+        <v>258</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+      <c r="D14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>264</v>
+      </c>
+      <c r="D15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>267</v>
+      </c>
+      <c r="D16" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>276</v>
+      </c>
+      <c r="D21" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4660A0F-0001-4A59-8D0F-2E53EB11BF5C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4588B35-0419-4A99-A836-6C071068D931}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Added video games category
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA32E906-F103-433A-BB09-584999D0E078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138FB7C-717C-4DA3-B0CC-E0CAA43A60C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5130" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anime" sheetId="1" r:id="rId1"/>
     <sheet name="Indie" sheetId="6" r:id="rId2"/>
-    <sheet name="Games" sheetId="7" r:id="rId3"/>
-    <sheet name="TV" sheetId="2" r:id="rId4"/>
+    <sheet name="Video Games" sheetId="7" r:id="rId3"/>
+    <sheet name="TV" sheetId="8" r:id="rId4"/>
     <sheet name="Top40" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="358">
   <si>
     <t>Name</t>
   </si>
@@ -382,9 +382,6 @@
     <t>https://www.youtube.com/embed/G8CFuZ9MseQ?si=AcAvfrCQuKQIaW6o</t>
   </si>
   <si>
-    <t>ttps://www.youtube.com/embed/kNyR46eHDxE?si=JJH9imobI4X7YBKI</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/embed/UjjTMNDZi-A?si=NDKOg-OGXXljvXp3</t>
   </si>
   <si>
@@ -766,118 +763,346 @@
     <t>The Only Thing I Know For Real</t>
   </si>
   <si>
-    <t>Metal Gear Rising: Revengeance</t>
-  </si>
-  <si>
     <t>Edge Of Dawn</t>
   </si>
   <si>
-    <t>Fire Emblem: Three Houses</t>
-  </si>
-  <si>
     <t>Forced Battle</t>
   </si>
   <si>
-    <t>Shin Megami Tensei III: Nocturne</t>
-  </si>
-  <si>
     <t>Persona 4</t>
   </si>
   <si>
+    <t>Code Vein</t>
+  </si>
+  <si>
+    <t>Requiem</t>
+  </si>
+  <si>
+    <t>Ornstein &amp; Smough</t>
+  </si>
+  <si>
+    <t>Dark Souls</t>
+  </si>
+  <si>
+    <t>Outer Wilds</t>
+  </si>
+  <si>
+    <t>14.3 Billion Years</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei V</t>
+  </si>
+  <si>
+    <t>Spring (The Valley Comes Alive)</t>
+  </si>
+  <si>
+    <t>Stardew Valley</t>
+  </si>
+  <si>
+    <t>Subnautica</t>
+  </si>
+  <si>
+    <t>Abandon Ship</t>
+  </si>
+  <si>
+    <t>Theme Of Laura</t>
+  </si>
+  <si>
+    <t>Silent Hill 2</t>
+  </si>
+  <si>
+    <t>Prologue</t>
+  </si>
+  <si>
+    <t>Shadow Of The Colossus</t>
+  </si>
+  <si>
+    <t>Baba Yetu</t>
+  </si>
+  <si>
+    <t>Dearly Beloved</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts</t>
+  </si>
+  <si>
+    <t>Final Fantasy X</t>
+  </si>
+  <si>
+    <t>Final Fantasy IX</t>
+  </si>
+  <si>
+    <t>To Zanarkand</t>
+  </si>
+  <si>
+    <t>Final Fantasy VII</t>
+  </si>
+  <si>
+    <t>One Winged Angel</t>
+  </si>
+  <si>
+    <t>I Really Want To Stay At Your House</t>
+  </si>
+  <si>
+    <t>Cyberpunk 2077</t>
+  </si>
+  <si>
+    <t>Outer Wilds - Easy</t>
+  </si>
+  <si>
+    <t>Cyberpunk 2077 - Easy</t>
+  </si>
+  <si>
+    <t>Outer Wilds - Hard</t>
+  </si>
+  <si>
+    <t>Andrew Prahlow</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl</t>
+  </si>
+  <si>
+    <t>Rosa Walton &amp; Hallie Coggins</t>
+  </si>
+  <si>
+    <t>Metal Gear Rising</t>
+  </si>
+  <si>
+    <t>Metal Gear Rising - Easy</t>
+  </si>
+  <si>
+    <t>Metal Gear Rising - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw</t>
+  </si>
+  <si>
+    <t>Fire Emblem Three Houses</t>
+  </si>
+  <si>
+    <t>Fire Emblem Three Houses - Easy</t>
+  </si>
+  <si>
+    <t>Fire Emblem Three Houses - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P</t>
+  </si>
+  <si>
+    <t>Takeru Kanazaki</t>
+  </si>
+  <si>
+    <t>Jamie Christopherson</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei III Nocturne</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei III Nocturne - Easy</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei III Nocturne - Hard</t>
+  </si>
+  <si>
+    <t>Heaven</t>
+  </si>
+  <si>
+    <t>Persona 4 - Easy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u</t>
+  </si>
+  <si>
+    <t>Persona 4 - Hard</t>
+  </si>
+  <si>
+    <t>Final Fantasy IX - Easy</t>
+  </si>
+  <si>
+    <t>Melodies of Life</t>
+  </si>
+  <si>
+    <t>Emiko Shiratori</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-</t>
+  </si>
+  <si>
+    <t>Final Fantasy IX - Hard</t>
+  </si>
+  <si>
+    <t>Code Vein - Easy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k</t>
+  </si>
+  <si>
+    <t>Go Shiina</t>
+  </si>
+  <si>
+    <t>Code Vein - Hard</t>
+  </si>
+  <si>
     <t>Persona 3</t>
   </si>
   <si>
-    <t>Code Vein</t>
-  </si>
-  <si>
-    <t>Requiem</t>
-  </si>
-  <si>
-    <t>Ornstein &amp; Smough</t>
-  </si>
-  <si>
-    <t>Dark Souls</t>
-  </si>
-  <si>
-    <t>The Place I'll Return To Someday</t>
-  </si>
-  <si>
-    <t>Outer Wilds</t>
-  </si>
-  <si>
-    <t>14.3 Billion Years</t>
-  </si>
-  <si>
     <t>Mass Destruction</t>
   </si>
   <si>
-    <t>https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0</t>
-  </si>
-  <si>
-    <t>Shin Megami Tensei V</t>
-  </si>
-  <si>
-    <t>Spring (The Valley Comes Alive)</t>
-  </si>
-  <si>
-    <t>Stardew Valley</t>
-  </si>
-  <si>
-    <t>Subnautica</t>
-  </si>
-  <si>
-    <t>Abandon Ship</t>
-  </si>
-  <si>
-    <t>Theme Of Laura</t>
-  </si>
-  <si>
-    <t>Silent Hill 2</t>
-  </si>
-  <si>
-    <t>Prologue</t>
-  </si>
-  <si>
-    <t>Shadow Of The Colossus</t>
-  </si>
-  <si>
-    <t>Baba Yetu</t>
-  </si>
-  <si>
-    <t>Civilisation 4</t>
-  </si>
-  <si>
-    <t>Dragonborn (Theme)</t>
-  </si>
-  <si>
-    <t>The Elder Scrolls V: Skyrim</t>
-  </si>
-  <si>
-    <t>Dearly Beloved</t>
-  </si>
-  <si>
-    <t>Kingdom Hearts</t>
-  </si>
-  <si>
-    <t>Final Fantasy X</t>
-  </si>
-  <si>
-    <t>Final Fantasy IX</t>
-  </si>
-  <si>
-    <t>To Zanarkand</t>
-  </si>
-  <si>
-    <t>Final Fantasy VII</t>
-  </si>
-  <si>
-    <t>One Winged Angel</t>
-  </si>
-  <si>
-    <t>I Really Want To Stay At Your House</t>
-  </si>
-  <si>
-    <t>Cyberpunk 2077</t>
+    <t>Persona 3 - Easy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C</t>
+  </si>
+  <si>
+    <t>Persona 3 - Hard</t>
+  </si>
+  <si>
+    <t>Dark Souls - Easy</t>
+  </si>
+  <si>
+    <t>Motoi Sakuraba</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q</t>
+  </si>
+  <si>
+    <t>Dark Souls - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl</t>
+  </si>
+  <si>
+    <t>Ryota Kozuka</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei V - Easy</t>
+  </si>
+  <si>
+    <t>Battle - Destruction</t>
+  </si>
+  <si>
+    <t>Shin Megami Tensei V - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf</t>
+  </si>
+  <si>
+    <t>Eric Barone</t>
+  </si>
+  <si>
+    <t>Stardew Valley - Easy</t>
+  </si>
+  <si>
+    <t>Stardew Valley - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx</t>
+  </si>
+  <si>
+    <t>Subnautica - Easy</t>
+  </si>
+  <si>
+    <t>Simon Chylinski</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E</t>
+  </si>
+  <si>
+    <t>Akira Yamaoka</t>
+  </si>
+  <si>
+    <t>Silent Hill 2 - Easy</t>
+  </si>
+  <si>
+    <t>Silent Hill 2 - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3</t>
+  </si>
+  <si>
+    <t>Shadow Of The Colossus - Easy</t>
+  </si>
+  <si>
+    <t>Kō Ōtani</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx</t>
+  </si>
+  <si>
+    <t>Christopher Tin</t>
+  </si>
+  <si>
+    <t>Civilisation IV</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J</t>
+  </si>
+  <si>
+    <t>Yoko Shimomura</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts - Easy</t>
+  </si>
+  <si>
+    <t>Kingdom Hearts - Hard</t>
+  </si>
+  <si>
+    <t>Nobuo Uematsu</t>
+  </si>
+  <si>
+    <t>Final Fantasy X - Easy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f</t>
+  </si>
+  <si>
+    <t>Final Fantasy X - Hard</t>
+  </si>
+  <si>
+    <t>Jeremy Soule</t>
+  </si>
+  <si>
+    <t>The Elder Scrolls V Skyrim</t>
+  </si>
+  <si>
+    <t>The Elder Scrolls V Skyrim - Easy</t>
+  </si>
+  <si>
+    <t>Dragonborn</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv</t>
+  </si>
+  <si>
+    <t>Final Fantasy VII - Easy</t>
+  </si>
+  <si>
+    <t>Final Fantasy VII - Hard</t>
+  </si>
+  <si>
+    <t>Breaking Bad - Easy</t>
+  </si>
+  <si>
+    <t>Breaking Bad</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2</t>
+  </si>
+  <si>
+    <t>Civilisation IV - Easy</t>
+  </si>
+  <si>
+    <t>Civilisation IV - Hard</t>
   </si>
 </sst>
 </file>
@@ -1244,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView topLeftCell="H33" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,11 +1849,11 @@
         <v>music/anime/Death Note OP1 - Easy</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>355</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Easy', 'ttps://www.youtube.com/embed/kNyR46eHDxE?si=JJH9imobI4X7YBKI');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Easy', 'https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2');</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1655,11 +1880,11 @@
         <v>music/anime/Death Note OP1 - Hard</v>
       </c>
       <c r="H13" t="s">
-        <v>117</v>
+        <v>355</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Hard', 'ttps://www.youtube.com/embed/kNyR46eHDxE?si=JJH9imobI4X7YBKI');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Hard', 'https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2');</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1686,7 +1911,7 @@
         <v>music/anime/Death Parade OP1 - Easy</v>
       </c>
       <c r="H14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1717,7 +1942,7 @@
         <v>music/anime/Death Parade OP1 - Hard</v>
       </c>
       <c r="H15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1748,7 +1973,7 @@
         <v>music/anime/Dragon Ball Z OP1 - Easy</v>
       </c>
       <c r="H16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1779,7 +2004,7 @@
         <v>music/anime/Dragon Ball Z OP1 - Hard</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1810,7 +2035,7 @@
         <v>music/anime/Ergo Proxy OP1 - Easy</v>
       </c>
       <c r="H18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1841,7 +2066,7 @@
         <v>music/anime/Ergo Proxy OP1 - Hard</v>
       </c>
       <c r="H19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1872,7 +2097,7 @@
         <v>music/anime/Evangelion OP1 - Easy</v>
       </c>
       <c r="H20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1903,7 +2128,7 @@
         <v>music/anime/Evangelion OP1 - Hard</v>
       </c>
       <c r="H21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1934,7 +2159,7 @@
         <v>music/anime/Fate Stay Night UBW OP2 - Easy</v>
       </c>
       <c r="H22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1965,7 +2190,7 @@
         <v>music/anime/Fate Stay Night UBW OP2 - Hard</v>
       </c>
       <c r="H23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="1"/>
@@ -1996,7 +2221,7 @@
         <v>music/anime/Guilty Crown OP1 - Easy</v>
       </c>
       <c r="H24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2027,7 +2252,7 @@
         <v>music/anime/Guilty Crown OP1 - Hard</v>
       </c>
       <c r="H25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2058,7 +2283,7 @@
         <v>music/anime/Jojo OP2 - Easy</v>
       </c>
       <c r="H26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2089,7 +2314,7 @@
         <v>music/anime/Jojo OP2 - Hard</v>
       </c>
       <c r="H27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2120,7 +2345,7 @@
         <v>music/anime/Jujutsu Kaisen OP2 - Easy</v>
       </c>
       <c r="H28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2151,7 +2376,7 @@
         <v>music/anime/Jujutsu Kaisen OP2 - Hard</v>
       </c>
       <c r="H29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2182,7 +2407,7 @@
         <v>music/anime/One Punch Man OP1 - Easy</v>
       </c>
       <c r="H30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2213,7 +2438,7 @@
         <v>music/anime/One Punch Man OP1 - Hard</v>
       </c>
       <c r="H31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2244,7 +2469,7 @@
         <v>music/anime/Psycho Pass OP2 - Easy</v>
       </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2275,7 +2500,7 @@
         <v>music/anime/Psycho Pass OP2 - Hard</v>
       </c>
       <c r="H33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2306,7 +2531,7 @@
         <v>music/anime/Ranking of Kings OP2 - Easy</v>
       </c>
       <c r="H34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2337,7 +2562,7 @@
         <v>music/anime/Ranking of Kings OP2 - Hard</v>
       </c>
       <c r="H35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2368,7 +2593,7 @@
         <v>music/anime/Soul Eater OP2 - Easy</v>
       </c>
       <c r="H36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I36" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2399,7 +2624,7 @@
         <v>music/anime/Soul Eater OP2 - Hard</v>
       </c>
       <c r="H37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2430,7 +2655,7 @@
         <v>music/anime/Tokyo Ghoul OP1 - Easy</v>
       </c>
       <c r="H38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2461,7 +2686,7 @@
         <v>music/anime/Tokyo Ghoul OP1 - Hard</v>
       </c>
       <c r="H39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2492,7 +2717,7 @@
         <v>music/anime/Vinland Saga OP1 - Easy</v>
       </c>
       <c r="H40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2523,7 +2748,7 @@
         <v>music/anime/Vinland Saga OP1 - Hard</v>
       </c>
       <c r="H41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -2539,8 +2764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7033B7E-9E28-44F0-AF22-AF8799EBF584}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="H35" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,1023 +2810,1023 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" t="s">
         <v>132</v>
       </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G43" si="0">"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
+        <v>music/indie/Bombay Bicycle Club - Easy</v>
+      </c>
+      <c r="H2" t="s">
+        <v>162</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f t="shared" ref="I2:I43" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bombay Bicycle Club - Easy', 'Bombay Bicycle Club', 'Easy', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music/indie/Bombay Bicycle Club - Easy', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" t="s">
         <v>132</v>
       </c>
-      <c r="F2" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" t="str">
-        <f>"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
-        <v>music/indie/The Mountain Goats - Easy</v>
-      </c>
-      <c r="H2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Mountain Goats - Easy', 'The Mountain Goats', 'Easy', 'Autoclave', 'The Mountain Goats', 'Indie', 'music/indie/The Mountain Goats - Easy', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>music/indie/Bombay Bicycle Club - Hard</v>
+      </c>
+      <c r="H3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bombay Bicycle Club - Hard', 'Bombay Bicycle Club', 'Hard', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music/indie/Bombay Bicycle Club - Hard', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1996</v>
+      </c>
+      <c r="E4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" t="s">
         <v>132</v>
       </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>music/indie/Brand New - Easy</v>
+      </c>
+      <c r="H4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Brand New - Easy', 'Brand New', 'Easy', '1996', 'Brand New', 'Indie', 'music/indie/Brand New - Easy', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1996</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F5" t="s">
         <v>132</v>
       </c>
-      <c r="F3" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" t="str">
-        <f>"music/"&amp;LOWER(F3)&amp;"/"&amp;A3</f>
-        <v>music/indie/The Mountain Goats - Hard</v>
-      </c>
-      <c r="H3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Mountain Goats - Hard', 'The Mountain Goats', 'Hard', 'Autoclave', 'The Mountain Goats', 'Indie', 'music/indie/The Mountain Goats - Hard', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G4" t="str">
-        <f t="shared" ref="G4:G41" si="0">"music/"&amp;LOWER(F4)&amp;"/"&amp;A4</f>
-        <v>music/indie/Frightened Rabbit - Easy</v>
-      </c>
-      <c r="H4" t="s">
-        <v>136</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f t="shared" ref="I4:I41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A4&amp;"'"&amp;", "&amp;"'"&amp;B4&amp;"'"&amp;", "&amp;"'"&amp;C4&amp;"'"&amp;", "&amp;"'"&amp;D4&amp;"'"&amp;", "&amp;"'"&amp;E4&amp;"'"&amp;", "&amp;"'"&amp;F4&amp;"'"&amp;", "&amp;"'"&amp;G4&amp;"', "&amp;"'"&amp;H4&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Frightened Rabbit - Easy', 'Frightened Rabbit', 'Easy', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music/indie/Frightened Rabbit - Easy', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" t="s">
-        <v>133</v>
-      </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Frightened Rabbit - Hard</v>
+        <v>music/indie/Brand New - Hard</v>
       </c>
       <c r="H5" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Frightened Rabbit - Hard', 'Frightened Rabbit', 'Hard', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music/indie/Frightened Rabbit - Hard', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Brand New - Hard', 'Brand New', 'Hard', '1996', 'Brand New', 'Indie', 'music/indie/Brand New - Hard', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>139</v>
+      <c r="D6" t="s">
+        <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Neutral Milk Hotel - Easy</v>
+        <v>music/indie/Bright Eyes - Easy</v>
       </c>
       <c r="H6" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Neutral Milk Hotel - Easy', 'Neutral Milk Hotel', 'Easy', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music/indie/Neutral Milk Hotel - Easy', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bright Eyes - Easy', 'Bright Eyes', 'Easy', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music/indie/Bright Eyes - Easy', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>139</v>
+      <c r="D7" t="s">
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Neutral Milk Hotel - Hard</v>
+        <v>music/indie/Bright Eyes - Hard</v>
       </c>
       <c r="H7" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Neutral Milk Hotel - Hard', 'Neutral Milk Hotel', 'Hard', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music/indie/Neutral Milk Hotel - Hard', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bright Eyes - Hard', 'Bright Eyes', 'Hard', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music/indie/Bright Eyes - Hard', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>224</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="E8" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Thermals - Easy</v>
+        <v>music/indie/Editors - Easy</v>
       </c>
       <c r="H8" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="I8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Thermals - Easy', 'The Thermals', 'Easy', 'Born to Kill', 'The Thermals', 'Indie', 'music/indie/The Thermals - Easy', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Editors - Easy', 'Editors', 'Easy', 'An End Has A Start', 'Editors', 'Indie', 'music/indie/Editors - Easy', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="F9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Thermals - Hard</v>
+        <v>music/indie/Editors - Hard</v>
       </c>
       <c r="H9" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Thermals - Hard', 'The Thermals', 'Hard', 'Born to Kill', 'The Thermals', 'Indie', 'music/indie/The Thermals - Hard', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Editors - Hard', 'Editors', 'Hard', 'An End Has A Start', 'Editors', 'Indie', 'music/indie/Editors - Hard', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C10" t="s">
         <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Mewithoutyou - Easy</v>
+        <v>music/indie/Frightened Rabbit - Easy</v>
       </c>
       <c r="H10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Mewithoutyou - Easy', 'Mewithoutyou', 'Easy', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music/indie/Mewithoutyou - Easy', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Frightened Rabbit - Easy', 'Frightened Rabbit', 'Easy', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music/indie/Frightened Rabbit - Easy', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E11" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Mewithoutyou - Hard</v>
+        <v>music/indie/Frightened Rabbit - Hard</v>
       </c>
       <c r="H11" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Mewithoutyou - Hard', 'Mewithoutyou', 'Hard', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music/indie/Mewithoutyou - Hard', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Frightened Rabbit - Hard', 'Frightened Rabbit', 'Hard', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music/indie/Frightened Rabbit - Hard', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="C12" t="s">
         <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Bright Eyes - Easy</v>
+        <v>music/indie/Funeral Suits - Easy</v>
       </c>
       <c r="H12" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bright Eyes - Easy', 'Bright Eyes', 'Easy', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music/indie/Bright Eyes - Easy', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Funeral Suits - Easy', 'Funeral Suits', 'Easy', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music/indie/Funeral Suits - Easy', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Bright Eyes - Hard</v>
+        <v>music/indie/Funeral Suits - Hard</v>
       </c>
       <c r="H13" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bright Eyes - Hard', 'Bright Eyes', 'Hard', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music/indie/Bright Eyes - Hard', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Funeral Suits - Hard', 'Funeral Suits', 'Hard', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music/indie/Funeral Suits - Hard', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="C14" t="s">
         <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Front Bottoms - Easy</v>
+        <v>music/indie/Half-Alive - Easy</v>
       </c>
       <c r="H14" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Front Bottoms - Easy', 'The Front Bottoms', 'Easy', 'Ginger', 'The Front Bottoms', 'Indie', 'music/indie/The Front Bottoms - Easy', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Half-Alive - Easy', 'Half-Alive', 'Easy', 'Still Feel', 'Half-Alive', 'Indie', 'music/indie/Half-Alive - Easy', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Front Bottoms - Hard</v>
+        <v>music/indie/Half-Alive - Hard</v>
       </c>
       <c r="H15" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Front Bottoms - Hard', 'The Front Bottoms', 'Hard', 'Ginger', 'The Front Bottoms', 'Indie', 'music/indie/The Front Bottoms - Hard', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Half-Alive - Hard', 'Half-Alive', 'Hard', 'Still Feel', 'Half-Alive', 'Indie', 'music/indie/Half-Alive - Hard', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="C16" t="s">
         <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="E16" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Modern Baseball - Easy</v>
+        <v>music/indie/I Don''t Know How But They Found Me - Easy</v>
       </c>
       <c r="H16" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Modern Baseball - Easy', 'Modern Baseball', 'Easy', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music/indie/Modern Baseball - Easy', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Easy', 'I Don''t Know How But They Found Me', 'Easy', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music/indie/I Don''t Know How But They Found Me - Easy', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="F17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Modern Baseball - Hard</v>
+        <v>music/indie/I Don''t Know How But They Found Me - Hard</v>
       </c>
       <c r="H17" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Modern Baseball - Hard', 'Modern Baseball', 'Hard', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music/indie/Modern Baseball - Hard', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Hard', 'I Don''t Know How But They Found Me', 'Hard', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music/indie/I Don''t Know How But They Found Me - Hard', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E18" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/KennyHoopla - Easy</v>
+        <v>music/indie/Interpol - Easy</v>
       </c>
       <c r="H18" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('KennyHoopla - Easy', 'KennyHoopla', 'Easy', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music/indie/KennyHoopla - Easy', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Interpol - Easy', 'Interpol', 'Easy', 'Evil', 'Interpol', 'Indie', 'music/indie/Interpol - Easy', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="F19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/KennyHoopla - Hard</v>
+        <v>music/indie/Interpol - Hard</v>
       </c>
       <c r="H19" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('KennyHoopla - Hard', 'KennyHoopla', 'Hard', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music/indie/KennyHoopla - Hard', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Interpol - Hard', 'Interpol', 'Hard', 'Evil', 'Interpol', 'Indie', 'music/indie/Interpol - Hard', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="C20" t="s">
         <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
+        <v>234</v>
       </c>
       <c r="E20" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="F20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Pat The Bunny - Easy</v>
+        <v>music/indie/Iron And Wine - Easy</v>
       </c>
       <c r="H20" t="s">
-        <v>160</v>
+        <v>235</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Pat The Bunny - Easy', 'Pat The Bunny', 'Easy', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music/indie/Pat The Bunny - Easy', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Iron And Wine - Easy', 'Iron And Wine', 'Easy', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music/indie/Iron And Wine - Easy', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>234</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="F21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Pat The Bunny - Hard</v>
+        <v>music/indie/Iron And Wine - Hard</v>
       </c>
       <c r="H21" t="s">
-        <v>160</v>
+        <v>235</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Pat The Bunny - Hard', 'Pat The Bunny', 'Hard', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music/indie/Pat The Bunny - Hard', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Iron And Wine - Hard', 'Iron And Wine', 'Hard', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music/indie/Iron And Wine - Hard', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C22" t="s">
         <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="E22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Bombay Bicycle Club - Easy</v>
+        <v>music/indie/KennyHoopla - Easy</v>
       </c>
       <c r="H22" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bombay Bicycle Club - Easy', 'Bombay Bicycle Club', 'Easy', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music/indie/Bombay Bicycle Club - Easy', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('KennyHoopla - Easy', 'KennyHoopla', 'Easy', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music/indie/KennyHoopla - Easy', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Bombay Bicycle Club - Hard</v>
+        <v>music/indie/KennyHoopla - Hard</v>
       </c>
       <c r="H23" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bombay Bicycle Club - Hard', 'Bombay Bicycle Club', 'Hard', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music/indie/Bombay Bicycle Club - Hard', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('KennyHoopla - Hard', 'KennyHoopla', 'Hard', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music/indie/KennyHoopla - Hard', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="C24" t="s">
         <v>67</v>
       </c>
       <c r="D24" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="E24" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="F24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/I Don''t Know How But They Found Me - Easy</v>
+        <v>music/indie/Mewithoutyou - Easy</v>
       </c>
       <c r="H24" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Easy', 'I Don''t Know How But They Found Me', 'Easy', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music/indie/I Don''t Know How But They Found Me - Easy', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Mewithoutyou - Easy', 'Mewithoutyou', 'Easy', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music/indie/Mewithoutyou - Easy', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="C25" t="s">
         <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
       <c r="E25" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/I Don''t Know How But They Found Me - Hard</v>
+        <v>music/indie/Mewithoutyou - Hard</v>
       </c>
       <c r="H25" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Hard', 'I Don''t Know How But They Found Me', 'Hard', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music/indie/I Don''t Know How But They Found Me - Hard', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Mewithoutyou - Hard', 'Mewithoutyou', 'Hard', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music/indie/Mewithoutyou - Hard', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C26" t="s">
         <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E26" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Shins - Easy</v>
+        <v>music/indie/Modern Baseball - Easy</v>
       </c>
       <c r="H26" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Shins - Easy', 'The Shins', 'Easy', 'Simple Song', 'The Shins', 'Indie', 'music/indie/The Shins - Easy', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Modern Baseball - Easy', 'Modern Baseball', 'Easy', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music/indie/Modern Baseball - Easy', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E27" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="F27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Shins - Hard</v>
+        <v>music/indie/Modern Baseball - Hard</v>
       </c>
       <c r="H27" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Shins - Hard', 'The Shins', 'Hard', 'Simple Song', 'The Shins', 'Indie', 'music/indie/The Shins - Hard', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Modern Baseball - Hard', 'Modern Baseball', 'Hard', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music/indie/Modern Baseball - Hard', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
       </c>
-      <c r="D28" t="s">
-        <v>169</v>
+      <c r="D28" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="E28" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="F28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Perma - Easy</v>
+        <v>music/indie/Neutral Milk Hotel - Easy</v>
       </c>
       <c r="H28" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Perma - Easy', 'Perma', 'Easy', 'Little Light', 'Perma', 'Indie', 'music/indie/Perma - Easy', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Neutral Milk Hotel - Easy', 'Neutral Milk Hotel', 'Easy', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music/indie/Neutral Milk Hotel - Easy', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="C29" t="s">
         <v>68</v>
       </c>
-      <c r="D29" t="s">
-        <v>169</v>
+      <c r="D29" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="E29" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Perma - Hard</v>
+        <v>music/indie/Neutral Milk Hotel - Hard</v>
       </c>
       <c r="H29" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Perma - Hard', 'Perma', 'Hard', 'Little Light', 'Perma', 'Indie', 'music/indie/Perma - Hard', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Neutral Milk Hotel - Hard', 'Neutral Milk Hotel', 'Hard', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music/indie/Neutral Milk Hotel - Hard', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B30" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
         <v>67</v>
       </c>
       <c r="D30" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="E30" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Interpol - Easy</v>
+        <v>music/indie/Pat The Bunny - Easy</v>
       </c>
       <c r="H30" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Interpol - Easy', 'Interpol', 'Easy', 'Evil', 'Interpol', 'Indie', 'music/indie/Interpol - Easy', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Pat The Bunny - Easy', 'Pat The Bunny', 'Easy', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music/indie/Pat The Bunny - Easy', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="C31" t="s">
         <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="E31" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="F31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Interpol - Hard</v>
+        <v>music/indie/Pat The Bunny - Hard</v>
       </c>
       <c r="H31" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Interpol - Hard', 'Interpol', 'Hard', 'Evil', 'Interpol', 'Indie', 'music/indie/Interpol - Hard', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Pat The Bunny - Hard', 'Pat The Bunny', 'Hard', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music/indie/Pat The Bunny - Hard', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B32" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C32" t="s">
         <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Half-Alive - Easy</v>
+        <v>music/indie/Perma - Easy</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Half-Alive - Easy', 'Half-Alive', 'Easy', 'Still Feel', 'Half-Alive', 'Indie', 'music/indie/Half-Alive - Easy', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Perma - Easy', 'Perma', 'Easy', 'Little Light', 'Perma', 'Indie', 'music/indie/Perma - Easy', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C33" t="s">
         <v>68</v>
       </c>
       <c r="D33" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Half-Alive - Hard</v>
+        <v>music/indie/Perma - Hard</v>
       </c>
       <c r="H33" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Half-Alive - Hard', 'Half-Alive', 'Hard', 'Still Feel', 'Half-Alive', 'Indie', 'music/indie/Half-Alive - Hard', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Perma - Hard', 'Perma', 'Hard', 'Little Light', 'Perma', 'Indie', 'music/indie/Perma - Hard', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B34" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
         <v>178</v>
       </c>
-      <c r="C34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>177</v>
+      </c>
+      <c r="F34" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>music/indie/Sorority Noise - Easy</v>
+      </c>
+      <c r="H34" t="s">
         <v>179</v>
-      </c>
-      <c r="E34" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" t="s">
-        <v>133</v>
-      </c>
-      <c r="G34" t="str">
-        <f t="shared" si="0"/>
-        <v>music/indie/Sorority Noise - Easy</v>
-      </c>
-      <c r="H34" t="s">
-        <v>180</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3610,29 +3835,29 @@
     </row>
     <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B35" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
         <v>178</v>
       </c>
-      <c r="C35" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" t="s">
+        <v>132</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>music/indie/Sorority Noise - Hard</v>
+      </c>
+      <c r="H35" t="s">
         <v>179</v>
-      </c>
-      <c r="E35" t="s">
-        <v>178</v>
-      </c>
-      <c r="F35" t="s">
-        <v>133</v>
-      </c>
-      <c r="G35" t="str">
-        <f t="shared" si="0"/>
-        <v>music/indie/Sorority Noise - Hard</v>
-      </c>
-      <c r="H35" t="s">
-        <v>180</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3641,253 +3866,256 @@
     </row>
     <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="B36" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="C36" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="3">
-        <v>1996</v>
+      <c r="D36" t="s">
+        <v>150</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="F36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Brand New - Easy</v>
+        <v>music/indie/The Front Bottoms - Easy</v>
       </c>
       <c r="H36" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="I36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Brand New - Easy', 'Brand New', 'Easy', '1996', 'Brand New', 'Indie', 'music/indie/Brand New - Easy', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Front Bottoms - Easy', 'The Front Bottoms', 'Easy', 'Ginger', 'The Front Bottoms', 'Indie', 'music/indie/The Front Bottoms - Easy', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="3">
-        <v>1996</v>
+      <c r="D37" t="s">
+        <v>150</v>
       </c>
       <c r="E37" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
       <c r="F37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Brand New - Hard</v>
+        <v>music/indie/The Front Bottoms - Hard</v>
       </c>
       <c r="H37" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="I37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Brand New - Hard', 'Brand New', 'Hard', '1996', 'Brand New', 'Indie', 'music/indie/Brand New - Hard', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Front Bottoms - Hard', 'The Front Bottoms', 'Hard', 'Ginger', 'The Front Bottoms', 'Indie', 'music/indie/The Front Bottoms - Hard', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="B38" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="C38" t="s">
         <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="E38" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="F38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Editors - Easy</v>
+        <v>music/indie/The Mountain Goats - Easy</v>
       </c>
       <c r="H38" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Editors - Easy', 'Editors', 'Easy', 'An End Has A Start', 'Editors', 'Indie', 'music/indie/Editors - Easy', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Mountain Goats - Easy', 'The Mountain Goats', 'Easy', 'Autoclave', 'The Mountain Goats', 'Indie', 'music/indie/The Mountain Goats - Easy', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="C39" t="s">
         <v>68</v>
       </c>
       <c r="D39" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="E39" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Editors - Hard</v>
+        <v>music/indie/The Mountain Goats - Hard</v>
       </c>
       <c r="H39" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Editors - Hard', 'Editors', 'Hard', 'An End Has A Start', 'Editors', 'Indie', 'music/indie/Editors - Hard', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Mountain Goats - Hard', 'The Mountain Goats', 'Hard', 'Autoclave', 'The Mountain Goats', 'Indie', 'music/indie/The Mountain Goats - Hard', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="B40" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="C40" t="s">
         <v>67</v>
       </c>
       <c r="D40" t="s">
-        <v>231</v>
+        <v>167</v>
       </c>
       <c r="E40" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="F40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Funeral Suits - Easy</v>
+        <v>music/indie/The Shins - Easy</v>
       </c>
       <c r="H40" t="s">
-        <v>227</v>
+        <v>165</v>
       </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Funeral Suits - Easy', 'Funeral Suits', 'Easy', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music/indie/Funeral Suits - Easy', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Shins - Easy', 'The Shins', 'Easy', 'Simple Song', 'The Shins', 'Indie', 'music/indie/The Shins - Easy', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
         <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>231</v>
+        <v>167</v>
       </c>
       <c r="E41" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="F41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Funeral Suits - Hard</v>
+        <v>music/indie/The Shins - Hard</v>
       </c>
       <c r="H41" t="s">
-        <v>227</v>
+        <v>165</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Funeral Suits - Hard', 'Funeral Suits', 'Hard', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music/indie/Funeral Suits - Hard', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Shins - Hard', 'The Shins', 'Hard', 'Simple Song', 'The Shins', 'Indie', 'music/indie/The Shins - Hard', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="B42" t="s">
-        <v>234</v>
+        <v>141</v>
       </c>
       <c r="C42" t="s">
         <v>67</v>
       </c>
       <c r="D42" t="s">
-        <v>235</v>
+        <v>142</v>
       </c>
       <c r="E42" t="s">
-        <v>234</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" ref="G42:G43" si="2">"music/"&amp;LOWER(F42)&amp;"/"&amp;A42</f>
-        <v>music/indie/Iron And Wine - Easy</v>
+        <f t="shared" si="0"/>
+        <v>music/indie/The Thermals - Easy</v>
       </c>
       <c r="H42" t="s">
-        <v>236</v>
+        <v>143</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f t="shared" ref="I42:I43" si="3">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A42&amp;"'"&amp;", "&amp;"'"&amp;B42&amp;"'"&amp;", "&amp;"'"&amp;C42&amp;"'"&amp;", "&amp;"'"&amp;D42&amp;"'"&amp;", "&amp;"'"&amp;E42&amp;"'"&amp;", "&amp;"'"&amp;F42&amp;"'"&amp;", "&amp;"'"&amp;G42&amp;"', "&amp;"'"&amp;H42&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Iron And Wine - Easy', 'Iron And Wine', 'Easy', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music/indie/Iron And Wine - Easy', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Thermals - Easy', 'The Thermals', 'Easy', 'Born to Kill', 'The Thermals', 'Indie', 'music/indie/The Thermals - Easy', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="B43" t="s">
-        <v>234</v>
+        <v>141</v>
       </c>
       <c r="C43" t="s">
         <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>235</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>234</v>
+        <v>141</v>
       </c>
       <c r="F43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="2"/>
-        <v>music/indie/Iron And Wine - Hard</v>
+        <f t="shared" si="0"/>
+        <v>music/indie/The Thermals - Hard</v>
       </c>
       <c r="H43" t="s">
-        <v>236</v>
+        <v>143</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Iron And Wine - Hard', 'Iron And Wine', 'Hard', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music/indie/Iron And Wine - Hard', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Thermals - Hard', 'The Thermals', 'Hard', 'Born to Kill', 'The Thermals', 'Indie', 'music/indie/The Thermals - Hard', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I43">
+    <sortCondition ref="A1:A43"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3896,23 +4124,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F96BC2-62DB-49FB-AD78-FA2CCE8FE0BD}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="107.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="108" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3946,237 +4174,1397 @@
     </row>
     <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>336</v>
       </c>
       <c r="C2" t="s">
         <v>67</v>
       </c>
       <c r="D2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F2" t="s">
         <v>240</v>
       </c>
-      <c r="E2" t="s">
-        <v>243</v>
-      </c>
-      <c r="F2" t="s">
-        <v>241</v>
-      </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G3" si="0">"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
-        <v>music/video games/Persona 5 - Easy</v>
+        <f t="shared" ref="G2:G43" si="0">"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
+        <v>music/video games/Civilisation IV - Easy</v>
       </c>
       <c r="H2" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" ref="I2:I3" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Easy', 'Persona 5', 'Easy', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Easy', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+        <f t="shared" ref="I2:I43" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Civilisation IV - Easy', 'Civilisation IV', 'Easy', 'Baba Yetu', 'Christopher Tin', 'Video Games', 'music/video games/Civilisation IV - Easy', 'https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx');</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>336</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
       </c>
       <c r="D3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F3" t="s">
         <v>240</v>
       </c>
-      <c r="E3" t="s">
-        <v>243</v>
-      </c>
-      <c r="F3" t="s">
-        <v>241</v>
-      </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 5 - Hard</v>
+        <v>music/video games/Civilisation IV - Hard</v>
       </c>
       <c r="H3" t="s">
-        <v>242</v>
+        <v>334</v>
       </c>
       <c r="I3" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Hard', 'Persona 5', 'Hard', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Hard', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Civilisation IV - Hard', 'Civilisation IV', 'Hard', 'Baba Yetu', 'Christopher Tin', 'Video Games', 'music/video games/Civilisation IV - Hard', 'https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>302</v>
+      </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>247</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="E4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Code Vein - Easy</v>
+      </c>
+      <c r="H4" t="s">
+        <v>303</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Vein - Easy', 'Code Vein', 'Easy', 'Requiem', 'Go Shiina', 'Video Games', 'music/video games/Code Vein - Easy', 'https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>305</v>
+      </c>
       <c r="B5" t="s">
         <v>247</v>
       </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
       <c r="D5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E5" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Code Vein - Hard</v>
+      </c>
+      <c r="H5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Vein - Hard', 'Code Vein', 'Hard', 'Requiem', 'Go Shiina', 'Video Games', 'music/video games/Code Vein - Hard', 'https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" t="s">
+        <v>278</v>
+      </c>
+      <c r="F6" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Cyberpunk 2077 - Easy</v>
+      </c>
+      <c r="H6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Cyberpunk 2077 - Easy', 'Cyberpunk 2077', 'Easy', 'I Really Want To Stay At Your House', 'Rosa Walton &amp; Hallie Coggins', 'Video Games', 'music/video games/Cyberpunk 2077 - Easy', 'https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E7" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" t="s">
+        <v>240</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Cyberpunk 2077 - Easy</v>
+      </c>
+      <c r="H7" t="s">
+        <v>277</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Cyberpunk 2077 - Easy', 'Cyberpunk 2077', 'Hard', 'I Really Want To Stay At Your House', 'Rosa Walton &amp; Hallie Coggins', 'Video Games', 'music/video games/Cyberpunk 2077 - Easy', 'https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8" t="s">
+        <v>240</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Dark Souls - Easy</v>
+      </c>
+      <c r="H8" t="s">
+        <v>313</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dark Souls - Easy', 'Dark Souls', 'Easy', 'Ornstein &amp; Smough', 'Motoi Sakuraba', 'Video Games', 'music/video games/Dark Souls - Easy', 'https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E9" t="s">
+        <v>312</v>
+      </c>
+      <c r="F9" t="s">
+        <v>240</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Dark Souls - Hard</v>
+      </c>
+      <c r="H9" t="s">
+        <v>313</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dark Souls - Hard', 'Dark Souls', 'Hard', 'Ornstein &amp; Smough', 'Motoi Sakuraba', 'Video Games', 'music/video games/Dark Souls - Hard', 'https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>298</v>
+      </c>
+      <c r="E10" t="s">
+        <v>299</v>
+      </c>
+      <c r="F10" t="s">
+        <v>240</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Final Fantasy IX - Easy</v>
+      </c>
+      <c r="H10" t="s">
+        <v>300</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy IX - Easy', 'Final Fantasy IX', 'Easy', 'Melodies of Life', 'Emiko Shiratori', 'Video Games', 'music/video games/Final Fantasy IX - Easy', 'https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>301</v>
+      </c>
+      <c r="B11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" t="s">
+        <v>298</v>
+      </c>
+      <c r="E11" t="s">
+        <v>299</v>
+      </c>
+      <c r="F11" t="s">
+        <v>240</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Final Fantasy IX - Hard</v>
+      </c>
+      <c r="H11" t="s">
+        <v>300</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy IX - Hard', 'Final Fantasy IX', 'Hard', 'Melodies of Life', 'Emiko Shiratori', 'Video Games', 'music/video games/Final Fantasy IX - Hard', 'https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>351</v>
+      </c>
+      <c r="B12" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>270</v>
+      </c>
+      <c r="E12" t="s">
+        <v>341</v>
+      </c>
+      <c r="F12" t="s">
+        <v>240</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Final Fantasy VII - Easy</v>
+      </c>
+      <c r="H12" t="s">
+        <v>350</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy VII - Easy', 'Final Fantasy VII', 'Easy', 'One Winged Angel', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy VII - Easy', 'https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>270</v>
+      </c>
+      <c r="E13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F13" t="s">
+        <v>240</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Final Fantasy VII - Hard</v>
+      </c>
+      <c r="H13" t="s">
+        <v>350</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy VII - Hard', 'Final Fantasy VII', 'Hard', 'One Winged Angel', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy VII - Hard', 'https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B14" t="s">
+        <v>266</v>
+      </c>
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" t="s">
+        <v>341</v>
+      </c>
+      <c r="F14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Final Fantasy X - Easy</v>
+      </c>
+      <c r="H14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy X - Easy', 'Final Fantasy X', 'Easy', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy X - Easy', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>268</v>
+      </c>
+      <c r="E15" t="s">
+        <v>341</v>
+      </c>
+      <c r="F15" t="s">
+        <v>240</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Final Fantasy X - Hard</v>
+      </c>
+      <c r="H15" t="s">
+        <v>343</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy X - Hard', 'Final Fantasy X', 'Hard', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy X - Hard', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>284</v>
+      </c>
+      <c r="B16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>287</v>
+      </c>
+      <c r="F16" t="s">
+        <v>240</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Fire Emblem Three Houses - Easy</v>
+      </c>
+      <c r="H16" t="s">
+        <v>286</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Easy', 'Fire Emblem Three Houses', 'Easy', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music/video games/Fire Emblem Three Houses - Easy', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B17" t="s">
+        <v>283</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E17" t="s">
+        <v>287</v>
+      </c>
+      <c r="F17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Fire Emblem Three Houses - Hard</v>
+      </c>
+      <c r="H17" t="s">
+        <v>286</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Hard', 'Fire Emblem Three Houses', 'Hard', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music/video games/Fire Emblem Three Houses - Hard', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>339</v>
+      </c>
+      <c r="B18" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>264</v>
+      </c>
+      <c r="E18" t="s">
+        <v>338</v>
+      </c>
+      <c r="F18" t="s">
+        <v>240</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Kingdom Hearts - Easy</v>
+      </c>
+      <c r="H18" t="s">
+        <v>337</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Kingdom Hearts - Easy', 'Kingdom Hearts', 'Easy', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music/video games/Kingdom Hearts - Easy', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>340</v>
+      </c>
+      <c r="B19" t="s">
+        <v>265</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>264</v>
+      </c>
+      <c r="E19" t="s">
+        <v>338</v>
+      </c>
+      <c r="F19" t="s">
+        <v>240</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Kingdom Hearts - Hard</v>
+      </c>
+      <c r="H19" t="s">
+        <v>337</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Kingdom Hearts - Hard', 'Kingdom Hearts', 'Hard', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music/video games/Kingdom Hearts - Hard', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" t="s">
+        <v>288</v>
+      </c>
+      <c r="F20" t="s">
+        <v>240</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Metal Gear Rising - Easy</v>
+      </c>
+      <c r="H20" t="s">
+        <v>282</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Metal Gear Rising - Easy', 'Metal Gear Rising', 'Easy', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music/video games/Metal Gear Rising - Easy', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>281</v>
+      </c>
+      <c r="B21" t="s">
+        <v>279</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" t="s">
+        <v>288</v>
+      </c>
+      <c r="F21" t="s">
+        <v>240</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Metal Gear Rising - Hard</v>
+      </c>
+      <c r="H21" t="s">
+        <v>282</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Metal Gear Rising - Hard', 'Metal Gear Rising', 'Hard', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music/video games/Metal Gear Rising - Hard', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>273</v>
+      </c>
+      <c r="B22" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>252</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F22" t="s">
+        <v>240</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Outer Wilds - Easy</v>
+      </c>
+      <c r="H22" t="s">
+        <v>253</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Outer Wilds - Easy', 'Outer Wilds', 'Easy', '14.3 Billion Years', 'Andrew Prahlow', 'Video Games', 'music/video games/Outer Wilds - Easy', 'https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>252</v>
+      </c>
+      <c r="E23" t="s">
+        <v>276</v>
+      </c>
+      <c r="F23" t="s">
+        <v>240</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Outer Wilds - Hard</v>
+      </c>
+      <c r="H23" t="s">
+        <v>253</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Outer Wilds - Hard', 'Outer Wilds', 'Hard', '14.3 Billion Years', 'Andrew Prahlow', 'Video Games', 'music/video games/Outer Wilds - Hard', 'https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>308</v>
+      </c>
+      <c r="B24" t="s">
+        <v>306</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>307</v>
+      </c>
+      <c r="E24" t="s">
+        <v>242</v>
+      </c>
+      <c r="F24" t="s">
+        <v>240</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 3 - Easy</v>
+      </c>
+      <c r="H24" t="s">
+        <v>309</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 3 - Easy', 'Persona 3', 'Easy', 'Mass Destruction', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 3 - Easy', 'https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>310</v>
+      </c>
+      <c r="B25" t="s">
+        <v>306</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>307</v>
+      </c>
+      <c r="E25" t="s">
+        <v>242</v>
+      </c>
+      <c r="F25" t="s">
+        <v>240</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 3 - Hard</v>
+      </c>
+      <c r="H25" t="s">
+        <v>309</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 3 - Hard', 'Persona 3', 'Hard', 'Mass Destruction', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 3 - Hard', 'https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>294</v>
+      </c>
+      <c r="B26" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>249</v>
-      </c>
-      <c r="D6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>251</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>293</v>
+      </c>
+      <c r="E26" t="s">
+        <v>242</v>
+      </c>
+      <c r="F26" t="s">
+        <v>240</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 4 - Easy</v>
+      </c>
+      <c r="H26" t="s">
+        <v>295</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 4 - Easy', 'Persona 4', 'Easy', 'Heaven', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 4 - Easy', 'https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>296</v>
+      </c>
+      <c r="B27" t="s">
+        <v>246</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>293</v>
+      </c>
+      <c r="E27" t="s">
+        <v>242</v>
+      </c>
+      <c r="F27" t="s">
+        <v>240</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 4 - Hard</v>
+      </c>
+      <c r="H27" t="s">
+        <v>295</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 4 - Hard', 'Persona 4', 'Hard', 'Heaven', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 4 - Hard', 'https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" t="s">
+        <v>239</v>
+      </c>
+      <c r="E28" t="s">
+        <v>242</v>
+      </c>
+      <c r="F28" t="s">
+        <v>240</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 5 - Easy</v>
+      </c>
+      <c r="H28" t="s">
+        <v>241</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Easy', 'Persona 5', 'Easy', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Easy', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>239</v>
+      </c>
+      <c r="E29" t="s">
+        <v>242</v>
+      </c>
+      <c r="F29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Persona 5 - Hard</v>
+      </c>
+      <c r="H29" t="s">
+        <v>241</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Hard', 'Persona 5', 'Hard', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Hard', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>332</v>
+      </c>
+      <c r="B30" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" t="s">
+        <v>261</v>
+      </c>
+      <c r="E30" t="s">
+        <v>333</v>
+      </c>
+      <c r="F30" t="s">
+        <v>240</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Shadow Of The Colossus - Easy</v>
+      </c>
+      <c r="H30" t="s">
+        <v>331</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Easy', 'Prologue', 'Kō Ōtani', 'Video Games', 'music/video games/Shadow Of The Colossus - Easy', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>332</v>
+      </c>
+      <c r="B31" t="s">
+        <v>262</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" t="s">
+        <v>261</v>
+      </c>
+      <c r="E31" t="s">
+        <v>333</v>
+      </c>
+      <c r="F31" t="s">
+        <v>240</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Shadow Of The Colossus - Easy</v>
+      </c>
+      <c r="H31" t="s">
+        <v>331</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Hard', 'Prologue', 'Kō Ōtani', 'Video Games', 'music/video games/Shadow Of The Colossus - Easy', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" t="s">
+        <v>290</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" t="s">
+        <v>245</v>
+      </c>
+      <c r="E32" t="s">
+        <v>242</v>
+      </c>
+      <c r="F32" t="s">
+        <v>240</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Shin Megami Tensei III Nocturne - Easy</v>
+      </c>
+      <c r="H32" t="s">
+        <v>289</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Easy', 'Shin Megami Tensei III Nocturne', 'Easy', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music/video games/Shin Megami Tensei III Nocturne - Easy', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>292</v>
+      </c>
+      <c r="B33" t="s">
+        <v>290</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>245</v>
+      </c>
+      <c r="E33" t="s">
+        <v>242</v>
+      </c>
+      <c r="F33" t="s">
+        <v>240</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Shin Megami Tensei III Nocturne - Hard</v>
+      </c>
+      <c r="H33" t="s">
+        <v>289</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Hard', 'Shin Megami Tensei III Nocturne', 'Hard', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music/video games/Shin Megami Tensei III Nocturne - Hard', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>317</v>
+      </c>
+      <c r="B34" t="s">
+        <v>254</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>318</v>
+      </c>
+      <c r="E34" t="s">
+        <v>316</v>
+      </c>
+      <c r="F34" t="s">
+        <v>240</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Shin Megami Tensei V - Easy</v>
+      </c>
+      <c r="H34" t="s">
+        <v>315</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei V - Easy', 'Shin Megami Tensei V', 'Easy', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music/video games/Shin Megami Tensei V - Easy', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>319</v>
+      </c>
+      <c r="B35" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>318</v>
+      </c>
+      <c r="E35" t="s">
+        <v>316</v>
+      </c>
+      <c r="F35" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Shin Megami Tensei V - Hard</v>
+      </c>
+      <c r="H35" t="s">
+        <v>315</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei V - Hard', 'Shin Megami Tensei V', 'Hard', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music/video games/Shin Megami Tensei V - Hard', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>329</v>
+      </c>
+      <c r="B36" t="s">
+        <v>260</v>
+      </c>
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>277</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E36" t="s">
+        <v>328</v>
+      </c>
+      <c r="F36" t="s">
+        <v>240</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Silent Hill 2 - Easy</v>
+      </c>
+      <c r="H36" t="s">
+        <v>327</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Silent Hill 2 - Easy', 'Silent Hill 2', 'Easy', 'Theme Of Laura', 'Akira Yamaoka', 'Video Games', 'music/video games/Silent Hill 2 - Easy', 'https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>330</v>
+      </c>
+      <c r="B37" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" t="s">
+        <v>259</v>
+      </c>
+      <c r="E37" t="s">
+        <v>328</v>
+      </c>
+      <c r="F37" t="s">
+        <v>240</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Silent Hill 2 - Hard</v>
+      </c>
+      <c r="H37" t="s">
+        <v>327</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Silent Hill 2 - Hard', 'Silent Hill 2', 'Hard', 'Theme Of Laura', 'Akira Yamaoka', 'Video Games', 'music/video games/Silent Hill 2 - Hard', 'https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E');</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>322</v>
+      </c>
+      <c r="B38" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>252</v>
-      </c>
-      <c r="D10" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
         <v>255</v>
       </c>
-      <c r="D11" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="E38" t="s">
+        <v>321</v>
+      </c>
+      <c r="F38" t="s">
+        <v>240</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Stardew Valley - Easy</v>
+      </c>
+      <c r="H38" t="s">
+        <v>320</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Stardew Valley - Easy', 'Stardew Valley', 'Easy', 'Spring (The Valley Comes Alive)', 'Eric Barone', 'Video Games', 'music/video games/Stardew Valley - Easy', 'https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf');</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>323</v>
+      </c>
+      <c r="B39" t="s">
+        <v>256</v>
+      </c>
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>255</v>
+      </c>
+      <c r="E39" t="s">
+        <v>321</v>
+      </c>
+      <c r="F39" t="s">
+        <v>240</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Stardew Valley - Hard</v>
+      </c>
+      <c r="H39" t="s">
+        <v>320</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Stardew Valley - Hard', 'Stardew Valley', 'Hard', 'Spring (The Valley Comes Alive)', 'Eric Barone', 'Video Games', 'music/video games/Stardew Valley - Hard', 'https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf');</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>325</v>
+      </c>
+      <c r="B40" t="s">
         <v>257</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
         <v>258</v>
       </c>
-      <c r="H12" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>263</v>
-      </c>
-      <c r="D14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>264</v>
-      </c>
-      <c r="D15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>267</v>
-      </c>
-      <c r="D16" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>269</v>
-      </c>
-      <c r="D17" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>271</v>
-      </c>
-      <c r="D18" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>273</v>
-      </c>
-      <c r="D19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>275</v>
-      </c>
-      <c r="D20" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>276</v>
-      </c>
-      <c r="D21" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>279</v>
-      </c>
-      <c r="D22" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>282</v>
-      </c>
-      <c r="D23" t="s">
-        <v>281</v>
+      <c r="E40" t="s">
+        <v>326</v>
+      </c>
+      <c r="F40" t="s">
+        <v>240</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Subnautica - Easy</v>
+      </c>
+      <c r="H40" t="s">
+        <v>324</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Easy', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music/video games/Subnautica - Easy', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>325</v>
+      </c>
+      <c r="B41" t="s">
+        <v>257</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>258</v>
+      </c>
+      <c r="E41" t="s">
+        <v>326</v>
+      </c>
+      <c r="F41" t="s">
+        <v>240</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/Subnautica - Easy</v>
+      </c>
+      <c r="H41" t="s">
+        <v>324</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Hard', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music/video games/Subnautica - Easy', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" t="s">
+        <v>346</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" t="s">
+        <v>348</v>
+      </c>
+      <c r="E42" t="s">
+        <v>345</v>
+      </c>
+      <c r="F42" t="s">
+        <v>240</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/The Elder Scrolls V Skyrim - Easy</v>
+      </c>
+      <c r="H42" t="s">
+        <v>349</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Easy', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music/video games/The Elder Scrolls V Skyrim - Easy', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>347</v>
+      </c>
+      <c r="B43" t="s">
+        <v>346</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" t="s">
+        <v>348</v>
+      </c>
+      <c r="E43" t="s">
+        <v>345</v>
+      </c>
+      <c r="F43" t="s">
+        <v>240</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>music/video games/The Elder Scrolls V Skyrim - Easy</v>
+      </c>
+      <c r="H43" t="s">
+        <v>349</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Hard', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music/video games/The Elder Scrolls V Skyrim - Easy', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I43">
+    <sortCondition ref="A1:A43"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4588B35-0419-4A99-A836-6C071068D931}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86584CCA-23E9-457B-BA96-43FBE00CFE13}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="107.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
+        <v>music/anime/Breaking Bad - Easy</v>
+      </c>
+      <c r="H2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Breaking Bad - Easy', 'Breaking Bad', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Breaking Bad - Easy', 'https://www.youtube.com/embed/Eksw56g-WBY?si=j9I6GsbSoH04xxcr');</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Switching to backend supplying mp3 files
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E138FB7C-717C-4DA3-B0CC-E0CAA43A60C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53422041-1387-419D-899E-DE7B6431719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5130" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anime" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1469,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="H33" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I41"/>
+    <sheetView tabSelected="1" topLeftCell="I36" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,15 +1543,15 @@
         <v>7</v>
       </c>
       <c r="G2" t="str">
-        <f>"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
-        <v>music/anime/Angel Beats OP1 - Easy</v>
+        <f>"music\"&amp;LOWER(F2)&amp;"\"&amp;A2&amp;".mp3"</f>
+        <v>music\anime\Angel Beats OP1 - Easy.mp3</v>
       </c>
       <c r="H2" t="s">
         <v>112</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Easy', 'https://www.youtube.com/embed/Eksw56g-WBY?si=j9I6GsbSoH04xxcr');</v>
+        <f>"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Angel Beats OP1 - Easy', 'Angel Beats', 'Easy', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music\anime\Angel Beats OP1 - Easy.mp3', 'https://www.youtube.com/embed/Eksw56g-WBY?si=j9I6GsbSoH04xxcr');</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1566,15 +1574,15 @@
         <v>7</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G41" si="0">"music/"&amp;LOWER(F3)&amp;"/"&amp;A3</f>
-        <v>music/anime/Angel Beats OP1 - Hard</v>
+        <f t="shared" ref="G3:G41" si="0">"music\"&amp;LOWER(F3)&amp;"\"&amp;A3&amp;".mp3"</f>
+        <v>music\anime\Angel Beats OP1 - Hard.mp3</v>
       </c>
       <c r="H3" t="s">
         <v>112</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music/anime/Angel Beats OP1 - Hard', 'https://www.youtube.com/embed/Eksw56g-WBY?si=j9I6GsbSoH04xxcr');</v>
+        <f t="shared" ref="I3:I41" si="1">"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Angel Beats OP1 - Hard', 'Angel Beats', 'Hard', 'My Soul, Your Beats!', 'Lia', 'Anime', 'music\anime\Angel Beats OP1 - Hard.mp3', 'https://www.youtube.com/embed/Eksw56g-WBY?si=j9I6GsbSoH04xxcr');</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1598,14 +1606,14 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Attack On Titan OP1 - Easy</v>
+        <v>music\anime\Attack On Titan OP1 - Easy.mp3</v>
       </c>
       <c r="H4" t="s">
         <v>113</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Easy', 'https://www.youtube.com/embed/8OkpRK2_gVs?si=-kglNm-YIt48I5Nn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Attack On Titan OP1 - Easy', 'Attack on Titan', 'Easy', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music\anime\Attack On Titan OP1 - Easy.mp3', 'https://www.youtube.com/embed/8OkpRK2_gVs?si=-kglNm-YIt48I5Nn');</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1629,14 +1637,14 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Attack On Titan OP1 - Hard</v>
+        <v>music\anime\Attack On Titan OP1 - Hard.mp3</v>
       </c>
       <c r="H5" t="s">
         <v>113</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music/anime/Attack On Titan OP1 - Hard', 'https://www.youtube.com/embed/8OkpRK2_gVs?si=-kglNm-YIt48I5Nn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Attack On Titan OP1 - Hard', 'Attack on Titan', 'Hard', 'Guren no Yumiya', 'Linked Horizon', 'Anime', 'music\anime\Attack On Titan OP1 - Hard.mp3', 'https://www.youtube.com/embed/8OkpRK2_gVs?si=-kglNm-YIt48I5Nn');</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1660,14 +1668,14 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Berserk OP1 - Easy</v>
+        <v>music\anime\Berserk OP1 - Easy.mp3</v>
       </c>
       <c r="H6" t="s">
         <v>114</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Easy', 'https://www.youtube.com/embed/9TRemrRaPjc?si=YpmGAgRTQ3IRXA0v');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Berserk OP1 - Easy', 'Berserk', 'Easy', 'Tell Me Why', 'PENPALS', 'Anime', 'music\anime\Berserk OP1 - Easy.mp3', 'https://www.youtube.com/embed/9TRemrRaPjc?si=YpmGAgRTQ3IRXA0v');</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1691,14 +1699,14 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Berserk OP1 - Hard</v>
+        <v>music\anime\Berserk OP1 - Hard.mp3</v>
       </c>
       <c r="H7" t="s">
         <v>114</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', 'music/anime/Berserk OP1 - Hard', 'https://www.youtube.com/embed/9TRemrRaPjc?si=YpmGAgRTQ3IRXA0v');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Berserk OP1 - Hard', 'Berserk', 'Hard', 'Tell Me Why', 'PENPALS', 'Anime', 'music\anime\Berserk OP1 - Hard.mp3', 'https://www.youtube.com/embed/9TRemrRaPjc?si=YpmGAgRTQ3IRXA0v');</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1722,14 +1730,14 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Chainsaw Man OP1 - Easy</v>
+        <v>music\anime\Chainsaw Man OP1 - Easy.mp3</v>
       </c>
       <c r="H8" t="s">
         <v>115</v>
       </c>
       <c r="I8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Easy', 'https://www.youtube.com/embed/dFlDRhvM4L0?si=E8piBUpyTulnz6Ez');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Chainsaw Man OP1 - Easy', 'Chainsaw Man', 'Easy', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music\anime\Chainsaw Man OP1 - Easy.mp3', 'https://www.youtube.com/embed/dFlDRhvM4L0?si=E8piBUpyTulnz6Ez');</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1753,14 +1761,14 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Chainsaw Man OP1 - Hard</v>
+        <v>music\anime\Chainsaw Man OP1 - Hard.mp3</v>
       </c>
       <c r="H9" t="s">
         <v>115</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music/anime/Chainsaw Man OP1 - Hard', 'https://www.youtube.com/embed/dFlDRhvM4L0?si=E8piBUpyTulnz6Ez');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Chainsaw Man OP1 - Hard', 'Chainsaw Man', 'Hard', 'Kick Back', 'Kenshi Yonezu', 'Anime', 'music\anime\Chainsaw Man OP1 - Hard.mp3', 'https://www.youtube.com/embed/dFlDRhvM4L0?si=E8piBUpyTulnz6Ez');</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1784,14 +1792,14 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Code Geass OP1 - Easy</v>
+        <v>music\anime\Code Geass OP1 - Easy.mp3</v>
       </c>
       <c r="H10" t="s">
         <v>116</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Easy', 'https://www.youtube.com/embed/G8CFuZ9MseQ?si=AcAvfrCQuKQIaW6o');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Code Geass OP1 - Easy', 'Code Geass', 'Easy', 'COLORS', 'FLOW', 'Anime', 'music\anime\Code Geass OP1 - Easy.mp3', 'https://www.youtube.com/embed/G8CFuZ9MseQ?si=AcAvfrCQuKQIaW6o');</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1815,14 +1823,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Code Geass OP1 - Hard</v>
+        <v>music\anime\Code Geass OP1 - Hard.mp3</v>
       </c>
       <c r="H11" t="s">
         <v>116</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', 'music/anime/Code Geass OP1 - Hard', 'https://www.youtube.com/embed/G8CFuZ9MseQ?si=AcAvfrCQuKQIaW6o');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Code Geass OP1 - Hard', 'Code Geass', 'Hard', 'COLORS', 'FLOW', 'Anime', 'music\anime\Code Geass OP1 - Hard.mp3', 'https://www.youtube.com/embed/G8CFuZ9MseQ?si=AcAvfrCQuKQIaW6o');</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1846,14 +1854,14 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Death Note OP1 - Easy</v>
+        <v>music\anime\Death Note OP1 - Easy.mp3</v>
       </c>
       <c r="H12" t="s">
         <v>355</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Easy', 'https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Death Note OP1 - Easy', 'Death Note', 'Easy', 'The World', 'Nightmare', 'Anime', 'music\anime\Death Note OP1 - Easy.mp3', 'https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2');</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1877,14 +1885,14 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Death Note OP1 - Hard</v>
+        <v>music\anime\Death Note OP1 - Hard.mp3</v>
       </c>
       <c r="H13" t="s">
         <v>355</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music/anime/Death Note OP1 - Hard', 'https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Death Note OP1 - Hard', 'Death Note', 'Hard', 'The World', 'Nightmare', 'Anime', 'music\anime\Death Note OP1 - Hard.mp3', 'https://www.youtube.com/embed/kNyR46eHDxE?si=GzSCcOA6C4Fkehs2');</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1908,14 +1916,14 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Death Parade OP1 - Easy</v>
+        <v>music\anime\Death Parade OP1 - Easy.mp3</v>
       </c>
       <c r="H14" t="s">
         <v>117</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Easy', 'https://www.youtube.com/embed/UjjTMNDZi-A?si=NDKOg-OGXXljvXp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Death Parade OP1 - Easy', 'Death Parade', 'Easy', 'Flyers', 'BRADIO', 'Anime', 'music\anime\Death Parade OP1 - Easy.mp3', 'https://www.youtube.com/embed/UjjTMNDZi-A?si=NDKOg-OGXXljvXp3');</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1939,14 +1947,14 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Death Parade OP1 - Hard</v>
+        <v>music\anime\Death Parade OP1 - Hard.mp3</v>
       </c>
       <c r="H15" t="s">
         <v>117</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', 'music/anime/Death Parade OP1 - Hard', 'https://www.youtube.com/embed/UjjTMNDZi-A?si=NDKOg-OGXXljvXp3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Death Parade OP1 - Hard', 'Death Parade', 'Hard', 'Flyers', 'BRADIO', 'Anime', 'music\anime\Death Parade OP1 - Hard.mp3', 'https://www.youtube.com/embed/UjjTMNDZi-A?si=NDKOg-OGXXljvXp3');</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1970,14 +1978,14 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Dragon Ball Z OP1 - Easy</v>
+        <v>music\anime\Dragon Ball Z OP1 - Easy.mp3</v>
       </c>
       <c r="H16" t="s">
         <v>118</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Easy', 'https://www.youtube.com/embed/0liOFNYuNMc?si=k_vHUXcqqbjDsgvF');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Dragon Ball Z OP1 - Easy', 'Dragon Ball Z', 'Easy', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music\anime\Dragon Ball Z OP1 - Easy.mp3', 'https://www.youtube.com/embed/0liOFNYuNMc?si=k_vHUXcqqbjDsgvF');</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2001,14 +2009,14 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Dragon Ball Z OP1 - Hard</v>
+        <v>music\anime\Dragon Ball Z OP1 - Hard.mp3</v>
       </c>
       <c r="H17" t="s">
         <v>118</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music/anime/Dragon Ball Z OP1 - Hard', 'https://www.youtube.com/embed/0liOFNYuNMc?si=k_vHUXcqqbjDsgvF');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Dragon Ball Z OP1 - Hard', 'Dragon Ball Z', 'Hard', 'Cha-La Head-Cha-La', 'Hironobu Kageyama', 'Anime', 'music\anime\Dragon Ball Z OP1 - Hard.mp3', 'https://www.youtube.com/embed/0liOFNYuNMc?si=k_vHUXcqqbjDsgvF');</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2032,14 +2040,14 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Ergo Proxy OP1 - Easy</v>
+        <v>music\anime\Ergo Proxy OP1 - Easy.mp3</v>
       </c>
       <c r="H18" t="s">
         <v>119</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Easy', 'https://www.youtube.com/embed/oAXrRWLKzko?si=kHLt_FT9Y4tQoQcM');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Easy', 'Ergo Proxy', 'Easy', 'Kiri', 'Monoral', 'Anime', 'music\anime\Ergo Proxy OP1 - Easy.mp3', 'https://www.youtube.com/embed/oAXrRWLKzko?si=kHLt_FT9Y4tQoQcM');</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2063,14 +2071,14 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Ergo Proxy OP1 - Hard</v>
+        <v>music\anime\Ergo Proxy OP1 - Hard.mp3</v>
       </c>
       <c r="H19" t="s">
         <v>119</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', 'music/anime/Ergo Proxy OP1 - Hard', 'https://www.youtube.com/embed/oAXrRWLKzko?si=kHLt_FT9Y4tQoQcM');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', 'music\anime\Ergo Proxy OP1 - Hard.mp3', 'https://www.youtube.com/embed/oAXrRWLKzko?si=kHLt_FT9Y4tQoQcM');</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2094,14 +2102,14 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Evangelion OP1 - Easy</v>
+        <v>music\anime\Evangelion OP1 - Easy.mp3</v>
       </c>
       <c r="H20" t="s">
         <v>120</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Easy', 'https://www.youtube.com/embed/fShlVhCfHig?si=uwmfyCY6EQBp3O5q');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music\anime\Evangelion OP1 - Easy.mp3', 'https://www.youtube.com/embed/fShlVhCfHig?si=uwmfyCY6EQBp3O5q');</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2125,17 +2133,17 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Evangelion OP1 - Hard</v>
+        <v>music\anime\Evangelion OP1 - Hard.mp3</v>
       </c>
       <c r="H21" t="s">
         <v>120</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music/anime/Evangelion OP1 - Hard', 'https://www.youtube.com/embed/fShlVhCfHig?si=uwmfyCY6EQBp3O5q');</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music\anime\Evangelion OP1 - Hard.mp3', 'https://www.youtube.com/embed/fShlVhCfHig?si=uwmfyCY6EQBp3O5q');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2156,17 +2164,17 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Fate Stay Night UBW OP2 - Easy</v>
+        <v>music\anime\Fate Stay Night UBW OP2 - Easy.mp3</v>
       </c>
       <c r="H22" t="s">
         <v>121</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Easy', 'https://www.youtube.com/embed/7vZp3yGxZXE?si=Wd1SS5UJbtOD6TET');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', 'music\anime\Fate Stay Night UBW OP2 - Easy.mp3', 'https://www.youtube.com/embed/7vZp3yGxZXE?si=Wd1SS5UJbtOD6TET');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2187,14 +2195,14 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Fate Stay Night UBW OP2 - Hard</v>
+        <v>music\anime\Fate Stay Night UBW OP2 - Hard.mp3</v>
       </c>
       <c r="H23" t="s">
         <v>121</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', 'music/anime/Fate Stay Night UBW OP2 - Hard', 'https://www.youtube.com/embed/7vZp3yGxZXE?si=Wd1SS5UJbtOD6TET');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Hard', 'Fate Stay Night - Unlimited Blade Works', 'Hard', 'Brave Shine', 'Aimer', 'Anime', 'music\anime\Fate Stay Night UBW OP2 - Hard.mp3', 'https://www.youtube.com/embed/7vZp3yGxZXE?si=Wd1SS5UJbtOD6TET');</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2218,14 +2226,14 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Guilty Crown OP1 - Easy</v>
+        <v>music\anime\Guilty Crown OP1 - Easy.mp3</v>
       </c>
       <c r="H24" t="s">
         <v>122</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Easy', 'https://www.youtube.com/embed/xmh3mNvgJBs?si=ZXfyeYtURU7QnKaz');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Guilty Crown OP1 - Easy', 'Guilty Crown', 'Easy', 'My Dearest', 'Koeda', 'Anime', 'music\anime\Guilty Crown OP1 - Easy.mp3', 'https://www.youtube.com/embed/xmh3mNvgJBs?si=ZXfyeYtURU7QnKaz');</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2249,14 +2257,14 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Guilty Crown OP1 - Hard</v>
+        <v>music\anime\Guilty Crown OP1 - Hard.mp3</v>
       </c>
       <c r="H25" t="s">
         <v>122</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', 'music/anime/Guilty Crown OP1 - Hard', 'https://www.youtube.com/embed/xmh3mNvgJBs?si=ZXfyeYtURU7QnKaz');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Guilty Crown OP1 - Hard', 'Guilty Crown', 'Hard', 'My Dearest', 'Koeda', 'Anime', 'music\anime\Guilty Crown OP1 - Hard.mp3', 'https://www.youtube.com/embed/xmh3mNvgJBs?si=ZXfyeYtURU7QnKaz');</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2280,14 +2288,14 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Jojo OP2 - Easy</v>
+        <v>music\anime\Jojo OP2 - Easy.mp3</v>
       </c>
       <c r="H26" t="s">
         <v>123</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Easy', 'https://www.youtube.com/embed/SJkCLcnGB-c?si=Dmi7p92S0nnDgt6b');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Jojo OP2 - Easy', 'Jojo''s Bizarre Adventure', 'Easy', 'Bloody Stream', 'Coda', 'Anime', 'music\anime\Jojo OP2 - Easy.mp3', 'https://www.youtube.com/embed/SJkCLcnGB-c?si=Dmi7p92S0nnDgt6b');</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2311,14 +2319,14 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Jojo OP2 - Hard</v>
+        <v>music\anime\Jojo OP2 - Hard.mp3</v>
       </c>
       <c r="H27" t="s">
         <v>123</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', 'music/anime/Jojo OP2 - Hard', 'https://www.youtube.com/embed/SJkCLcnGB-c?si=Dmi7p92S0nnDgt6b');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Jojo OP2 - Hard', 'Jojo''s Bizarre Adventure', 'Hard', 'Bloody Stream', 'Coda', 'Anime', 'music\anime\Jojo OP2 - Hard.mp3', 'https://www.youtube.com/embed/SJkCLcnGB-c?si=Dmi7p92S0nnDgt6b');</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2342,14 +2350,14 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Jujutsu Kaisen OP2 - Easy</v>
+        <v>music\anime\Jujutsu Kaisen OP2 - Easy.mp3</v>
       </c>
       <c r="H28" t="s">
         <v>124</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Easy', 'https://www.youtube.com/embed/8nNujr378EA?si=gLS_j0N6pSuCTBl0');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Easy', 'Jujutsu Kaisen', 'Easy', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music\anime\Jujutsu Kaisen OP2 - Easy.mp3', 'https://www.youtube.com/embed/8nNujr378EA?si=gLS_j0N6pSuCTBl0');</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2373,17 +2381,17 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Jujutsu Kaisen OP2 - Hard</v>
+        <v>music\anime\Jujutsu Kaisen OP2 - Hard.mp3</v>
       </c>
       <c r="H29" t="s">
         <v>124</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music/anime/Jujutsu Kaisen OP2 - Hard', 'https://www.youtube.com/embed/8nNujr378EA?si=gLS_j0N6pSuCTBl0');</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music\anime\Jujutsu Kaisen OP2 - Hard.mp3', 'https://www.youtube.com/embed/8nNujr378EA?si=gLS_j0N6pSuCTBl0');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2404,17 +2412,17 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/One Punch Man OP1 - Easy</v>
+        <v>music\anime\One Punch Man OP1 - Easy.mp3</v>
       </c>
       <c r="H30" t="s">
         <v>125</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Easy', 'https://www.youtube.com/embed/atxYe-nOa9w?si=uA85dxeTJX_olQuQ');</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music\anime\One Punch Man OP1 - Easy.mp3', 'https://www.youtube.com/embed/atxYe-nOa9w?si=uA85dxeTJX_olQuQ');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2435,14 +2443,14 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/One Punch Man OP1 - Hard</v>
+        <v>music\anime\One Punch Man OP1 - Hard.mp3</v>
       </c>
       <c r="H31" t="s">
         <v>125</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music/anime/One Punch Man OP1 - Hard', 'https://www.youtube.com/embed/atxYe-nOa9w?si=uA85dxeTJX_olQuQ');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('One Punch Man OP1 - Hard', 'One Punch Man', 'Hard', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music\anime\One Punch Man OP1 - Hard.mp3', 'https://www.youtube.com/embed/atxYe-nOa9w?si=uA85dxeTJX_olQuQ');</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2466,14 +2474,14 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Psycho Pass OP2 - Easy</v>
+        <v>music\anime\Psycho Pass OP2 - Easy.mp3</v>
       </c>
       <c r="H32" t="s">
         <v>126</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Easy', 'https://www.youtube.com/embed/SJ-aUXmJM8Q?si=vpLQ53nAOc6o4iG0');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Psycho Pass OP2 - Easy', 'Psycho Pass', 'Easy', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music\anime\Psycho Pass OP2 - Easy.mp3', 'https://www.youtube.com/embed/SJ-aUXmJM8Q?si=vpLQ53nAOc6o4iG0');</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2497,14 +2505,14 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Psycho Pass OP2 - Hard</v>
+        <v>music\anime\Psycho Pass OP2 - Hard.mp3</v>
       </c>
       <c r="H33" t="s">
         <v>126</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music/anime/Psycho Pass OP2 - Hard', 'https://www.youtube.com/embed/SJ-aUXmJM8Q?si=vpLQ53nAOc6o4iG0');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Psycho Pass OP2 - Hard', 'Psycho Pass', 'Hard', 'Out of Control', 'Nothing''s Carved in Stone', 'Anime', 'music\anime\Psycho Pass OP2 - Hard.mp3', 'https://www.youtube.com/embed/SJ-aUXmJM8Q?si=vpLQ53nAOc6o4iG0');</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2528,14 +2536,14 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Ranking of Kings OP2 - Easy</v>
+        <v>music\anime\Ranking of Kings OP2 - Easy.mp3</v>
       </c>
       <c r="H34" t="s">
         <v>127</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Easy', 'https://www.youtube.com/embed/dWZAH5w8jkQ?si=9RGXofT18-IxHqHV');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Ranking of Kings OP2 - Easy', 'Ranking of Kings', 'Easy', 'Naked Hero', 'Vaundy', 'Anime', 'music\anime\Ranking of Kings OP2 - Easy.mp3', 'https://www.youtube.com/embed/dWZAH5w8jkQ?si=9RGXofT18-IxHqHV');</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2559,14 +2567,14 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Ranking of Kings OP2 - Hard</v>
+        <v>music\anime\Ranking of Kings OP2 - Hard.mp3</v>
       </c>
       <c r="H35" t="s">
         <v>127</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', 'music/anime/Ranking of Kings OP2 - Hard', 'https://www.youtube.com/embed/dWZAH5w8jkQ?si=9RGXofT18-IxHqHV');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Ranking of Kings OP2 - Hard', 'Ranking of Kings', 'Hard', 'Naked Hero', 'Vaundy', 'Anime', 'music\anime\Ranking of Kings OP2 - Hard.mp3', 'https://www.youtube.com/embed/dWZAH5w8jkQ?si=9RGXofT18-IxHqHV');</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2590,14 +2598,14 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Soul Eater OP2 - Easy</v>
+        <v>music\anime\Soul Eater OP2 - Easy.mp3</v>
       </c>
       <c r="H36" t="s">
         <v>128</v>
       </c>
       <c r="I36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Easy', 'https://www.youtube.com/embed/-eYK3YP524A?si=MgtUBwZPkveHTnk9');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Soul Eater OP2 - Easy', 'Soul Eater', 'Easy', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music\anime\Soul Eater OP2 - Easy.mp3', 'https://www.youtube.com/embed/-eYK3YP524A?si=MgtUBwZPkveHTnk9');</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2621,14 +2629,14 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Soul Eater OP2 - Hard</v>
+        <v>music\anime\Soul Eater OP2 - Hard.mp3</v>
       </c>
       <c r="H37" t="s">
         <v>128</v>
       </c>
       <c r="I37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music/anime/Soul Eater OP2 - Hard', 'https://www.youtube.com/embed/-eYK3YP524A?si=MgtUBwZPkveHTnk9');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Soul Eater OP2 - Hard', 'Soul Eater', 'Hard', 'Black Paper Moon', 'Tomoko Kawase', 'Anime', 'music\anime\Soul Eater OP2 - Hard.mp3', 'https://www.youtube.com/embed/-eYK3YP524A?si=MgtUBwZPkveHTnk9');</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2652,14 +2660,14 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Tokyo Ghoul OP1 - Easy</v>
+        <v>music\anime\Tokyo Ghoul OP1 - Easy.mp3</v>
       </c>
       <c r="H38" t="s">
         <v>129</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Easy', 'https://www.youtube.com/embed/7aMOurgDB-o?si=tXyvDGxch3IYZdrx');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Tokyo Ghoul OP1 - Easy', 'Tokyo Ghoul', 'Easy', 'Unravel', 'TK', 'Anime', 'music\anime\Tokyo Ghoul OP1 - Easy.mp3', 'https://www.youtube.com/embed/7aMOurgDB-o?si=tXyvDGxch3IYZdrx');</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2683,14 +2691,14 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Tokyo Ghoul OP1 - Hard</v>
+        <v>music\anime\Tokyo Ghoul OP1 - Hard.mp3</v>
       </c>
       <c r="H39" t="s">
         <v>129</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', 'music/anime/Tokyo Ghoul OP1 - Hard', 'https://www.youtube.com/embed/7aMOurgDB-o?si=tXyvDGxch3IYZdrx');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Tokyo Ghoul OP1 - Hard', 'Tokyo Ghoul', 'Hard', 'Unravel', 'TK', 'Anime', 'music\anime\Tokyo Ghoul OP1 - Hard.mp3', 'https://www.youtube.com/embed/7aMOurgDB-o?si=tXyvDGxch3IYZdrx');</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2714,14 +2722,14 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Vinland Saga OP1 - Easy</v>
+        <v>music\anime\Vinland Saga OP1 - Easy.mp3</v>
       </c>
       <c r="H40" t="s">
         <v>130</v>
       </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Easy', 'https://www.youtube.com/embed/7U7BDn-gU18?si=IwsLLB0GPUVaxQ4W');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Vinland Saga OP1 - Easy', 'Vinland Saga', 'Easy', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music\anime\Vinland Saga OP1 - Easy.mp3', 'https://www.youtube.com/embed/7U7BDn-gU18?si=IwsLLB0GPUVaxQ4W');</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2745,14 +2753,14 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>music/anime/Vinland Saga OP1 - Hard</v>
+        <v>music\anime\Vinland Saga OP1 - Hard.mp3</v>
       </c>
       <c r="H41" t="s">
         <v>130</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music/anime/Vinland Saga OP1 - Hard', 'https://www.youtube.com/embed/7U7BDn-gU18?si=IwsLLB0GPUVaxQ4W');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Vinland Saga OP1 - Hard', 'Vinland Saga', 'Hard', 'Mukanjyo', 'Survive Said The Prophet', 'Anime', 'music\anime\Vinland Saga OP1 - Hard.mp3', 'https://www.youtube.com/embed/7U7BDn-gU18?si=IwsLLB0GPUVaxQ4W');</v>
       </c>
     </row>
   </sheetData>
@@ -4126,7 +4134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F96BC2-62DB-49FB-AD78-FA2CCE8FE0BD}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleaning up mp3 fetch transition remnants from earlier approach
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53422041-1387-419D-899E-DE7B6431719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B7BFE3-6FA0-4D6C-B437-633DFDB8A331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5130" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5130" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anime" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1477,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I36" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="I36" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2073,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Ergo Proxy OP1 - Hard', 'Ergo Proxy', 'Hard', 'Kiri', 'Monoral', 'Anime', 'music\anime\Ergo Proxy OP1 - Hard.mp3', 'https://www.youtube.com/embed/oAXrRWLKzko?si=kHLt_FT9Y4tQoQcM');</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2112,7 +2104,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Evangelion OP1 - Easy', 'Neon Genesis Evangelion', 'Easy', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music\anime\Evangelion OP1 - Easy.mp3', 'https://www.youtube.com/embed/fShlVhCfHig?si=uwmfyCY6EQBp3O5q');</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2143,7 +2135,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Evangelion OP1 - Hard', 'Neon Genesis Evangelion', 'Hard', 'A Cruel Angel''s Thesis', 'Yoko Takahashi', 'Anime', 'music\anime\Evangelion OP1 - Hard.mp3', 'https://www.youtube.com/embed/fShlVhCfHig?si=uwmfyCY6EQBp3O5q');</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2174,7 +2166,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fate Stay Night UBW OP2 - Easy', 'Fate Stay Night - Unlimited Blade Works', 'Easy', 'Brave Shine', 'Aimer', 'Anime', 'music\anime\Fate Stay Night UBW OP2 - Easy.mp3', 'https://www.youtube.com/embed/7vZp3yGxZXE?si=Wd1SS5UJbtOD6TET');</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2391,7 +2383,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Jujutsu Kaisen OP2 - Hard', 'Jujutsu Kaisen', 'Hard', 'Vivid Vice', 'Who-Ya Extended', 'Anime', 'music\anime\Jujutsu Kaisen OP2 - Hard.mp3', 'https://www.youtube.com/embed/8nNujr378EA?si=gLS_j0N6pSuCTBl0');</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2422,7 +2414,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('One Punch Man OP1 - Easy', 'One Punch Man', 'Easy', 'The Hero!! ~Ikareru Ken ni Honō o Tsukeru~', 'JAM Project', 'Anime', 'music\anime\One Punch Man OP1 - Easy.mp3', 'https://www.youtube.com/embed/atxYe-nOa9w?si=uA85dxeTJX_olQuQ');</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2772,7 +2764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7033B7E-9E28-44F0-AF22-AF8799EBF584}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="H35" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="I38" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I43"/>
     </sheetView>
   </sheetViews>
@@ -2818,7 +2810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>208</v>
       </c>
@@ -2838,15 +2830,15 @@
         <v>132</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G43" si="0">"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
-        <v>music/indie/Bombay Bicycle Club - Easy</v>
+        <f>"music\"&amp;LOWER(F2)&amp;"\"&amp;A2&amp;".mp3"</f>
+        <v>music\indie\Bombay Bicycle Club - Easy.mp3</v>
       </c>
       <c r="H2" t="s">
         <v>162</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" ref="I2:I43" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bombay Bicycle Club - Easy', 'Bombay Bicycle Club', 'Easy', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music/indie/Bombay Bicycle Club - Easy', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
+        <f>"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Bombay Bicycle Club - Easy', 'Bombay Bicycle Club', 'Easy', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music\indie\Bombay Bicycle Club - Easy.mp3', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -2869,18 +2861,18 @@
         <v>132</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>music/indie/Bombay Bicycle Club - Hard</v>
+        <f t="shared" ref="G3:G43" si="0">"music\"&amp;LOWER(F3)&amp;"\"&amp;A3&amp;".mp3"</f>
+        <v>music\indie\Bombay Bicycle Club - Hard.mp3</v>
       </c>
       <c r="H3" t="s">
         <v>162</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bombay Bicycle Club - Hard', 'Bombay Bicycle Club', 'Hard', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music/indie/Bombay Bicycle Club - Hard', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I43" si="1">"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Bombay Bicycle Club - Hard', 'Bombay Bicycle Club', 'Hard', 'Always Like This', 'Bombay Bicycle Club', 'Indie', 'music\indie\Bombay Bicycle Club - Hard.mp3', 'https://www.youtube.com/embed/Vh9FfmMN-ik?si=v5hHaoibu8dFQ49O');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>222</v>
       </c>
@@ -2901,17 +2893,17 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Brand New - Easy</v>
+        <v>music\indie\Brand New - Easy.mp3</v>
       </c>
       <c r="H4" t="s">
         <v>180</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Brand New - Easy', 'Brand New', 'Easy', '1996', 'Brand New', 'Indie', 'music/indie/Brand New - Easy', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Brand New - Easy', 'Brand New', 'Easy', '1996', 'Brand New', 'Indie', 'music\indie\Brand New - Easy.mp3', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>223</v>
       </c>
@@ -2932,17 +2924,17 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Brand New - Hard</v>
+        <v>music\indie\Brand New - Hard.mp3</v>
       </c>
       <c r="H5" t="s">
         <v>180</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Brand New - Hard', 'Brand New', 'Hard', '1996', 'Brand New', 'Indie', 'music/indie/Brand New - Hard', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Brand New - Hard', 'Brand New', 'Hard', '1996', 'Brand New', 'Indie', 'music\indie\Brand New - Hard.mp3', 'https://www.youtube.com/embed/eXmCWvT6X3I?si=YL26XjrrVn0Nlib2');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -2963,14 +2955,14 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Bright Eyes - Easy</v>
+        <v>music\indie\Bright Eyes - Easy.mp3</v>
       </c>
       <c r="H6" t="s">
         <v>148</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bright Eyes - Easy', 'Bright Eyes', 'Easy', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music/indie/Bright Eyes - Easy', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Bright Eyes - Easy', 'Bright Eyes', 'Easy', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music\indie\Bright Eyes - Easy.mp3', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2994,14 +2986,14 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Bright Eyes - Hard</v>
+        <v>music\indie\Bright Eyes - Hard.mp3</v>
       </c>
       <c r="H7" t="s">
         <v>148</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Bright Eyes - Hard', 'Bright Eyes', 'Hard', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music/indie/Bright Eyes - Hard', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Bright Eyes - Hard', 'Bright Eyes', 'Hard', ' Let''s Not Shit Ourselves (To Love And To Be Loved)', 'Bright Eyes', 'Indie', 'music\indie\Bright Eyes - Hard.mp3', 'https://www.youtube.com/embed/3dhXOMvsnak?si=ehoEGKvJVENRK6Vm');</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3025,14 +3017,14 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Editors - Easy</v>
+        <v>music\indie\Editors - Easy.mp3</v>
       </c>
       <c r="H8" t="s">
         <v>182</v>
       </c>
       <c r="I8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Editors - Easy', 'Editors', 'Easy', 'An End Has A Start', 'Editors', 'Indie', 'music/indie/Editors - Easy', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Editors - Easy', 'Editors', 'Easy', 'An End Has A Start', 'Editors', 'Indie', 'music\indie\Editors - Easy.mp3', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3056,14 +3048,14 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Editors - Hard</v>
+        <v>music\indie\Editors - Hard.mp3</v>
       </c>
       <c r="H9" t="s">
         <v>182</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Editors - Hard', 'Editors', 'Hard', 'An End Has A Start', 'Editors', 'Indie', 'music/indie/Editors - Hard', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Editors - Hard', 'Editors', 'Hard', 'An End Has A Start', 'Editors', 'Indie', 'music\indie\Editors - Hard.mp3', 'https://www.youtube.com/embed/UBpzJ-TLpbE?si=vHK5L91iq3dNULsd');</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3087,14 +3079,14 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Frightened Rabbit - Easy</v>
+        <v>music\indie\Frightened Rabbit - Easy.mp3</v>
       </c>
       <c r="H10" t="s">
         <v>135</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Frightened Rabbit - Easy', 'Frightened Rabbit', 'Easy', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music/indie/Frightened Rabbit - Easy', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Frightened Rabbit - Easy', 'Frightened Rabbit', 'Easy', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music\indie\Frightened Rabbit - Easy.mp3', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3118,14 +3110,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Frightened Rabbit - Hard</v>
+        <v>music\indie\Frightened Rabbit - Hard.mp3</v>
       </c>
       <c r="H11" t="s">
         <v>135</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Frightened Rabbit - Hard', 'Frightened Rabbit', 'Hard', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music/indie/Frightened Rabbit - Hard', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Frightened Rabbit - Hard', 'Frightened Rabbit', 'Hard', 'Keep Yourself Warm', 'Frightened Rabbit', 'Indie', 'music\indie\Frightened Rabbit - Hard.mp3', 'https://www.youtube.com/embed/J8fVX41-Njg?si=ubJYGVC8wM9zd34r');</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3149,14 +3141,14 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Funeral Suits - Easy</v>
+        <v>music\indie\Funeral Suits - Easy.mp3</v>
       </c>
       <c r="H12" t="s">
         <v>226</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Funeral Suits - Easy', 'Funeral Suits', 'Easy', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music/indie/Funeral Suits - Easy', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Funeral Suits - Easy', 'Funeral Suits', 'Easy', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music\indie\Funeral Suits - Easy.mp3', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3180,14 +3172,14 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Funeral Suits - Hard</v>
+        <v>music\indie\Funeral Suits - Hard.mp3</v>
       </c>
       <c r="H13" t="s">
         <v>226</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Funeral Suits - Hard', 'Funeral Suits', 'Hard', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music/indie/Funeral Suits - Hard', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Funeral Suits - Hard', 'Funeral Suits', 'Hard', 'All Those Friendly People', 'Funeral Suits', 'Indie', 'music\indie\Funeral Suits - Hard.mp3', 'https://www.youtube.com/embed/Sw4uj_od5pg?si=jDG1TLMkg2SDB1t6');</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3211,14 +3203,14 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Half-Alive - Easy</v>
+        <v>music\indie\Half-Alive - Easy.mp3</v>
       </c>
       <c r="H14" t="s">
         <v>176</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Half-Alive - Easy', 'Half-Alive', 'Easy', 'Still Feel', 'Half-Alive', 'Indie', 'music/indie/Half-Alive - Easy', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Half-Alive - Easy', 'Half-Alive', 'Easy', 'Still Feel', 'Half-Alive', 'Indie', 'music\indie\Half-Alive - Easy.mp3', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3242,14 +3234,14 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Half-Alive - Hard</v>
+        <v>music\indie\Half-Alive - Hard.mp3</v>
       </c>
       <c r="H15" t="s">
         <v>176</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Half-Alive - Hard', 'Half-Alive', 'Hard', 'Still Feel', 'Half-Alive', 'Indie', 'music/indie/Half-Alive - Hard', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Half-Alive - Hard', 'Half-Alive', 'Hard', 'Still Feel', 'Half-Alive', 'Indie', 'music\indie\Half-Alive - Hard.mp3', 'https://www.youtube.com/embed/C2RA8cRiInk?si=guNpRJmxX3KvZYfn');</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3273,14 +3265,14 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/I Don''t Know How But They Found Me - Easy</v>
+        <v>music\indie\I Don''t Know How But They Found Me - Easy.mp3</v>
       </c>
       <c r="H16" t="s">
         <v>164</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Easy', 'I Don''t Know How But They Found Me', 'Easy', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music/indie/I Don''t Know How But They Found Me - Easy', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Easy', 'I Don''t Know How But They Found Me', 'Easy', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music\indie\I Don''t Know How But They Found Me - Easy.mp3', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3304,14 +3296,14 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/I Don''t Know How But They Found Me - Hard</v>
+        <v>music\indie\I Don''t Know How But They Found Me - Hard.mp3</v>
       </c>
       <c r="H17" t="s">
         <v>164</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Hard', 'I Don''t Know How But They Found Me', 'Hard', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music/indie/I Don''t Know How But They Found Me - Hard', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('I Don''t Know How But They Found Me - Hard', 'I Don''t Know How But They Found Me', 'Hard', 'Choke', 'I Don''t Know How But They Found Me', 'Indie', 'music\indie\I Don''t Know How But They Found Me - Hard.mp3', 'https://www.youtube.com/embed/mvJjmWTg7Qo?si=J_NIFoDM1JSS1jzn');</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3335,14 +3327,14 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Interpol - Easy</v>
+        <v>music\indie\Interpol - Easy.mp3</v>
       </c>
       <c r="H18" t="s">
         <v>171</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Interpol - Easy', 'Interpol', 'Easy', 'Evil', 'Interpol', 'Indie', 'music/indie/Interpol - Easy', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Interpol - Easy', 'Interpol', 'Easy', 'Evil', 'Interpol', 'Indie', 'music\indie\Interpol - Easy.mp3', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3366,14 +3358,14 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Interpol - Hard</v>
+        <v>music\indie\Interpol - Hard.mp3</v>
       </c>
       <c r="H19" t="s">
         <v>171</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Interpol - Hard', 'Interpol', 'Hard', 'Evil', 'Interpol', 'Indie', 'music/indie/Interpol - Hard', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Interpol - Hard', 'Interpol', 'Hard', 'Evil', 'Interpol', 'Indie', 'music\indie\Interpol - Hard.mp3', 'https://www.youtube.com/embed/uUOMQzQdU34?si=ilsoc6fkZjHAkNXB');</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3397,14 +3389,14 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Iron And Wine - Easy</v>
+        <v>music\indie\Iron And Wine - Easy.mp3</v>
       </c>
       <c r="H20" t="s">
         <v>235</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Iron And Wine - Easy', 'Iron And Wine', 'Easy', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music/indie/Iron And Wine - Easy', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Iron And Wine - Easy', 'Iron And Wine', 'Easy', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music\indie\Iron And Wine - Easy.mp3', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3428,14 +3420,14 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Iron And Wine - Hard</v>
+        <v>music\indie\Iron And Wine - Hard.mp3</v>
       </c>
       <c r="H21" t="s">
         <v>235</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Iron And Wine - Hard', 'Iron And Wine', 'Hard', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music/indie/Iron And Wine - Hard', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Iron And Wine - Hard', 'Iron And Wine', 'Hard', 'Upwards Over The Mountain', 'Iron And Wine', 'Indie', 'music\indie\Iron And Wine - Hard.mp3', 'https://www.youtube.com/embed/Cg4CCy2kbuA?si=aQCou_0oyb2DhueN');</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3459,14 +3451,14 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/KennyHoopla - Easy</v>
+        <v>music\indie\KennyHoopla - Easy.mp3</v>
       </c>
       <c r="H22" t="s">
         <v>156</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('KennyHoopla - Easy', 'KennyHoopla', 'Easy', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music/indie/KennyHoopla - Easy', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('KennyHoopla - Easy', 'KennyHoopla', 'Easy', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music\indie\KennyHoopla - Easy.mp3', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -3490,14 +3482,14 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/KennyHoopla - Hard</v>
+        <v>music\indie\KennyHoopla - Hard.mp3</v>
       </c>
       <c r="H23" t="s">
         <v>156</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('KennyHoopla - Hard', 'KennyHoopla', 'Hard', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music/indie/KennyHoopla - Hard', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('KennyHoopla - Hard', 'KennyHoopla', 'Hard', 'How Will I Rest In Peace If I''m Buried By A Highway?', 'KennyHoopla', 'Indie', 'music\indie\KennyHoopla - Hard.mp3', 'https://www.youtube.com/embed/nDYNduUs2UY?si=pVN008HxyEH-V7Fz');</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3521,14 +3513,14 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Mewithoutyou - Easy</v>
+        <v>music\indie\Mewithoutyou - Easy.mp3</v>
       </c>
       <c r="H24" t="s">
         <v>144</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Mewithoutyou - Easy', 'Mewithoutyou', 'Easy', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music/indie/Mewithoutyou - Easy', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Mewithoutyou - Easy', 'Mewithoutyou', 'Easy', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music\indie\Mewithoutyou - Easy.mp3', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3552,14 +3544,14 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Mewithoutyou - Hard</v>
+        <v>music\indie\Mewithoutyou - Hard.mp3</v>
       </c>
       <c r="H25" t="s">
         <v>144</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Mewithoutyou - Hard', 'Mewithoutyou', 'Hard', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music/indie/Mewithoutyou - Hard', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Mewithoutyou - Hard', 'Mewithoutyou', 'Hard', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music\indie\Mewithoutyou - Hard.mp3', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3583,14 +3575,14 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Modern Baseball - Easy</v>
+        <v>music\indie\Modern Baseball - Easy.mp3</v>
       </c>
       <c r="H26" t="s">
         <v>152</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Modern Baseball - Easy', 'Modern Baseball', 'Easy', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music/indie/Modern Baseball - Easy', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Modern Baseball - Easy', 'Modern Baseball', 'Easy', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music\indie\Modern Baseball - Easy.mp3', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3614,14 +3606,14 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Modern Baseball - Hard</v>
+        <v>music\indie\Modern Baseball - Hard.mp3</v>
       </c>
       <c r="H27" t="s">
         <v>152</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Modern Baseball - Hard', 'Modern Baseball', 'Hard', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music/indie/Modern Baseball - Hard', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Modern Baseball - Hard', 'Modern Baseball', 'Hard', 'Wedding Singer', 'Modern Baseball', 'Indie', 'music\indie\Modern Baseball - Hard.mp3', 'https://www.youtube.com/embed/huMavLO2aBk?si=K8mci6IHL5L8rygH');</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3645,14 +3637,14 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Neutral Milk Hotel - Easy</v>
+        <v>music\indie\Neutral Milk Hotel - Easy.mp3</v>
       </c>
       <c r="H28" t="s">
         <v>140</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Neutral Milk Hotel - Easy', 'Neutral Milk Hotel', 'Easy', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music/indie/Neutral Milk Hotel - Easy', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Neutral Milk Hotel - Easy', 'Neutral Milk Hotel', 'Easy', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music\indie\Neutral Milk Hotel - Easy.mp3', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3676,14 +3668,14 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Neutral Milk Hotel - Hard</v>
+        <v>music\indie\Neutral Milk Hotel - Hard.mp3</v>
       </c>
       <c r="H29" t="s">
         <v>140</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Neutral Milk Hotel - Hard', 'Neutral Milk Hotel', 'Hard', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music/indie/Neutral Milk Hotel - Hard', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Neutral Milk Hotel - Hard', 'Neutral Milk Hotel', 'Hard', 'Holland, 1945', 'Neutral Milk Hotel', 'Indie', 'music\indie\Neutral Milk Hotel - Hard.mp3', 'https://www.youtube.com/embed/3eNK38nmzw4?si=Ax8ifLUCopOxGNM7');</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3707,14 +3699,14 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Pat The Bunny - Easy</v>
+        <v>music\indie\Pat The Bunny - Easy.mp3</v>
       </c>
       <c r="H30" t="s">
         <v>159</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Pat The Bunny - Easy', 'Pat The Bunny', 'Easy', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music/indie/Pat The Bunny - Easy', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Pat The Bunny - Easy', 'Pat The Bunny', 'Easy', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music\indie\Pat The Bunny - Easy.mp3', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3738,14 +3730,14 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Pat The Bunny - Hard</v>
+        <v>music\indie\Pat The Bunny - Hard.mp3</v>
       </c>
       <c r="H31" t="s">
         <v>159</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Pat The Bunny - Hard', 'Pat The Bunny', 'Hard', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music/indie/Pat The Bunny - Hard', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Pat The Bunny - Hard', 'Pat The Bunny', 'Hard', 'From Here To Utopia', 'Pat The Bunny', 'Indie', 'music\indie\Pat The Bunny - Hard.mp3', 'https://www.youtube.com/embed/YTpFLcR1PCw?si=Jiuj-JZaMyetwkou');</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3769,14 +3761,14 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Perma - Easy</v>
+        <v>music\indie\Perma - Easy.mp3</v>
       </c>
       <c r="H32" t="s">
         <v>170</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Perma - Easy', 'Perma', 'Easy', 'Little Light', 'Perma', 'Indie', 'music/indie/Perma - Easy', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Perma - Easy', 'Perma', 'Easy', 'Little Light', 'Perma', 'Indie', 'music\indie\Perma - Easy.mp3', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3800,14 +3792,14 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Perma - Hard</v>
+        <v>music\indie\Perma - Hard.mp3</v>
       </c>
       <c r="H33" t="s">
         <v>170</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Perma - Hard', 'Perma', 'Hard', 'Little Light', 'Perma', 'Indie', 'music/indie/Perma - Hard', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Perma - Hard', 'Perma', 'Hard', 'Little Light', 'Perma', 'Indie', 'music\indie\Perma - Hard.mp3', 'https://www.youtube.com/embed/NWa-JHsOJ9g?si=VV69n60jF29oy3a2');</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3831,14 +3823,14 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Sorority Noise - Easy</v>
+        <v>music\indie\Sorority Noise - Easy.mp3</v>
       </c>
       <c r="H34" t="s">
         <v>179</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Sorority Noise - Easy', 'Sorority Noise', 'Easy', 'No Halo', 'Sorority Noise', 'Indie', 'music/indie/Sorority Noise - Easy', 'https://www.youtube.com/embed/BSk8kY_rcrk?si=hMC-v7LEjTWEOj_P');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Sorority Noise - Easy', 'Sorority Noise', 'Easy', 'No Halo', 'Sorority Noise', 'Indie', 'music\indie\Sorority Noise - Easy.mp3', 'https://www.youtube.com/embed/BSk8kY_rcrk?si=hMC-v7LEjTWEOj_P');</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3862,14 +3854,14 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/Sorority Noise - Hard</v>
+        <v>music\indie\Sorority Noise - Hard.mp3</v>
       </c>
       <c r="H35" t="s">
         <v>179</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Sorority Noise - Hard', 'Sorority Noise', 'Hard', 'No Halo', 'Sorority Noise', 'Indie', 'music/indie/Sorority Noise - Hard', 'https://www.youtube.com/embed/BSk8kY_rcrk?si=hMC-v7LEjTWEOj_P');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Sorority Noise - Hard', 'Sorority Noise', 'Hard', 'No Halo', 'Sorority Noise', 'Indie', 'music\indie\Sorority Noise - Hard.mp3', 'https://www.youtube.com/embed/BSk8kY_rcrk?si=hMC-v7LEjTWEOj_P');</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3893,14 +3885,14 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Front Bottoms - Easy</v>
+        <v>music\indie\The Front Bottoms - Easy.mp3</v>
       </c>
       <c r="H36" t="s">
         <v>151</v>
       </c>
       <c r="I36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Front Bottoms - Easy', 'The Front Bottoms', 'Easy', 'Ginger', 'The Front Bottoms', 'Indie', 'music/indie/The Front Bottoms - Easy', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Front Bottoms - Easy', 'The Front Bottoms', 'Easy', 'Ginger', 'The Front Bottoms', 'Indie', 'music\indie\The Front Bottoms - Easy.mp3', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3924,14 +3916,14 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Front Bottoms - Hard</v>
+        <v>music\indie\The Front Bottoms - Hard.mp3</v>
       </c>
       <c r="H37" t="s">
         <v>151</v>
       </c>
       <c r="I37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Front Bottoms - Hard', 'The Front Bottoms', 'Hard', 'Ginger', 'The Front Bottoms', 'Indie', 'music/indie/The Front Bottoms - Hard', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Front Bottoms - Hard', 'The Front Bottoms', 'Hard', 'Ginger', 'The Front Bottoms', 'Indie', 'music\indie\The Front Bottoms - Hard.mp3', 'https://www.youtube.com/embed/Dz1SQQxLQtg?si=gH8KglYlaLDZ_qwq');</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3955,14 +3947,14 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Mountain Goats - Easy</v>
+        <v>music\indie\The Mountain Goats - Easy.mp3</v>
       </c>
       <c r="H38" t="s">
         <v>134</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Mountain Goats - Easy', 'The Mountain Goats', 'Easy', 'Autoclave', 'The Mountain Goats', 'Indie', 'music/indie/The Mountain Goats - Easy', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Mountain Goats - Easy', 'The Mountain Goats', 'Easy', 'Autoclave', 'The Mountain Goats', 'Indie', 'music\indie\The Mountain Goats - Easy.mp3', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3986,14 +3978,14 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Mountain Goats - Hard</v>
+        <v>music\indie\The Mountain Goats - Hard.mp3</v>
       </c>
       <c r="H39" t="s">
         <v>134</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Mountain Goats - Hard', 'The Mountain Goats', 'Hard', 'Autoclave', 'The Mountain Goats', 'Indie', 'music/indie/The Mountain Goats - Hard', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Mountain Goats - Hard', 'The Mountain Goats', 'Hard', 'Autoclave', 'The Mountain Goats', 'Indie', 'music\indie\The Mountain Goats - Hard.mp3', 'https://www.youtube.com/embed/BO0RPit2-rQ?si=YP5o5hmYoeVh90lE');</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4017,14 +4009,14 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Shins - Easy</v>
+        <v>music\indie\The Shins - Easy.mp3</v>
       </c>
       <c r="H40" t="s">
         <v>165</v>
       </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Shins - Easy', 'The Shins', 'Easy', 'Simple Song', 'The Shins', 'Indie', 'music/indie/The Shins - Easy', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Shins - Easy', 'The Shins', 'Easy', 'Simple Song', 'The Shins', 'Indie', 'music\indie\The Shins - Easy.mp3', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4048,14 +4040,14 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Shins - Hard</v>
+        <v>music\indie\The Shins - Hard.mp3</v>
       </c>
       <c r="H41" t="s">
         <v>165</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Shins - Hard', 'The Shins', 'Hard', 'Simple Song', 'The Shins', 'Indie', 'music/indie/The Shins - Hard', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Shins - Hard', 'The Shins', 'Hard', 'Simple Song', 'The Shins', 'Indie', 'music\indie\The Shins - Hard.mp3', 'https://www.youtube.com/embed/GyAJ4V06izg?si=7h1uVCC0UDxYWOzL');</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4079,14 +4071,14 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Thermals - Easy</v>
+        <v>music\indie\The Thermals - Easy.mp3</v>
       </c>
       <c r="H42" t="s">
         <v>143</v>
       </c>
       <c r="I42" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Thermals - Easy', 'The Thermals', 'Easy', 'Born to Kill', 'The Thermals', 'Indie', 'music/indie/The Thermals - Easy', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Thermals - Easy', 'The Thermals', 'Easy', 'Born to Kill', 'The Thermals', 'Indie', 'music\indie\The Thermals - Easy.mp3', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4110,14 +4102,14 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>music/indie/The Thermals - Hard</v>
+        <v>music\indie\The Thermals - Hard.mp3</v>
       </c>
       <c r="H43" t="s">
         <v>143</v>
       </c>
       <c r="I43" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Thermals - Hard', 'The Thermals', 'Hard', 'Born to Kill', 'The Thermals', 'Indie', 'music/indie/The Thermals - Hard', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Thermals - Hard', 'The Thermals', 'Hard', 'Born to Kill', 'The Thermals', 'Indie', 'music\indie\The Thermals - Hard.mp3', 'https://www.youtube.com/embed/cLlonHZP9Fk?si=27w6JvGmLIpRy5Eb');</v>
       </c>
     </row>
   </sheetData>
@@ -4134,8 +4126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F96BC2-62DB-49FB-AD78-FA2CCE8FE0BD}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="I38" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4180,7 +4172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>356</v>
       </c>
@@ -4200,15 +4192,15 @@
         <v>240</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G43" si="0">"music/"&amp;LOWER(F2)&amp;"/"&amp;A2</f>
-        <v>music/video games/Civilisation IV - Easy</v>
+        <f>"music\"&amp;LOWER(F2)&amp;"\"&amp;A2&amp;".mp3"</f>
+        <v>music\video games\Civilisation IV - Easy.mp3</v>
       </c>
       <c r="H2" t="s">
         <v>334</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" ref="I2:I43" si="1">"INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Civilisation IV - Easy', 'Civilisation IV', 'Easy', 'Baba Yetu', 'Christopher Tin', 'Video Games', 'music/video games/Civilisation IV - Easy', 'https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx');</v>
+        <f>"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A2&amp;"'"&amp;", "&amp;"'"&amp;B2&amp;"'"&amp;", "&amp;"'"&amp;C2&amp;"'"&amp;", "&amp;"'"&amp;D2&amp;"'"&amp;", "&amp;"'"&amp;E2&amp;"'"&amp;", "&amp;"'"&amp;F2&amp;"'"&amp;", "&amp;"'"&amp;G2&amp;"', "&amp;"'"&amp;H2&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Civilisation IV - Easy', 'Civilisation IV', 'Easy', 'Baba Yetu', 'Christopher Tin', 'Video Games', 'music\video games\Civilisation IV - Easy.mp3', 'https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx');</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4231,15 +4223,15 @@
         <v>240</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="0"/>
-        <v>music/video games/Civilisation IV - Hard</v>
+        <f t="shared" ref="G3:G43" si="0">"music\"&amp;LOWER(F3)&amp;"\"&amp;A3&amp;".mp3"</f>
+        <v>music\video games\Civilisation IV - Hard.mp3</v>
       </c>
       <c r="H3" t="s">
         <v>334</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Civilisation IV - Hard', 'Civilisation IV', 'Hard', 'Baba Yetu', 'Christopher Tin', 'Video Games', 'music/video games/Civilisation IV - Hard', 'https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx');</v>
+        <f t="shared" ref="I3:I43" si="1">"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Civilisation IV - Hard', 'Civilisation IV', 'Hard', 'Baba Yetu', 'Christopher Tin', 'Video Games', 'music\video games\Civilisation IV - Hard.mp3', 'https://www.youtube.com/embed/5e0Qelqp-Cc?si=M20JmfUyT2sfHPsx');</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4263,14 +4255,14 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Code Vein - Easy</v>
+        <v>music\video games\Code Vein - Easy.mp3</v>
       </c>
       <c r="H4" t="s">
         <v>303</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Vein - Easy', 'Code Vein', 'Easy', 'Requiem', 'Go Shiina', 'Video Games', 'music/video games/Code Vein - Easy', 'https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Code Vein - Easy', 'Code Vein', 'Easy', 'Requiem', 'Go Shiina', 'Video Games', 'music\video games\Code Vein - Easy.mp3', 'https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k');</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4294,17 +4286,17 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Code Vein - Hard</v>
+        <v>music\video games\Code Vein - Hard.mp3</v>
       </c>
       <c r="H5" t="s">
         <v>303</v>
       </c>
       <c r="I5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Code Vein - Hard', 'Code Vein', 'Hard', 'Requiem', 'Go Shiina', 'Video Games', 'music/video games/Code Vein - Hard', 'https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Code Vein - Hard', 'Code Vein', 'Hard', 'Requiem', 'Go Shiina', 'Video Games', 'music\video games\Code Vein - Hard.mp3', 'https://www.youtube.com/embed/xfBF1SGOJiY?si=mEq7r1aHnepCsh3k');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>274</v>
       </c>
@@ -4325,17 +4317,17 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Cyberpunk 2077 - Easy</v>
+        <v>music\video games\Cyberpunk 2077 - Easy.mp3</v>
       </c>
       <c r="H6" t="s">
         <v>277</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Cyberpunk 2077 - Easy', 'Cyberpunk 2077', 'Easy', 'I Really Want To Stay At Your House', 'Rosa Walton &amp; Hallie Coggins', 'Video Games', 'music/video games/Cyberpunk 2077 - Easy', 'https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Cyberpunk 2077 - Easy', 'Cyberpunk 2077', 'Easy', 'I Really Want To Stay At Your House', 'Rosa Walton &amp; Hallie Coggins', 'Video Games', 'music\video games\Cyberpunk 2077 - Easy.mp3', 'https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>274</v>
       </c>
@@ -4356,14 +4348,14 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Cyberpunk 2077 - Easy</v>
+        <v>music\video games\Cyberpunk 2077 - Easy.mp3</v>
       </c>
       <c r="H7" t="s">
         <v>277</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Cyberpunk 2077 - Easy', 'Cyberpunk 2077', 'Hard', 'I Really Want To Stay At Your House', 'Rosa Walton &amp; Hallie Coggins', 'Video Games', 'music/video games/Cyberpunk 2077 - Easy', 'https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Cyberpunk 2077 - Easy', 'Cyberpunk 2077', 'Hard', 'I Really Want To Stay At Your House', 'Rosa Walton &amp; Hallie Coggins', 'Video Games', 'music\video games\Cyberpunk 2077 - Easy.mp3', 'https://www.youtube.com/embed/gzbLODUb1sA?si=tTdlOTbFJLIbBFsl');</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4387,14 +4379,14 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Dark Souls - Easy</v>
+        <v>music\video games\Dark Souls - Easy.mp3</v>
       </c>
       <c r="H8" t="s">
         <v>313</v>
       </c>
       <c r="I8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dark Souls - Easy', 'Dark Souls', 'Easy', 'Ornstein &amp; Smough', 'Motoi Sakuraba', 'Video Games', 'music/video games/Dark Souls - Easy', 'https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Dark Souls - Easy', 'Dark Souls', 'Easy', 'Ornstein &amp; Smough', 'Motoi Sakuraba', 'Video Games', 'music\video games\Dark Souls - Easy.mp3', 'https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q');</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4418,14 +4410,14 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Dark Souls - Hard</v>
+        <v>music\video games\Dark Souls - Hard.mp3</v>
       </c>
       <c r="H9" t="s">
         <v>313</v>
       </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Dark Souls - Hard', 'Dark Souls', 'Hard', 'Ornstein &amp; Smough', 'Motoi Sakuraba', 'Video Games', 'music/video games/Dark Souls - Hard', 'https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Dark Souls - Hard', 'Dark Souls', 'Hard', 'Ornstein &amp; Smough', 'Motoi Sakuraba', 'Video Games', 'music\video games\Dark Souls - Hard.mp3', 'https://www.youtube.com/embed/Nsps0I58yUM?si=xQD3dUE4olSvED7Q');</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4449,14 +4441,14 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Final Fantasy IX - Easy</v>
+        <v>music\video games\Final Fantasy IX - Easy.mp3</v>
       </c>
       <c r="H10" t="s">
         <v>300</v>
       </c>
       <c r="I10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy IX - Easy', 'Final Fantasy IX', 'Easy', 'Melodies of Life', 'Emiko Shiratori', 'Video Games', 'music/video games/Final Fantasy IX - Easy', 'https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy IX - Easy', 'Final Fantasy IX', 'Easy', 'Melodies of Life', 'Emiko Shiratori', 'Video Games', 'music\video games\Final Fantasy IX - Easy.mp3', 'https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-');</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4480,14 +4472,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Final Fantasy IX - Hard</v>
+        <v>music\video games\Final Fantasy IX - Hard.mp3</v>
       </c>
       <c r="H11" t="s">
         <v>300</v>
       </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy IX - Hard', 'Final Fantasy IX', 'Hard', 'Melodies of Life', 'Emiko Shiratori', 'Video Games', 'music/video games/Final Fantasy IX - Hard', 'https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy IX - Hard', 'Final Fantasy IX', 'Hard', 'Melodies of Life', 'Emiko Shiratori', 'Video Games', 'music\video games\Final Fantasy IX - Hard.mp3', 'https://www.youtube.com/embed/Ye7BGnlTZmQ?si=yeEJI5luiQRazYF-');</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4511,14 +4503,14 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Final Fantasy VII - Easy</v>
+        <v>music\video games\Final Fantasy VII - Easy.mp3</v>
       </c>
       <c r="H12" t="s">
         <v>350</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy VII - Easy', 'Final Fantasy VII', 'Easy', 'One Winged Angel', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy VII - Easy', 'https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy VII - Easy', 'Final Fantasy VII', 'Easy', 'One Winged Angel', 'Nobuo Uematsu', 'Video Games', 'music\video games\Final Fantasy VII - Easy.mp3', 'https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv');</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4542,14 +4534,14 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Final Fantasy VII - Hard</v>
+        <v>music\video games\Final Fantasy VII - Hard.mp3</v>
       </c>
       <c r="H13" t="s">
         <v>350</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy VII - Hard', 'Final Fantasy VII', 'Hard', 'One Winged Angel', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy VII - Hard', 'https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy VII - Hard', 'Final Fantasy VII', 'Hard', 'One Winged Angel', 'Nobuo Uematsu', 'Video Games', 'music\video games\Final Fantasy VII - Hard.mp3', 'https://www.youtube.com/embed/mYdf0yqK_Fc?si=xSaZJiGFa4XPVusv');</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4573,14 +4565,14 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Final Fantasy X - Easy</v>
+        <v>music\video games\Final Fantasy X - Easy.mp3</v>
       </c>
       <c r="H14" t="s">
         <v>343</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy X - Easy', 'Final Fantasy X', 'Easy', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy X - Easy', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy X - Easy', 'Final Fantasy X', 'Easy', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music\video games\Final Fantasy X - Easy.mp3', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4604,17 +4596,17 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Final Fantasy X - Hard</v>
+        <v>music\video games\Final Fantasy X - Hard.mp3</v>
       </c>
       <c r="H15" t="s">
         <v>343</v>
       </c>
       <c r="I15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Final Fantasy X - Hard', 'Final Fantasy X', 'Hard', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music/video games/Final Fantasy X - Hard', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy X - Hard', 'Final Fantasy X', 'Hard', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music\video games\Final Fantasy X - Hard.mp3', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>284</v>
       </c>
@@ -4635,17 +4627,17 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Fire Emblem Three Houses - Easy</v>
+        <v>music\video games\Fire Emblem Three Houses - Easy.mp3</v>
       </c>
       <c r="H16" t="s">
         <v>286</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Easy', 'Fire Emblem Three Houses', 'Easy', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music/video games/Fire Emblem Three Houses - Easy', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Easy', 'Fire Emblem Three Houses', 'Easy', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music\video games\Fire Emblem Three Houses - Easy.mp3', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>285</v>
       </c>
@@ -4666,14 +4658,14 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Fire Emblem Three Houses - Hard</v>
+        <v>music\video games\Fire Emblem Three Houses - Hard.mp3</v>
       </c>
       <c r="H17" t="s">
         <v>286</v>
       </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Hard', 'Fire Emblem Three Houses', 'Hard', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music/video games/Fire Emblem Three Houses - Hard', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Hard', 'Fire Emblem Three Houses', 'Hard', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music\video games\Fire Emblem Three Houses - Hard.mp3', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4697,14 +4689,14 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Kingdom Hearts - Easy</v>
+        <v>music\video games\Kingdom Hearts - Easy.mp3</v>
       </c>
       <c r="H18" t="s">
         <v>337</v>
       </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Kingdom Hearts - Easy', 'Kingdom Hearts', 'Easy', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music/video games/Kingdom Hearts - Easy', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Kingdom Hearts - Easy', 'Kingdom Hearts', 'Easy', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music\video games\Kingdom Hearts - Easy.mp3', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4728,17 +4720,17 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Kingdom Hearts - Hard</v>
+        <v>music\video games\Kingdom Hearts - Hard.mp3</v>
       </c>
       <c r="H19" t="s">
         <v>337</v>
       </c>
       <c r="I19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Kingdom Hearts - Hard', 'Kingdom Hearts', 'Hard', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music/video games/Kingdom Hearts - Hard', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Kingdom Hearts - Hard', 'Kingdom Hearts', 'Hard', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music\video games\Kingdom Hearts - Hard.mp3', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>280</v>
       </c>
@@ -4759,17 +4751,17 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Metal Gear Rising - Easy</v>
+        <v>music\video games\Metal Gear Rising - Easy.mp3</v>
       </c>
       <c r="H20" t="s">
         <v>282</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Metal Gear Rising - Easy', 'Metal Gear Rising', 'Easy', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music/video games/Metal Gear Rising - Easy', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Metal Gear Rising - Easy', 'Metal Gear Rising', 'Easy', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music\video games\Metal Gear Rising - Easy.mp3', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>281</v>
       </c>
@@ -4790,14 +4782,14 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Metal Gear Rising - Hard</v>
+        <v>music\video games\Metal Gear Rising - Hard.mp3</v>
       </c>
       <c r="H21" t="s">
         <v>282</v>
       </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Metal Gear Rising - Hard', 'Metal Gear Rising', 'Hard', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music/video games/Metal Gear Rising - Hard', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Metal Gear Rising - Hard', 'Metal Gear Rising', 'Hard', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music\video games\Metal Gear Rising - Hard.mp3', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4821,14 +4813,14 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Outer Wilds - Easy</v>
+        <v>music\video games\Outer Wilds - Easy.mp3</v>
       </c>
       <c r="H22" t="s">
         <v>253</v>
       </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Outer Wilds - Easy', 'Outer Wilds', 'Easy', '14.3 Billion Years', 'Andrew Prahlow', 'Video Games', 'music/video games/Outer Wilds - Easy', 'https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Outer Wilds - Easy', 'Outer Wilds', 'Easy', '14.3 Billion Years', 'Andrew Prahlow', 'Video Games', 'music\video games\Outer Wilds - Easy.mp3', 'https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0');</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4852,14 +4844,14 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Outer Wilds - Hard</v>
+        <v>music\video games\Outer Wilds - Hard.mp3</v>
       </c>
       <c r="H23" t="s">
         <v>253</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Outer Wilds - Hard', 'Outer Wilds', 'Hard', '14.3 Billion Years', 'Andrew Prahlow', 'Video Games', 'music/video games/Outer Wilds - Hard', 'https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Outer Wilds - Hard', 'Outer Wilds', 'Hard', '14.3 Billion Years', 'Andrew Prahlow', 'Video Games', 'music\video games\Outer Wilds - Hard.mp3', 'https://www.youtube.com/embed/XOrygf_iLhw?si=aLNfbxiTuwz1X_X0');</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4883,14 +4875,14 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 3 - Easy</v>
+        <v>music\video games\Persona 3 - Easy.mp3</v>
       </c>
       <c r="H24" t="s">
         <v>309</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 3 - Easy', 'Persona 3', 'Easy', 'Mass Destruction', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 3 - Easy', 'https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Persona 3 - Easy', 'Persona 3', 'Easy', 'Mass Destruction', 'Shoji Meguro', 'Video Games', 'music\video games\Persona 3 - Easy.mp3', 'https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C');</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4914,14 +4906,14 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 3 - Hard</v>
+        <v>music\video games\Persona 3 - Hard.mp3</v>
       </c>
       <c r="H25" t="s">
         <v>309</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 3 - Hard', 'Persona 3', 'Hard', 'Mass Destruction', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 3 - Hard', 'https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Persona 3 - Hard', 'Persona 3', 'Hard', 'Mass Destruction', 'Shoji Meguro', 'Video Games', 'music\video games\Persona 3 - Hard.mp3', 'https://www.youtube.com/embed/6jFaoLrLzd4?si=kgHXTSzUFm9Oyb9C');</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4945,14 +4937,14 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 4 - Easy</v>
+        <v>music\video games\Persona 4 - Easy.mp3</v>
       </c>
       <c r="H26" t="s">
         <v>295</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 4 - Easy', 'Persona 4', 'Easy', 'Heaven', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 4 - Easy', 'https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Persona 4 - Easy', 'Persona 4', 'Easy', 'Heaven', 'Shoji Meguro', 'Video Games', 'music\video games\Persona 4 - Easy.mp3', 'https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u');</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -4976,14 +4968,14 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 4 - Hard</v>
+        <v>music\video games\Persona 4 - Hard.mp3</v>
       </c>
       <c r="H27" t="s">
         <v>295</v>
       </c>
       <c r="I27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 4 - Hard', 'Persona 4', 'Hard', 'Heaven', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 4 - Hard', 'https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Persona 4 - Hard', 'Persona 4', 'Hard', 'Heaven', 'Shoji Meguro', 'Video Games', 'music\video games\Persona 4 - Hard.mp3', 'https://www.youtube.com/embed/0d9Oqm0Dt60?si=g4ESFZp6SrrEJq4u');</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5007,14 +4999,14 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 5 - Easy</v>
+        <v>music\video games\Persona 5 - Easy.mp3</v>
       </c>
       <c r="H28" t="s">
         <v>241</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Easy', 'Persona 5', 'Easy', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Easy', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Persona 5 - Easy', 'Persona 5', 'Easy', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music\video games\Persona 5 - Easy.mp3', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5038,14 +5030,14 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Persona 5 - Hard</v>
+        <v>music\video games\Persona 5 - Hard.mp3</v>
       </c>
       <c r="H29" t="s">
         <v>241</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Persona 5 - Hard', 'Persona 5', 'Hard', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music/video games/Persona 5 - Hard', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Persona 5 - Hard', 'Persona 5', 'Hard', 'Last Surprise', 'Shoji Meguro', 'Video Games', 'music\video games\Persona 5 - Hard.mp3', 'https://www.youtube.com/embed/Ec4YbVP9R-A?si=0e-P9iwxDCMkviKH');</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5069,14 +5061,14 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Shadow Of The Colossus - Easy</v>
+        <v>music\video games\Shadow Of The Colossus - Easy.mp3</v>
       </c>
       <c r="H30" t="s">
         <v>331</v>
       </c>
       <c r="I30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Easy', 'Prologue', 'Kō Ōtani', 'Video Games', 'music/video games/Shadow Of The Colossus - Easy', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Easy', 'Prologue', 'Kō Ōtani', 'Video Games', 'music\video games\Shadow Of The Colossus - Easy.mp3', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5100,17 +5092,17 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Shadow Of The Colossus - Easy</v>
+        <v>music\video games\Shadow Of The Colossus - Easy.mp3</v>
       </c>
       <c r="H31" t="s">
         <v>331</v>
       </c>
       <c r="I31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Hard', 'Prologue', 'Kō Ōtani', 'Video Games', 'music/video games/Shadow Of The Colossus - Easy', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Hard', 'Prologue', 'Kō Ōtani', 'Video Games', 'music\video games\Shadow Of The Colossus - Easy.mp3', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>291</v>
       </c>
@@ -5131,17 +5123,17 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Shin Megami Tensei III Nocturne - Easy</v>
+        <v>music\video games\Shin Megami Tensei III Nocturne - Easy.mp3</v>
       </c>
       <c r="H32" t="s">
         <v>289</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Easy', 'Shin Megami Tensei III Nocturne', 'Easy', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music/video games/Shin Megami Tensei III Nocturne - Easy', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Easy', 'Shin Megami Tensei III Nocturne', 'Easy', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music\video games\Shin Megami Tensei III Nocturne - Easy.mp3', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>292</v>
       </c>
@@ -5162,17 +5154,17 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Shin Megami Tensei III Nocturne - Hard</v>
+        <v>music\video games\Shin Megami Tensei III Nocturne - Hard.mp3</v>
       </c>
       <c r="H33" t="s">
         <v>289</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Hard', 'Shin Megami Tensei III Nocturne', 'Hard', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music/video games/Shin Megami Tensei III Nocturne - Hard', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Hard', 'Shin Megami Tensei III Nocturne', 'Hard', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music\video games\Shin Megami Tensei III Nocturne - Hard.mp3', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>317</v>
       </c>
@@ -5193,17 +5185,17 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Shin Megami Tensei V - Easy</v>
+        <v>music\video games\Shin Megami Tensei V - Easy.mp3</v>
       </c>
       <c r="H34" t="s">
         <v>315</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei V - Easy', 'Shin Megami Tensei V', 'Easy', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music/video games/Shin Megami Tensei V - Easy', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei V - Easy', 'Shin Megami Tensei V', 'Easy', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music\video games\Shin Megami Tensei V - Easy.mp3', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>319</v>
       </c>
@@ -5224,14 +5216,14 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Shin Megami Tensei V - Hard</v>
+        <v>music\video games\Shin Megami Tensei V - Hard.mp3</v>
       </c>
       <c r="H35" t="s">
         <v>315</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Shin Megami Tensei V - Hard', 'Shin Megami Tensei V', 'Hard', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music/video games/Shin Megami Tensei V - Hard', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei V - Hard', 'Shin Megami Tensei V', 'Hard', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music\video games\Shin Megami Tensei V - Hard.mp3', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5255,14 +5247,14 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Silent Hill 2 - Easy</v>
+        <v>music\video games\Silent Hill 2 - Easy.mp3</v>
       </c>
       <c r="H36" t="s">
         <v>327</v>
       </c>
       <c r="I36" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Silent Hill 2 - Easy', 'Silent Hill 2', 'Easy', 'Theme Of Laura', 'Akira Yamaoka', 'Video Games', 'music/video games/Silent Hill 2 - Easy', 'https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Silent Hill 2 - Easy', 'Silent Hill 2', 'Easy', 'Theme Of Laura', 'Akira Yamaoka', 'Video Games', 'music\video games\Silent Hill 2 - Easy.mp3', 'https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E');</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5286,14 +5278,14 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Silent Hill 2 - Hard</v>
+        <v>music\video games\Silent Hill 2 - Hard.mp3</v>
       </c>
       <c r="H37" t="s">
         <v>327</v>
       </c>
       <c r="I37" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Silent Hill 2 - Hard', 'Silent Hill 2', 'Hard', 'Theme Of Laura', 'Akira Yamaoka', 'Video Games', 'music/video games/Silent Hill 2 - Hard', 'https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Silent Hill 2 - Hard', 'Silent Hill 2', 'Hard', 'Theme Of Laura', 'Akira Yamaoka', 'Video Games', 'music\video games\Silent Hill 2 - Hard.mp3', 'https://www.youtube.com/embed/6LB7LZZGpkw?si=unm8x14F1AcOVE3E');</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5317,14 +5309,14 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Stardew Valley - Easy</v>
+        <v>music\video games\Stardew Valley - Easy.mp3</v>
       </c>
       <c r="H38" t="s">
         <v>320</v>
       </c>
       <c r="I38" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Stardew Valley - Easy', 'Stardew Valley', 'Easy', 'Spring (The Valley Comes Alive)', 'Eric Barone', 'Video Games', 'music/video games/Stardew Valley - Easy', 'https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Stardew Valley - Easy', 'Stardew Valley', 'Easy', 'Spring (The Valley Comes Alive)', 'Eric Barone', 'Video Games', 'music\video games\Stardew Valley - Easy.mp3', 'https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf');</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5348,14 +5340,14 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Stardew Valley - Hard</v>
+        <v>music\video games\Stardew Valley - Hard.mp3</v>
       </c>
       <c r="H39" t="s">
         <v>320</v>
       </c>
       <c r="I39" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Stardew Valley - Hard', 'Stardew Valley', 'Hard', 'Spring (The Valley Comes Alive)', 'Eric Barone', 'Video Games', 'music/video games/Stardew Valley - Hard', 'https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Stardew Valley - Hard', 'Stardew Valley', 'Hard', 'Spring (The Valley Comes Alive)', 'Eric Barone', 'Video Games', 'music\video games\Stardew Valley - Hard.mp3', 'https://www.youtube.com/embed/fI9QzlD_sm0?si=21Qxj3ocPy1OrrZf');</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5379,14 +5371,14 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Subnautica - Easy</v>
+        <v>music\video games\Subnautica - Easy.mp3</v>
       </c>
       <c r="H40" t="s">
         <v>324</v>
       </c>
       <c r="I40" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Easy', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music/video games/Subnautica - Easy', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Easy', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music\video games\Subnautica - Easy.mp3', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5410,14 +5402,14 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/Subnautica - Easy</v>
+        <v>music\video games\Subnautica - Easy.mp3</v>
       </c>
       <c r="H41" t="s">
         <v>324</v>
       </c>
       <c r="I41" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Hard', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music/video games/Subnautica - Easy', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Hard', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music\video games\Subnautica - Easy.mp3', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5441,14 +5433,14 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/The Elder Scrolls V Skyrim - Easy</v>
+        <v>music\video games\The Elder Scrolls V Skyrim - Easy.mp3</v>
       </c>
       <c r="H42" t="s">
         <v>349</v>
       </c>
       <c r="I42" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Easy', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music/video games/The Elder Scrolls V Skyrim - Easy', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Easy', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music\video games\The Elder Scrolls V Skyrim - Easy.mp3', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5472,14 +5464,14 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>music/video games/The Elder Scrolls V Skyrim - Easy</v>
+        <v>music\video games\The Elder Scrolls V Skyrim - Easy.mp3</v>
       </c>
       <c r="H43" t="s">
         <v>349</v>
       </c>
       <c r="I43" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, arist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Hard', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music/video games/The Elder Scrolls V Skyrim - Easy', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Hard', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music\video games\The Elder Scrolls V Skyrim - Easy.mp3', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding tv show tracks
</commit_message>
<xml_diff>
--- a/SQL.xlsx
+++ b/SQL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Web Development Projects\Personal Projects\Online Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342998C0-D620-466D-B011-82BB96099BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61519729-5C1F-4EF9-9AF2-380296C065F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5130" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anime" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="434">
   <si>
     <t>Name</t>
   </si>
@@ -1203,6 +1211,135 @@
   </si>
   <si>
     <t>https://www.youtube.com/embed/6F1QNfmiqHc?si=VL8NmgNNRHDnaJqC</t>
+  </si>
+  <si>
+    <t>Game of Thrones - Easy</t>
+  </si>
+  <si>
+    <t>Futurama - Easy</t>
+  </si>
+  <si>
+    <t>Futurama - Hard</t>
+  </si>
+  <si>
+    <t>Game of Thrones - Hard</t>
+  </si>
+  <si>
+    <t>Game of Thrones</t>
+  </si>
+  <si>
+    <t>Game of Thrones Theme</t>
+  </si>
+  <si>
+    <t>Ramin Djawadi</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/s7L2PVdrb_8?si=yiFJ25qmae4KlKRY</t>
+  </si>
+  <si>
+    <t>Fringe</t>
+  </si>
+  <si>
+    <t>Fringe - Easy</t>
+  </si>
+  <si>
+    <t>Fringe - Hard</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/c4Vvs_JAh04?si=BZFkWxo86XrR3T0Z</t>
+  </si>
+  <si>
+    <t>J.J. Abrams</t>
+  </si>
+  <si>
+    <t>Fringe Main Title Theme</t>
+  </si>
+  <si>
+    <t>Doctor Who - Easy</t>
+  </si>
+  <si>
+    <t>Doctor Who - Hard</t>
+  </si>
+  <si>
+    <t>Doctor Who</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/sWuAt0swt7k?si=mRqECVYwk5nMnkP2</t>
+  </si>
+  <si>
+    <t>Ron Grainer</t>
+  </si>
+  <si>
+    <t>Doctor Who Theme</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/vpAol_17mO0?si=RNiARjVBLEtpGGv0</t>
+  </si>
+  <si>
+    <t>Angel - Easy</t>
+  </si>
+  <si>
+    <t>Angel - Hard</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Darling Violetta</t>
+  </si>
+  <si>
+    <t>The Sanctuary</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/1nCqRmx3Dnw?si=eJpPAceg6sOQwkuG</t>
+  </si>
+  <si>
+    <t>The Fresh Prince of Bel Air</t>
+  </si>
+  <si>
+    <t>The Fresh Prince of Bel Air - Easy</t>
+  </si>
+  <si>
+    <t>The Fresh Prince of Bel Air - Hard</t>
+  </si>
+  <si>
+    <t>Yo Home to Bel-Air</t>
+  </si>
+  <si>
+    <t>DJ Jazzy Jeff &amp; Will Smith</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/b4T1M5C6MUY?si=5y2gVU6xsDynFbes</t>
+  </si>
+  <si>
+    <t>What We Do In The Shadows</t>
+  </si>
+  <si>
+    <t>What We Do In The Shadows - Easy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/ATRgllo_9aE?si=ewcgOFR464d0BvpC</t>
+  </si>
+  <si>
+    <t>Chuck - Easy</t>
+  </si>
+  <si>
+    <t>Chuck - Hard</t>
+  </si>
+  <si>
+    <t>Chuck</t>
+  </si>
+  <si>
+    <t>Short Skirt / Long Jacket</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>You're Dead</t>
+  </si>
+  <si>
+    <t>Norma Tanega</t>
   </si>
 </sst>
 </file>
@@ -1263,9 +1400,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3637,7 +3774,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Mewithoutyou - Easy', 'Mewithoutyou', 'Easy', 'Messes of Men', 'Mewithoutyou', 'Indie', 'music\indie\Mewithoutyou - Easy.mp3', 'https://www.youtube.com/embed/qN_j1bz3i4s?si=1QYUAVgNrQmhD_MV');</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -4720,7 +4857,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Final Fantasy X - Hard', 'Final Fantasy X', 'Hard', 'To Zanarkand', 'Nobuo Uematsu', 'Video Games', 'music\video games\Final Fantasy X - Hard.mp3', 'https://www.youtube.com/embed/6fp81GzKarQ?si=fvwACNCjrosghv8f');</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>284</v>
       </c>
@@ -4751,7 +4888,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fire Emblem Three Houses - Easy', 'Fire Emblem Three Houses', 'Easy', 'Edge Of Dawn', 'Takeru Kanazaki', 'Video Games', 'music\video games\Fire Emblem Three Houses - Easy.mp3', 'https://www.youtube.com/embed/FSXuM2v0YLY?si=KlMT97qL7LZSGX1P');</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>285</v>
       </c>
@@ -4844,7 +4981,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Kingdom Hearts - Hard', 'Kingdom Hearts', 'Hard', 'Dearly Beloved', 'Yoko Shimomura', 'Video Games', 'music\video games\Kingdom Hearts - Hard.mp3', 'https://www.youtube.com/embed/Jk4P10nsq4c?si=owgNpSU1U9HPoG6J');</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>280</v>
       </c>
@@ -4875,7 +5012,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Metal Gear Rising - Easy', 'Metal Gear Rising', 'Easy', 'The Only Thing I Know For Real', 'Jamie Christopherson', 'Video Games', 'music\video games\Metal Gear Rising - Easy.mp3', 'https://www.youtube.com/embed/ZDupR9FXwCU?si=pGWWJUz0kaFVJrQw');</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>281</v>
       </c>
@@ -5216,7 +5353,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shadow Of The Colossus - Easy', 'Shadow Of The Colossus', 'Hard', 'Prologue', 'Kō Ōtani', 'Video Games', 'music\video games\Shadow Of The Colossus - Easy.mp3', 'https://www.youtube.com/embed/Pdi1DSqBZ6Q?si=aAbPNeRIURfJ8SU3');</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>291</v>
       </c>
@@ -5247,7 +5384,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Easy', 'Shin Megami Tensei III Nocturne', 'Easy', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music\video games\Shin Megami Tensei III Nocturne - Easy.mp3', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>292</v>
       </c>
@@ -5278,7 +5415,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei III Nocturne - Hard', 'Shin Megami Tensei III Nocturne', 'Hard', 'Forced Battle', 'Shoji Meguro', 'Video Games', 'music\video games\Shin Megami Tensei III Nocturne - Hard.mp3', 'https://www.youtube.com/embed/RT2ZW63KJJo?si=VTlJLTXcg2Y6g1BV');</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>317</v>
       </c>
@@ -5309,7 +5446,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Shin Megami Tensei V - Easy', 'Shin Megami Tensei V', 'Easy', 'Battle - Destruction', 'Ryota Kozuka', 'Video Games', 'music\video games\Shin Megami Tensei V - Easy.mp3', 'https://www.youtube.com/embed/NApN0GduuwM?si=s3YoeEflFm8aZWHl');</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>319</v>
       </c>
@@ -5526,7 +5663,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Subnautica - Easy', 'Subnautica', 'Hard', 'Abandon Ship', 'Simon Chylinski', 'Video Games', 'music\video games\Subnautica - Easy.mp3', 'https://www.youtube.com/embed/nf30qQzw7rk?si=rykvO-aWqeFqUyHx');</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>347</v>
       </c>
@@ -5557,7 +5694,7 @@
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Elder Scrolls V Skyrim - Easy', 'The Elder Scrolls V Skyrim', 'Easy', 'Dragonborn', 'Jeremy Soule', 'Video Games', 'music\video games\The Elder Scrolls V Skyrim - Easy.mp3', 'https://www.youtube.com/embed/5OWdMHIRld8?si=JoGTud7pVhVSrEKY');</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>347</v>
       </c>
@@ -5601,8 +5738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88789C06-C192-4D6D-A590-6AFD60FC6CAC}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5670,7 +5807,7 @@
         <f>"music\"&amp;LOWER(F2)&amp;"\"&amp;A2&amp;".mp3"</f>
         <v>music\tv shows\Breaking Bad - Easy.mp3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>361</v>
       </c>
       <c r="I2" s="1" t="str">
@@ -5698,14 +5835,14 @@
         <v>367</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G13" si="0">"music\"&amp;LOWER(F3)&amp;"\"&amp;A3&amp;".mp3"</f>
+        <f t="shared" ref="G3:G37" si="0">"music\"&amp;LOWER(F3)&amp;"\"&amp;A3&amp;".mp3"</f>
         <v>music\tv shows\Breaking Bad - Hard.mp3</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" t="s">
         <v>361</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I13" si="1">"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
+        <f t="shared" ref="I3:I37" si="1">"INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('"&amp;A3&amp;"'"&amp;", "&amp;"'"&amp;B3&amp;"'"&amp;", "&amp;"'"&amp;C3&amp;"'"&amp;", "&amp;"'"&amp;D3&amp;"'"&amp;", "&amp;"'"&amp;E3&amp;"'"&amp;", "&amp;"'"&amp;F3&amp;"'"&amp;", "&amp;"'"&amp;G3&amp;"', "&amp;"'"&amp;H3&amp;"');"</f>
         <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Breaking Bad - Hard', 'Breaking Bad', 'Hard', 'Breaking Bad Main Title Theme', 'Dave Porter', 'TV Shows', 'music\tv shows\Breaking Bad - Hard.mp3', 'https://www.youtube.com/embed/3U6PSWyv5sc?si=aWNCnkHAEkqAdZdk');</v>
       </c>
     </row>
@@ -5732,7 +5869,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Friends - Easy.mp3</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" t="s">
         <v>368</v>
       </c>
       <c r="I4" s="1" t="str">
@@ -5763,7 +5900,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Friends - Hard.mp3</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" t="s">
         <v>368</v>
       </c>
       <c r="I5" s="1" t="str">
@@ -5794,7 +5931,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Charmed - Easy.mp3</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" t="s">
         <v>369</v>
       </c>
       <c r="I6" s="1" t="str">
@@ -5825,7 +5962,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Charmed - Hard.mp3</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" t="s">
         <v>369</v>
       </c>
       <c r="I7" s="1" t="str">
@@ -5856,7 +5993,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Supernatural - Easy.mp3</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" t="s">
         <v>376</v>
       </c>
       <c r="I8" s="1" t="str">
@@ -5887,7 +6024,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Supernatural - Hard.mp3</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" t="s">
         <v>376</v>
       </c>
       <c r="I9" s="1" t="str">
@@ -5918,7 +6055,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Gilmore Girls - Easy.mp3</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" t="s">
         <v>386</v>
       </c>
       <c r="I10" s="1" t="str">
@@ -5949,7 +6086,7 @@
         <f t="shared" si="0"/>
         <v>music\tv shows\Gilmore Girls - Hard.mp3</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" t="s">
         <v>386</v>
       </c>
       <c r="I11" s="1" t="str">
@@ -5959,7 +6096,7 @@
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B12" t="s">
         <v>387</v>
@@ -5978,19 +6115,19 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>music\tv shows\Futurama.mp3</v>
-      </c>
-      <c r="H12" s="5" t="s">
+        <v>music\tv shows\Futurama - Easy.mp3</v>
+      </c>
+      <c r="H12" t="s">
         <v>390</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Futurama', 'Futurama', 'Easy', 'Futurama Theme Song', 'Christopher Tyng', 'TV Shows', 'music\tv shows\Futurama.mp3', 'https://www.youtube.com/embed/6F1QNfmiqHc?si=VL8NmgNNRHDnaJqC');</v>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Futurama - Easy', 'Futurama', 'Easy', 'Futurama Theme Song', 'Christopher Tyng', 'TV Shows', 'music\tv shows\Futurama - Easy.mp3', 'https://www.youtube.com/embed/6F1QNfmiqHc?si=VL8NmgNNRHDnaJqC');</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B13" t="s">
         <v>387</v>
@@ -6009,146 +6146,608 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>music\tv shows\Futurama.mp3</v>
-      </c>
-      <c r="H13" s="5" t="s">
+        <v>music\tv shows\Futurama - Hard.mp3</v>
+      </c>
+      <c r="H13" t="s">
         <v>390</v>
       </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Futurama', 'Futurama', 'Hard', 'Futurama Theme Song', 'Christopher Tyng', 'TV Shows', 'music\tv shows\Futurama.mp3', 'https://www.youtube.com/embed/6F1QNfmiqHc?si=VL8NmgNNRHDnaJqC');</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Futurama - Hard', 'Futurama', 'Hard', 'Futurama Theme Song', 'Christopher Tyng', 'TV Shows', 'music\tv shows\Futurama - Hard.mp3', 'https://www.youtube.com/embed/6F1QNfmiqHc?si=VL8NmgNNRHDnaJqC');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>391</v>
+      </c>
+      <c r="B14" t="s">
+        <v>395</v>
+      </c>
       <c r="C14" t="s">
         <v>67</v>
+      </c>
+      <c r="D14" t="s">
+        <v>396</v>
+      </c>
+      <c r="E14" t="s">
+        <v>397</v>
       </c>
       <c r="F14" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Game of Thrones - Easy.mp3</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Game of Thrones - Easy', 'Game of Thrones', 'Easy', 'Game of Thrones Theme', 'Ramin Djawadi', 'TV Shows', 'music\tv shows\Game of Thrones - Easy.mp3', 'https://www.youtube.com/embed/s7L2PVdrb_8?si=yiFJ25qmae4KlKRY');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B15" t="s">
+        <v>395</v>
+      </c>
       <c r="C15" t="s">
         <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>396</v>
+      </c>
+      <c r="E15" t="s">
+        <v>397</v>
       </c>
       <c r="F15" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Game of Thrones - Hard.mp3</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Game of Thrones - Hard', 'Game of Thrones', 'Hard', 'Game of Thrones Theme', 'Ramin Djawadi', 'TV Shows', 'music\tv shows\Game of Thrones - Hard.mp3', 'https://www.youtube.com/embed/s7L2PVdrb_8?si=yiFJ25qmae4KlKRY');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>400</v>
+      </c>
+      <c r="B16" t="s">
+        <v>399</v>
+      </c>
       <c r="C16" t="s">
         <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>404</v>
+      </c>
+      <c r="E16" t="s">
+        <v>403</v>
       </c>
       <c r="F16" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Fringe - Easy.mp3</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fringe - Easy', 'Fringe', 'Easy', 'Fringe Main Title Theme', 'J.J. Abrams', 'TV Shows', 'music\tv shows\Fringe - Easy.mp3', 'https://www.youtube.com/embed/c4Vvs_JAh04?si=BZFkWxo86XrR3T0Z');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>401</v>
+      </c>
+      <c r="B17" t="s">
+        <v>399</v>
+      </c>
       <c r="C17" t="s">
         <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>404</v>
+      </c>
+      <c r="E17" t="s">
+        <v>403</v>
       </c>
       <c r="F17" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Fringe - Hard.mp3</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Fringe - Hard', 'Fringe', 'Hard', 'Fringe Main Title Theme', 'J.J. Abrams', 'TV Shows', 'music\tv shows\Fringe - Hard.mp3', 'https://www.youtube.com/embed/c4Vvs_JAh04?si=BZFkWxo86XrR3T0Z');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>405</v>
+      </c>
+      <c r="B18" t="s">
+        <v>407</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>410</v>
+      </c>
+      <c r="E18" t="s">
+        <v>409</v>
+      </c>
       <c r="F18" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Doctor Who - Easy.mp3</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Doctor Who - Easy', 'Doctor Who', 'Easy', 'Doctor Who Theme', 'Ron Grainer', 'TV Shows', 'music\tv shows\Doctor Who - Easy.mp3', 'https://www.youtube.com/embed/sWuAt0swt7k?si=mRqECVYwk5nMnkP2');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>406</v>
+      </c>
+      <c r="B19" t="s">
+        <v>407</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>410</v>
+      </c>
+      <c r="E19" t="s">
+        <v>409</v>
+      </c>
       <c r="F19" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Doctor Who - Hard.mp3</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Doctor Who - Hard', 'Doctor Who', 'Hard', 'Doctor Who Theme', 'Ron Grainer', 'TV Shows', 'music\tv shows\Doctor Who - Hard.mp3', 'https://www.youtube.com/embed/sWuAt0swt7k?si=mRqECVYwk5nMnkP2');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>412</v>
+      </c>
+      <c r="B20" t="s">
+        <v>414</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>416</v>
+      </c>
+      <c r="E20" t="s">
+        <v>415</v>
+      </c>
       <c r="F20" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Angel - Easy.mp3</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Angel - Easy', 'Angel', 'Easy', 'The Sanctuary', 'Darling Violetta', 'TV Shows', 'music\tv shows\Angel - Easy.mp3', 'https://www.youtube.com/embed/vpAol_17mO0?si=RNiARjVBLEtpGGv0');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>413</v>
+      </c>
+      <c r="B21" t="s">
+        <v>414</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>416</v>
+      </c>
+      <c r="E21" t="s">
+        <v>415</v>
+      </c>
       <c r="F21" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Angel - Hard.mp3</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Angel - Hard', 'Angel', 'Hard', 'The Sanctuary', 'Darling Violetta', 'TV Shows', 'music\tv shows\Angel - Hard.mp3', 'https://www.youtube.com/embed/vpAol_17mO0?si=RNiARjVBLEtpGGv0');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>419</v>
+      </c>
+      <c r="B22" t="s">
+        <v>418</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>421</v>
+      </c>
+      <c r="E22" t="s">
+        <v>422</v>
+      </c>
       <c r="F22" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\The Fresh Prince of Bel Air - Easy.mp3</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Fresh Prince of Bel Air - Easy', 'The Fresh Prince of Bel Air', 'Easy', 'Yo Home to Bel-Air', 'DJ Jazzy Jeff &amp; Will Smith', 'TV Shows', 'music\tv shows\The Fresh Prince of Bel Air - Easy.mp3', 'https://www.youtube.com/embed/1nCqRmx3Dnw?si=eJpPAceg6sOQwkuG');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>420</v>
+      </c>
+      <c r="B23" t="s">
+        <v>418</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>421</v>
+      </c>
+      <c r="E23" t="s">
+        <v>422</v>
+      </c>
       <c r="F23" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\The Fresh Prince of Bel Air - Hard.mp3</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('The Fresh Prince of Bel Air - Hard', 'The Fresh Prince of Bel Air', 'Hard', 'Yo Home to Bel-Air', 'DJ Jazzy Jeff &amp; Will Smith', 'TV Shows', 'music\tv shows\The Fresh Prince of Bel Air - Hard.mp3', 'https://www.youtube.com/embed/1nCqRmx3Dnw?si=eJpPAceg6sOQwkuG');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>425</v>
+      </c>
+      <c r="B24" t="s">
+        <v>424</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>432</v>
+      </c>
+      <c r="E24" t="s">
+        <v>433</v>
+      </c>
       <c r="F24" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\What We Do In The Shadows - Easy.mp3</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('What We Do In The Shadows - Easy', 'What We Do In The Shadows', 'Easy', 'You're Dead', 'Norma Tanega', 'TV Shows', 'music\tv shows\What We Do In The Shadows - Easy.mp3', 'https://www.youtube.com/embed/b4T1M5C6MUY?si=5y2gVU6xsDynFbes');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>425</v>
+      </c>
+      <c r="B25" t="s">
+        <v>424</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>432</v>
+      </c>
+      <c r="E25" t="s">
+        <v>433</v>
+      </c>
       <c r="F25" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\What We Do In The Shadows - Easy.mp3</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('What We Do In The Shadows - Easy', 'What We Do In The Shadows', 'Hard', 'You're Dead', 'Norma Tanega', 'TV Shows', 'music\tv shows\What We Do In The Shadows - Easy.mp3', 'https://www.youtube.com/embed/b4T1M5C6MUY?si=5y2gVU6xsDynFbes');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>427</v>
+      </c>
+      <c r="B26" t="s">
+        <v>429</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" t="s">
+        <v>430</v>
+      </c>
+      <c r="E26" t="s">
+        <v>431</v>
+      </c>
       <c r="F26" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Chuck - Easy.mp3</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Chuck - Easy', 'Chuck', 'Easy', 'Short Skirt / Long Jacket', 'Cake', 'TV Shows', 'music\tv shows\Chuck - Easy.mp3', 'https://www.youtube.com/embed/ATRgllo_9aE?si=ewcgOFR464d0BvpC');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>428</v>
+      </c>
+      <c r="B27" t="s">
+        <v>429</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>430</v>
+      </c>
+      <c r="E27" t="s">
+        <v>431</v>
+      </c>
       <c r="F27" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\Chuck - Hard.mp3</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('Chuck - Hard', 'Chuck', 'Hard', 'Short Skirt / Long Jacket', 'Cake', 'TV Shows', 'music\tv shows\Chuck - Hard.mp3', 'https://www.youtube.com/embed/ATRgllo_9aE?si=ewcgOFR464d0BvpC');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
       <c r="F28" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Easy', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
       <c r="F29" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Hard', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
       <c r="F30" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Easy', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
       <c r="F31" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Hard', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
       <c r="F32" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Easy', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
       <c r="F33" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Hard', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
       <c r="F34" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Easy', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
       <c r="F35" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Hard', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>67</v>
+      </c>
       <c r="F36" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Easy', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
       <c r="F37" t="s">
         <v>367</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>music\tv shows\.mp3</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO songs (name, property, difficulty, song_name, artist, category, location, video_link) VALUES ('', '', 'Hard', '', '', 'TV Shows', 'music\tv shows\.mp3', '');</v>
       </c>
     </row>
   </sheetData>
@@ -6230,7 +6829,7 @@
         <f>"music\"&amp;LOWER(F2)&amp;"\"&amp;A2&amp;".mp3"</f>
         <v>music\tv shows\Breaking Bad - Easy.mp3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" t="s">
         <v>361</v>
       </c>
       <c r="I2" s="1" t="str">
@@ -6261,7 +6860,7 @@
         <f t="shared" ref="G3" si="0">"music\"&amp;LOWER(F3)&amp;"\"&amp;A3&amp;".mp3"</f>
         <v>music\tv shows\Breaking Bad - Hard.mp3</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" t="s">
         <v>361</v>
       </c>
       <c r="I3" s="1" t="str">
@@ -6288,7 +6887,7 @@
       <c r="F4" t="s">
         <v>367</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6311,7 +6910,7 @@
       <c r="F5" t="s">
         <v>367</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>368</v>
       </c>
     </row>
@@ -6334,7 +6933,7 @@
       <c r="F6" t="s">
         <v>367</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>